<commit_message>
generate random string added for text fields
</commit_message>
<xml_diff>
--- a/Testdata/TestData.xlsx
+++ b/Testdata/TestData.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\turtlemint_poc\turtlemint\TestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\poc\turtlemint\Testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F439FFF-4581-4FA3-A482-95E969325EB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAC0BD90-8E0E-4EFD-9A1E-1DBE7802768B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="21">
   <si>
     <t>TC_01</t>
   </si>
@@ -51,9 +51,6 @@
     <t>No</t>
   </si>
   <si>
-    <t>Less than Rs 2.5 lakhs</t>
-  </si>
-  <si>
     <t>insurance type</t>
   </si>
   <si>
@@ -66,9 +63,6 @@
     <t>member have any disease</t>
   </si>
   <si>
-    <t>534442</t>
-  </si>
-  <si>
     <t>income bracket</t>
   </si>
   <si>
@@ -76,6 +70,24 @@
   </si>
   <si>
     <t>Self-42 years;Wife-40 years</t>
+  </si>
+  <si>
+    <t>500051</t>
+  </si>
+  <si>
+    <t>More than Rs 10 lakhs</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>UNIQUE@gmail.com</t>
+  </si>
+  <si>
+    <t>8106443203</t>
+  </si>
+  <si>
+    <t>mobile</t>
   </si>
 </sst>
 </file>
@@ -340,7 +352,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="14" fillId="9" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -350,10 +362,9 @@
     </xf>
     <xf numFmtId="49" fontId="17" fillId="0" borderId="2" xfId="18" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="10" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -758,9 +769,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:ALG9"/>
+  <dimension ref="A1:ALF9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
       <selection activeCell="J1" sqref="J1"/>
     </sheetView>
   </sheetViews>
@@ -768,48 +779,55 @@
   <cols>
     <col min="1" max="1" width="11" style="1" customWidth="1"/>
     <col min="2" max="2" width="16.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="59.140625" style="8" customWidth="1"/>
+    <col min="3" max="3" width="59.140625" style="6" customWidth="1"/>
     <col min="4" max="4" width="38.140625" style="1" customWidth="1"/>
     <col min="5" max="5" width="17" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="27.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="28.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="11.42578125" style="1"/>
     <col min="9" max="9" width="26.7109375" style="6" bestFit="1" customWidth="1"/>
-    <col min="10" max="995" width="11.42578125" style="1"/>
-    <col min="996" max="1013" width="8.7109375" customWidth="1"/>
+    <col min="10" max="10" width="16.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="19.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="994" width="11.42578125" style="1"/>
+    <col min="995" max="1012" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:995" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:994" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>1</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C1" s="7" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E1" s="4" t="s">
         <v>3</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H1" s="4" t="s">
         <v>4</v>
       </c>
       <c r="I1" s="4" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
-      <c r="J1" s="4"/>
+      <c r="J1" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>17</v>
+      </c>
     </row>
-    <row r="2" spans="1:995" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:994" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
@@ -820,10 +838,10 @@
         <v>6</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>7</v>
@@ -832,19 +850,25 @@
         <v>7</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>8</v>
+        <v>16</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="K2" s="5" t="s">
+        <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:995" s="10" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:994" s="9" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="3"/>
       <c r="B3" s="3"/>
       <c r="C3" s="5"/>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
-      <c r="F3" s="9"/>
+      <c r="F3" s="8"/>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
       <c r="I3" s="3"/>
@@ -1833,9 +1857,8 @@
       <c r="ALD3" s="1"/>
       <c r="ALE3" s="1"/>
       <c r="ALF3" s="1"/>
-      <c r="ALG3" s="1"/>
     </row>
-    <row r="4" spans="1:995" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:994" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
@@ -2830,14 +2853,13 @@
       <c r="ALD4" s="1"/>
       <c r="ALE4" s="1"/>
       <c r="ALF4" s="1"/>
-      <c r="ALG4" s="1"/>
     </row>
-    <row r="5" spans="1:995" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:994" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
-      <c r="E5" s="9"/>
+      <c r="E5" s="8"/>
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
@@ -3827,9 +3849,8 @@
       <c r="ALD5" s="1"/>
       <c r="ALE5" s="1"/>
       <c r="ALF5" s="1"/>
-      <c r="ALG5" s="1"/>
     </row>
-    <row r="6" spans="1:995" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:994" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
@@ -4824,16 +4845,15 @@
       <c r="ALD6" s="1"/>
       <c r="ALE6" s="1"/>
       <c r="ALF6" s="1"/>
-      <c r="ALG6" s="1"/>
     </row>
-    <row r="7" spans="1:995" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:994" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
-      <c r="G7" s="9"/>
+      <c r="G7" s="8"/>
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
       <c r="J7" s="1"/>
@@ -5821,9 +5841,8 @@
       <c r="ALD7" s="1"/>
       <c r="ALE7" s="1"/>
       <c r="ALF7" s="1"/>
-      <c r="ALG7" s="1"/>
     </row>
-    <row r="8" spans="1:995" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:994" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
@@ -6818,9 +6837,8 @@
       <c r="ALD8" s="1"/>
       <c r="ALE8" s="1"/>
       <c r="ALF8" s="1"/>
-      <c r="ALG8" s="1"/>
     </row>
-    <row r="9" spans="1:995" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:994" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
@@ -7815,12 +7833,14 @@
       <c r="ALD9" s="1"/>
       <c r="ALE9" s="1"/>
       <c r="ALF9" s="1"/>
-      <c r="ALG9" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="16" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="K2" r:id="rId1" xr:uid="{A111A7B2-D9C5-4F09-955C-F59643DB73F8}"/>
+  </hyperlinks>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0249999999999999" bottom="1.0249999999999999" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageSetup orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;"Arial,Regular"&amp;10&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Arial,Regular"&amp;10Page &amp;P</oddFooter>

</xml_diff>

<commit_message>
Reviewed and updated code
</commit_message>
<xml_diff>
--- a/Testdata/TestData.xlsx
+++ b/Testdata/TestData.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\poc\turtlemint\Testdata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\QualiZeal\POC_project\TurtleMint\tm-auto-code\turtlemint\Testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAC0BD90-8E0E-4EFD-9A1E-1DBE7802768B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24F910E2-A355-4F88-9D7C-54570BAED194}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="policy" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
   <si>
     <t>TC_01</t>
   </si>
@@ -51,21 +51,6 @@
     <t>No</t>
   </si>
   <si>
-    <t>insurance type</t>
-  </si>
-  <si>
-    <t>members to be insured</t>
-  </si>
-  <si>
-    <t>planning to have kids</t>
-  </si>
-  <si>
-    <t>member have any disease</t>
-  </si>
-  <si>
-    <t>income bracket</t>
-  </si>
-  <si>
     <t>Self;Wife</t>
   </si>
   <si>
@@ -75,19 +60,61 @@
     <t>500051</t>
   </si>
   <si>
-    <t>More than Rs 10 lakhs</t>
-  </si>
-  <si>
     <t>email</t>
-  </si>
-  <si>
-    <t>UNIQUE@gmail.com</t>
   </si>
   <si>
     <t>8106443203</t>
   </si>
   <si>
     <t>mobile</t>
+  </si>
+  <si>
+    <t>insurance_type</t>
+  </si>
+  <si>
+    <t>members_to_be_ insured</t>
+  </si>
+  <si>
+    <t>planning_to_have kids</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>when_are_you_planning_kids</t>
+  </si>
+  <si>
+    <t>MORETHAN3YRS</t>
+  </si>
+  <si>
+    <t>member_have_any_disease</t>
+  </si>
+  <si>
+    <t>income_bracket</t>
+  </si>
+  <si>
+    <t>LESSTHAN2.5LAKHS</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>AutoTestUNIQUE</t>
+  </si>
+  <si>
+    <t>AutoTestUNIQUE@gmail.com</t>
+  </si>
+  <si>
+    <t>customize_policyheader</t>
+  </si>
+  <si>
+    <t>Self &amp; spouse</t>
+  </si>
+  <si>
+    <t>policy_cover</t>
+  </si>
+  <si>
+    <t>5 Lakhs</t>
   </si>
 </sst>
 </file>
@@ -769,65 +796,82 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:ALF9"/>
+  <dimension ref="A1:ALH41"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
-      <selection activeCell="J1" sqref="J1"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="11" style="1" customWidth="1"/>
-    <col min="2" max="2" width="16.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="59.140625" style="6" customWidth="1"/>
-    <col min="4" max="4" width="38.140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="16.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="59.109375" style="6" customWidth="1"/>
+    <col min="4" max="4" width="38.109375" style="1" customWidth="1"/>
     <col min="5" max="5" width="17" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="27.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="28.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.42578125" style="1"/>
-    <col min="9" max="9" width="26.7109375" style="6" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="19.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="994" width="11.42578125" style="1"/>
-    <col min="995" max="1012" width="8.7109375" customWidth="1"/>
+    <col min="6" max="6" width="27.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="27.88671875" style="1" customWidth="1"/>
+    <col min="8" max="8" width="28.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.44140625" style="1"/>
+    <col min="10" max="10" width="26.6640625" style="6" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="26.6640625" style="6" customWidth="1"/>
+    <col min="12" max="12" width="16.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="19.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="25.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13.6640625" style="1" customWidth="1"/>
+    <col min="16" max="16" width="16.21875" style="1" customWidth="1"/>
+    <col min="17" max="996" width="11.44140625" style="1"/>
+    <col min="997" max="1014" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:994" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:996" s="2" customFormat="1" ht="16.8" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>1</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="C1" s="7" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="E1" s="4" t="s">
         <v>3</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="G1" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="M1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="H1" s="4" t="s">
-        <v>4</v>
+      <c r="N1" s="2" t="s">
+        <v>26</v>
       </c>
-      <c r="I1" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>17</v>
+      <c r="O1" s="2" t="s">
+        <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:994" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:996" s="3" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
@@ -838,31 +882,43 @@
         <v>6</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="F2" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="G2" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>15</v>
-      </c>
       <c r="I2" s="3" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
-      <c r="K2" s="5" t="s">
-        <v>18</v>
+      <c r="K2" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="M2" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="N2" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="O2" s="3" t="s">
+        <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:994" s="9" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:996" s="9" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" s="3"/>
       <c r="B3" s="3"/>
       <c r="C3" s="5"/>
@@ -871,8 +927,8 @@
       <c r="F3" s="8"/>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
-      <c r="I3" s="3"/>
-      <c r="J3" s="1"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="3"/>
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
@@ -1857,8 +1913,10 @@
       <c r="ALD3" s="1"/>
       <c r="ALE3" s="1"/>
       <c r="ALF3" s="1"/>
+      <c r="ALG3" s="1"/>
+      <c r="ALH3" s="1"/>
     </row>
-    <row r="4" spans="1:994" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:996" s="9" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
@@ -1868,7 +1926,7 @@
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
-      <c r="J4" s="1"/>
+      <c r="J4" s="3"/>
       <c r="K4" s="1"/>
       <c r="L4" s="1"/>
       <c r="M4" s="1"/>
@@ -2853,8 +2911,10 @@
       <c r="ALD4" s="1"/>
       <c r="ALE4" s="1"/>
       <c r="ALF4" s="1"/>
+      <c r="ALG4" s="1"/>
+      <c r="ALH4" s="1"/>
     </row>
-    <row r="5" spans="1:994" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:996" s="9" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
@@ -2864,7 +2924,7 @@
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
-      <c r="J5" s="1"/>
+      <c r="J5" s="3"/>
       <c r="K5" s="1"/>
       <c r="L5" s="1"/>
       <c r="M5" s="1"/>
@@ -3849,8 +3909,10 @@
       <c r="ALD5" s="1"/>
       <c r="ALE5" s="1"/>
       <c r="ALF5" s="1"/>
+      <c r="ALG5" s="1"/>
+      <c r="ALH5" s="1"/>
     </row>
-    <row r="6" spans="1:994" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:996" s="9" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
@@ -3860,7 +3922,7 @@
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
-      <c r="J6" s="1"/>
+      <c r="J6" s="3"/>
       <c r="K6" s="1"/>
       <c r="L6" s="1"/>
       <c r="M6" s="1"/>
@@ -4845,18 +4907,20 @@
       <c r="ALD6" s="1"/>
       <c r="ALE6" s="1"/>
       <c r="ALF6" s="1"/>
+      <c r="ALG6" s="1"/>
+      <c r="ALH6" s="1"/>
     </row>
-    <row r="7" spans="1:994" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:996" s="9" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
-      <c r="G7" s="8"/>
-      <c r="H7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="8"/>
       <c r="I7" s="1"/>
-      <c r="J7" s="1"/>
+      <c r="J7" s="3"/>
       <c r="K7" s="1"/>
       <c r="L7" s="1"/>
       <c r="M7" s="1"/>
@@ -5841,8 +5905,10 @@
       <c r="ALD7" s="1"/>
       <c r="ALE7" s="1"/>
       <c r="ALF7" s="1"/>
+      <c r="ALG7" s="1"/>
+      <c r="ALH7" s="1"/>
     </row>
-    <row r="8" spans="1:994" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:996" s="9" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
@@ -5852,7 +5918,7 @@
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
-      <c r="J8" s="1"/>
+      <c r="J8" s="3"/>
       <c r="K8" s="1"/>
       <c r="L8" s="1"/>
       <c r="M8" s="1"/>
@@ -6837,8 +6903,10 @@
       <c r="ALD8" s="1"/>
       <c r="ALE8" s="1"/>
       <c r="ALF8" s="1"/>
+      <c r="ALG8" s="1"/>
+      <c r="ALH8" s="1"/>
     </row>
-    <row r="9" spans="1:994" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:996" s="9" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
@@ -6848,7 +6916,7 @@
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
-      <c r="J9" s="1"/>
+      <c r="J9" s="3"/>
       <c r="K9" s="1"/>
       <c r="L9" s="1"/>
       <c r="M9" s="1"/>
@@ -7833,11 +7901,132 @@
       <c r="ALD9" s="1"/>
       <c r="ALE9" s="1"/>
       <c r="ALF9" s="1"/>
+      <c r="ALG9" s="1"/>
+      <c r="ALH9" s="1"/>
+    </row>
+    <row r="10" spans="1:996" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="J10" s="3"/>
+      <c r="K10" s="1"/>
+    </row>
+    <row r="11" spans="1:996" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="J11" s="3"/>
+      <c r="K11" s="1"/>
+    </row>
+    <row r="12" spans="1:996" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="J12" s="3"/>
+      <c r="K12" s="1"/>
+    </row>
+    <row r="13" spans="1:996" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="J13" s="3"/>
+      <c r="K13" s="1"/>
+    </row>
+    <row r="14" spans="1:996" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="J14" s="3"/>
+      <c r="K14" s="1"/>
+    </row>
+    <row r="15" spans="1:996" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="J15" s="3"/>
+      <c r="K15" s="1"/>
+    </row>
+    <row r="16" spans="1:996" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="J16" s="3"/>
+      <c r="K16" s="1"/>
+    </row>
+    <row r="17" spans="10:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="J17" s="3"/>
+      <c r="K17" s="1"/>
+    </row>
+    <row r="18" spans="10:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="J18" s="3"/>
+      <c r="K18" s="1"/>
+    </row>
+    <row r="19" spans="10:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="J19" s="3"/>
+      <c r="K19" s="1"/>
+    </row>
+    <row r="20" spans="10:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="J20" s="3"/>
+      <c r="K20" s="1"/>
+    </row>
+    <row r="21" spans="10:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="J21" s="3"/>
+      <c r="K21" s="1"/>
+    </row>
+    <row r="22" spans="10:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="J22" s="3"/>
+      <c r="K22" s="1"/>
+    </row>
+    <row r="23" spans="10:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="J23" s="3"/>
+      <c r="K23" s="1"/>
+    </row>
+    <row r="24" spans="10:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="J24" s="3"/>
+      <c r="K24" s="1"/>
+    </row>
+    <row r="25" spans="10:11" x14ac:dyDescent="0.3">
+      <c r="K25" s="1"/>
+    </row>
+    <row r="26" spans="10:11" x14ac:dyDescent="0.3">
+      <c r="K26" s="1"/>
+    </row>
+    <row r="27" spans="10:11" x14ac:dyDescent="0.3">
+      <c r="K27" s="1"/>
+    </row>
+    <row r="28" spans="10:11" x14ac:dyDescent="0.3">
+      <c r="K28" s="1"/>
+    </row>
+    <row r="29" spans="10:11" x14ac:dyDescent="0.3">
+      <c r="K29" s="1"/>
+    </row>
+    <row r="30" spans="10:11" x14ac:dyDescent="0.3">
+      <c r="K30" s="1"/>
+    </row>
+    <row r="31" spans="10:11" x14ac:dyDescent="0.3">
+      <c r="K31" s="1"/>
+    </row>
+    <row r="32" spans="10:11" x14ac:dyDescent="0.3">
+      <c r="K32" s="1"/>
+    </row>
+    <row r="33" spans="11:11" x14ac:dyDescent="0.3">
+      <c r="K33" s="1"/>
+    </row>
+    <row r="34" spans="11:11" x14ac:dyDescent="0.3">
+      <c r="K34" s="1"/>
+    </row>
+    <row r="35" spans="11:11" x14ac:dyDescent="0.3">
+      <c r="K35" s="1"/>
+    </row>
+    <row r="36" spans="11:11" x14ac:dyDescent="0.3">
+      <c r="K36" s="1"/>
+    </row>
+    <row r="37" spans="11:11" x14ac:dyDescent="0.3">
+      <c r="K37" s="1"/>
+    </row>
+    <row r="38" spans="11:11" x14ac:dyDescent="0.3">
+      <c r="K38" s="1"/>
+    </row>
+    <row r="39" spans="11:11" x14ac:dyDescent="0.3">
+      <c r="K39" s="1"/>
+    </row>
+    <row r="40" spans="11:11" x14ac:dyDescent="0.3">
+      <c r="K40" s="1"/>
+    </row>
+    <row r="41" spans="11:11" x14ac:dyDescent="0.3">
+      <c r="K41" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="16" type="noConversion"/>
+  <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G29" xr:uid="{F5E067AE-9E98-48C4-8B1E-338F1C170DC3}">
+      <formula1>"IN1YR,IN3YRS,MORETHAN3YRS"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2:J24" xr:uid="{4FF073F2-2DA2-43FC-869C-552FD33A464D}">
+      <formula1>"LESSTHAN2.5LAKHS,UPTO5LAKHS,UPTO10LAKHS,MORETHAN10LAKHS"</formula1>
+    </dataValidation>
+  </dataValidations>
   <hyperlinks>
-    <hyperlink ref="K2" r:id="rId1" xr:uid="{A111A7B2-D9C5-4F09-955C-F59643DB73F8}"/>
+    <hyperlink ref="M2" r:id="rId1" xr:uid="{A111A7B2-D9C5-4F09-955C-F59643DB73F8}"/>
   </hyperlinks>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0249999999999999" bottom="1.0249999999999999" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>

</xml_diff>

<commit_message>
updated according to comments
</commit_message>
<xml_diff>
--- a/Testdata/TestData.xlsx
+++ b/Testdata/TestData.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\QualiZeal\POC_project\TurtleMint\tm-auto-code\turtlemint\Testdata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\poc\turtlemint\Testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24F910E2-A355-4F88-9D7C-54570BAED194}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA741E7D-A08E-47C2-9498-097E89620A89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="policy" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="29">
   <si>
     <t>TC_01</t>
   </si>
@@ -57,13 +57,7 @@
     <t>Self-42 years;Wife-40 years</t>
   </si>
   <si>
-    <t>500051</t>
-  </si>
-  <si>
     <t>email</t>
-  </si>
-  <si>
-    <t>8106443203</t>
   </si>
   <si>
     <t>mobile</t>
@@ -78,13 +72,7 @@
     <t>planning_to_have kids</t>
   </si>
   <si>
-    <t>Yes</t>
-  </si>
-  <si>
     <t>when_are_you_planning_kids</t>
-  </si>
-  <si>
-    <t>MORETHAN3YRS</t>
   </si>
   <si>
     <t>member_have_any_disease</t>
@@ -93,13 +81,7 @@
     <t>income_bracket</t>
   </si>
   <si>
-    <t>LESSTHAN2.5LAKHS</t>
-  </si>
-  <si>
     <t>name</t>
-  </si>
-  <si>
-    <t>AutoTestUNIQUE</t>
   </si>
   <si>
     <t>AutoTestUNIQUE@gmail.com</t>
@@ -116,12 +98,27 @@
   <si>
     <t>5 Lakhs</t>
   </si>
+  <si>
+    <t>UNIQUEphno</t>
+  </si>
+  <si>
+    <t>500051</t>
+  </si>
+  <si>
+    <t>UPTO10LAKHS</t>
+  </si>
+  <si>
+    <t>UNIQUEfullname</t>
+  </si>
+  <si>
+    <t>IN1YR</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -256,6 +253,12 @@
       <name val="Consolas"/>
       <family val="3"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9CDCFE"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
   </fonts>
   <fills count="11">
     <fill>
@@ -379,7 +382,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="14" fillId="9" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -396,6 +399,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="19">
     <cellStyle name="Accent 1 17" xfId="1" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
@@ -798,80 +804,80 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:ALH41"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11" style="1" customWidth="1"/>
-    <col min="2" max="2" width="16.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="59.109375" style="6" customWidth="1"/>
-    <col min="4" max="4" width="38.109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="16.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="59.140625" style="6" customWidth="1"/>
+    <col min="4" max="4" width="38.140625" style="1" customWidth="1"/>
     <col min="5" max="5" width="17" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="27.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="27.88671875" style="1" customWidth="1"/>
-    <col min="8" max="8" width="28.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.44140625" style="1"/>
-    <col min="10" max="10" width="26.6640625" style="6" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="26.6640625" style="6" customWidth="1"/>
-    <col min="12" max="12" width="16.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="19.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="25.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="13.6640625" style="1" customWidth="1"/>
-    <col min="16" max="16" width="16.21875" style="1" customWidth="1"/>
-    <col min="17" max="996" width="11.44140625" style="1"/>
-    <col min="997" max="1014" width="8.6640625" customWidth="1"/>
+    <col min="6" max="6" width="27.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="27.85546875" style="1" customWidth="1"/>
+    <col min="8" max="8" width="28.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.42578125" style="1"/>
+    <col min="10" max="10" width="26.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="26.7109375" style="6" customWidth="1"/>
+    <col min="12" max="12" width="25.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="31.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="25.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13.7109375" style="1" customWidth="1"/>
+    <col min="16" max="16" width="16.28515625" style="1" customWidth="1"/>
+    <col min="17" max="996" width="11.42578125" style="1"/>
+    <col min="997" max="1014" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:996" s="2" customFormat="1" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:996" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>1</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C1" s="7" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E1" s="4" t="s">
         <v>3</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="I1" s="4" t="s">
         <v>4</v>
       </c>
       <c r="J1" s="4" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="K1" s="4" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="M1" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="N1" s="2" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="O1" s="2" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:996" s="3" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:996" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
@@ -888,37 +894,37 @@
         <v>9</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="H2" s="3" t="s">
         <v>7</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="K2" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="L2" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="L2" s="3" t="s">
-        <v>12</v>
-      </c>
       <c r="M2" s="3" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="N2" s="3" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="O2" s="3" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:996" s="9" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:996" s="9" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="3"/>
       <c r="B3" s="3"/>
       <c r="C3" s="5"/>
@@ -926,7 +932,6 @@
       <c r="E3" s="1"/>
       <c r="F3" s="8"/>
       <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
       <c r="I3" s="1"/>
       <c r="J3" s="3"/>
       <c r="K3" s="1"/>
@@ -1916,7 +1921,7 @@
       <c r="ALG3" s="1"/>
       <c r="ALH3" s="1"/>
     </row>
-    <row r="4" spans="1:996" s="9" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:996" s="9" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
@@ -2914,7 +2919,7 @@
       <c r="ALG4" s="1"/>
       <c r="ALH4" s="1"/>
     </row>
-    <row r="5" spans="1:996" s="9" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:996" s="9" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
@@ -3912,7 +3917,7 @@
       <c r="ALG5" s="1"/>
       <c r="ALH5" s="1"/>
     </row>
-    <row r="6" spans="1:996" s="9" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:996" s="9" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
@@ -4910,7 +4915,7 @@
       <c r="ALG6" s="1"/>
       <c r="ALH6" s="1"/>
     </row>
-    <row r="7" spans="1:996" s="9" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:996" s="9" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -5908,7 +5913,7 @@
       <c r="ALG7" s="1"/>
       <c r="ALH7" s="1"/>
     </row>
-    <row r="8" spans="1:996" s="9" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:996" s="9" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
@@ -6906,7 +6911,7 @@
       <c r="ALG8" s="1"/>
       <c r="ALH8" s="1"/>
     </row>
-    <row r="9" spans="1:996" s="9" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:996" s="9" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
@@ -7904,115 +7909,115 @@
       <c r="ALG9" s="1"/>
       <c r="ALH9" s="1"/>
     </row>
-    <row r="10" spans="1:996" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:996" ht="15.75" x14ac:dyDescent="0.25">
       <c r="J10" s="3"/>
       <c r="K10" s="1"/>
     </row>
-    <row r="11" spans="1:996" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:996" ht="15.75" x14ac:dyDescent="0.25">
       <c r="J11" s="3"/>
       <c r="K11" s="1"/>
     </row>
-    <row r="12" spans="1:996" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:996" ht="15.75" x14ac:dyDescent="0.25">
       <c r="J12" s="3"/>
       <c r="K12" s="1"/>
     </row>
-    <row r="13" spans="1:996" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:996" ht="15.75" x14ac:dyDescent="0.25">
       <c r="J13" s="3"/>
       <c r="K13" s="1"/>
     </row>
-    <row r="14" spans="1:996" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:996" ht="15.75" x14ac:dyDescent="0.25">
       <c r="J14" s="3"/>
       <c r="K14" s="1"/>
     </row>
-    <row r="15" spans="1:996" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:996" ht="15.75" x14ac:dyDescent="0.25">
       <c r="J15" s="3"/>
       <c r="K15" s="1"/>
     </row>
-    <row r="16" spans="1:996" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:996" ht="15.75" x14ac:dyDescent="0.25">
       <c r="J16" s="3"/>
       <c r="K16" s="1"/>
     </row>
-    <row r="17" spans="10:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="17" spans="10:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="J17" s="3"/>
       <c r="K17" s="1"/>
     </row>
-    <row r="18" spans="10:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="18" spans="10:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="J18" s="3"/>
       <c r="K18" s="1"/>
     </row>
-    <row r="19" spans="10:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="19" spans="10:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="J19" s="3"/>
       <c r="K19" s="1"/>
     </row>
-    <row r="20" spans="10:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="20" spans="10:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="J20" s="3"/>
       <c r="K20" s="1"/>
     </row>
-    <row r="21" spans="10:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="21" spans="10:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="J21" s="3"/>
       <c r="K21" s="1"/>
     </row>
-    <row r="22" spans="10:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="22" spans="10:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="J22" s="3"/>
       <c r="K22" s="1"/>
     </row>
-    <row r="23" spans="10:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="23" spans="10:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="J23" s="3"/>
       <c r="K23" s="1"/>
     </row>
-    <row r="24" spans="10:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="24" spans="10:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="J24" s="3"/>
       <c r="K24" s="1"/>
     </row>
-    <row r="25" spans="10:11" x14ac:dyDescent="0.3">
+    <row r="25" spans="10:11" x14ac:dyDescent="0.25">
       <c r="K25" s="1"/>
     </row>
-    <row r="26" spans="10:11" x14ac:dyDescent="0.3">
+    <row r="26" spans="10:11" x14ac:dyDescent="0.25">
       <c r="K26" s="1"/>
     </row>
-    <row r="27" spans="10:11" x14ac:dyDescent="0.3">
+    <row r="27" spans="10:11" x14ac:dyDescent="0.25">
       <c r="K27" s="1"/>
     </row>
-    <row r="28" spans="10:11" x14ac:dyDescent="0.3">
+    <row r="28" spans="10:11" x14ac:dyDescent="0.25">
       <c r="K28" s="1"/>
     </row>
-    <row r="29" spans="10:11" x14ac:dyDescent="0.3">
+    <row r="29" spans="10:11" x14ac:dyDescent="0.25">
       <c r="K29" s="1"/>
     </row>
-    <row r="30" spans="10:11" x14ac:dyDescent="0.3">
+    <row r="30" spans="10:11" x14ac:dyDescent="0.25">
       <c r="K30" s="1"/>
     </row>
-    <row r="31" spans="10:11" x14ac:dyDescent="0.3">
+    <row r="31" spans="10:11" x14ac:dyDescent="0.25">
       <c r="K31" s="1"/>
     </row>
-    <row r="32" spans="10:11" x14ac:dyDescent="0.3">
+    <row r="32" spans="10:11" x14ac:dyDescent="0.25">
       <c r="K32" s="1"/>
     </row>
-    <row r="33" spans="11:11" x14ac:dyDescent="0.3">
+    <row r="33" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K33" s="1"/>
     </row>
-    <row r="34" spans="11:11" x14ac:dyDescent="0.3">
+    <row r="34" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K34" s="1"/>
     </row>
-    <row r="35" spans="11:11" x14ac:dyDescent="0.3">
+    <row r="35" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K35" s="1"/>
     </row>
-    <row r="36" spans="11:11" x14ac:dyDescent="0.3">
+    <row r="36" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K36" s="1"/>
     </row>
-    <row r="37" spans="11:11" x14ac:dyDescent="0.3">
+    <row r="37" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K37" s="1"/>
     </row>
-    <row r="38" spans="11:11" x14ac:dyDescent="0.3">
+    <row r="38" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K38" s="1"/>
     </row>
-    <row r="39" spans="11:11" x14ac:dyDescent="0.3">
+    <row r="39" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K39" s="1"/>
     </row>
-    <row r="40" spans="11:11" x14ac:dyDescent="0.3">
+    <row r="40" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K40" s="1"/>
     </row>
-    <row r="41" spans="11:11" x14ac:dyDescent="0.3">
+    <row r="41" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K41" s="1"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated health results validation
</commit_message>
<xml_diff>
--- a/Testdata/TestData.xlsx
+++ b/Testdata/TestData.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\poc\turtlemint\Testdata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\QualiZeal\POC_project\TurtleMint\tm-auto-code\turtlemint\Testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA741E7D-A08E-47C2-9498-097E89620A89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98765EB1-144F-40F7-A0E3-AFA16DF1A292}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="policy" sheetId="1" r:id="rId1"/>
@@ -84,9 +84,6 @@
     <t>name</t>
   </si>
   <si>
-    <t>AutoTestUNIQUE@gmail.com</t>
-  </si>
-  <si>
     <t>customize_policyheader</t>
   </si>
   <si>
@@ -99,26 +96,29 @@
     <t>5 Lakhs</t>
   </si>
   <si>
-    <t>UNIQUEphno</t>
-  </si>
-  <si>
     <t>500051</t>
   </si>
   <si>
     <t>UPTO10LAKHS</t>
   </si>
   <si>
-    <t>UNIQUEfullname</t>
+    <t>IN1YR</t>
   </si>
   <si>
-    <t>IN1YR</t>
+    <t>RANDOM_NAME</t>
+  </si>
+  <si>
+    <t>RANDOM_PHONENUMBER</t>
+  </si>
+  <si>
+    <t>RANDOM_EMAILID</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -253,12 +253,6 @@
       <name val="Consolas"/>
       <family val="3"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9CDCFE"/>
-      <name val="Consolas"/>
-      <family val="3"/>
-    </font>
   </fonts>
   <fills count="11">
     <fill>
@@ -382,7 +376,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="14" fillId="9" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -399,9 +393,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="19">
     <cellStyle name="Accent 1 17" xfId="1" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
@@ -804,33 +795,33 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:ALH41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
+      <selection activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="11" style="1" customWidth="1"/>
-    <col min="2" max="2" width="16.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="59.140625" style="6" customWidth="1"/>
-    <col min="4" max="4" width="38.140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="16.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="59.109375" style="6" customWidth="1"/>
+    <col min="4" max="4" width="38.109375" style="1" customWidth="1"/>
     <col min="5" max="5" width="17" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="27.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="27.85546875" style="1" customWidth="1"/>
-    <col min="8" max="8" width="28.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.42578125" style="1"/>
-    <col min="10" max="10" width="26.7109375" style="6" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="26.7109375" style="6" customWidth="1"/>
-    <col min="12" max="12" width="25.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="31.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="25.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="13.7109375" style="1" customWidth="1"/>
-    <col min="16" max="16" width="16.28515625" style="1" customWidth="1"/>
-    <col min="17" max="996" width="11.42578125" style="1"/>
-    <col min="997" max="1014" width="8.7109375" customWidth="1"/>
+    <col min="6" max="6" width="27.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="27.88671875" style="1" customWidth="1"/>
+    <col min="8" max="8" width="28.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.44140625" style="1"/>
+    <col min="10" max="10" width="26.6640625" style="6" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="26.6640625" style="6" customWidth="1"/>
+    <col min="12" max="12" width="25.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="31.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="25.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13.6640625" style="1" customWidth="1"/>
+    <col min="16" max="16" width="16.33203125" style="1" customWidth="1"/>
+    <col min="17" max="996" width="11.44140625" style="1"/>
+    <col min="997" max="1014" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:996" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:996" s="2" customFormat="1" ht="16.8" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>1</v>
       </c>
@@ -871,13 +862,13 @@
         <v>10</v>
       </c>
       <c r="N1" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="O1" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:996" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:996" s="3" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
@@ -897,34 +888,34 @@
         <v>7</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="H2" s="3" t="s">
         <v>7</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="J2" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="K2" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="K2" s="1" t="s">
+      <c r="L2" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="L2" s="10" t="s">
-        <v>24</v>
-      </c>
       <c r="M2" s="3" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="N2" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="O2" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:996" s="9" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:996" s="9" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" s="3"/>
       <c r="B3" s="3"/>
       <c r="C3" s="5"/>
@@ -1921,7 +1912,7 @@
       <c r="ALG3" s="1"/>
       <c r="ALH3" s="1"/>
     </row>
-    <row r="4" spans="1:996" s="9" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:996" s="9" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
@@ -2919,7 +2910,7 @@
       <c r="ALG4" s="1"/>
       <c r="ALH4" s="1"/>
     </row>
-    <row r="5" spans="1:996" s="9" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:996" s="9" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
@@ -3917,7 +3908,7 @@
       <c r="ALG5" s="1"/>
       <c r="ALH5" s="1"/>
     </row>
-    <row r="6" spans="1:996" s="9" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:996" s="9" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
@@ -4915,7 +4906,7 @@
       <c r="ALG6" s="1"/>
       <c r="ALH6" s="1"/>
     </row>
-    <row r="7" spans="1:996" s="9" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:996" s="9" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -5913,7 +5904,7 @@
       <c r="ALG7" s="1"/>
       <c r="ALH7" s="1"/>
     </row>
-    <row r="8" spans="1:996" s="9" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:996" s="9" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
@@ -6911,7 +6902,7 @@
       <c r="ALG8" s="1"/>
       <c r="ALH8" s="1"/>
     </row>
-    <row r="9" spans="1:996" s="9" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:996" s="9" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
@@ -7909,115 +7900,115 @@
       <c r="ALG9" s="1"/>
       <c r="ALH9" s="1"/>
     </row>
-    <row r="10" spans="1:996" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:996" ht="15.6" x14ac:dyDescent="0.3">
       <c r="J10" s="3"/>
       <c r="K10" s="1"/>
     </row>
-    <row r="11" spans="1:996" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:996" ht="15.6" x14ac:dyDescent="0.3">
       <c r="J11" s="3"/>
       <c r="K11" s="1"/>
     </row>
-    <row r="12" spans="1:996" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:996" ht="15.6" x14ac:dyDescent="0.3">
       <c r="J12" s="3"/>
       <c r="K12" s="1"/>
     </row>
-    <row r="13" spans="1:996" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:996" ht="15.6" x14ac:dyDescent="0.3">
       <c r="J13" s="3"/>
       <c r="K13" s="1"/>
     </row>
-    <row r="14" spans="1:996" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:996" ht="15.6" x14ac:dyDescent="0.3">
       <c r="J14" s="3"/>
       <c r="K14" s="1"/>
     </row>
-    <row r="15" spans="1:996" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:996" ht="15.6" x14ac:dyDescent="0.3">
       <c r="J15" s="3"/>
       <c r="K15" s="1"/>
     </row>
-    <row r="16" spans="1:996" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:996" ht="15.6" x14ac:dyDescent="0.3">
       <c r="J16" s="3"/>
       <c r="K16" s="1"/>
     </row>
-    <row r="17" spans="10:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="17" spans="10:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="J17" s="3"/>
       <c r="K17" s="1"/>
     </row>
-    <row r="18" spans="10:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="18" spans="10:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="J18" s="3"/>
       <c r="K18" s="1"/>
     </row>
-    <row r="19" spans="10:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="19" spans="10:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="J19" s="3"/>
       <c r="K19" s="1"/>
     </row>
-    <row r="20" spans="10:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="20" spans="10:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="J20" s="3"/>
       <c r="K20" s="1"/>
     </row>
-    <row r="21" spans="10:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="21" spans="10:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="J21" s="3"/>
       <c r="K21" s="1"/>
     </row>
-    <row r="22" spans="10:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="22" spans="10:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="J22" s="3"/>
       <c r="K22" s="1"/>
     </row>
-    <row r="23" spans="10:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="23" spans="10:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="J23" s="3"/>
       <c r="K23" s="1"/>
     </row>
-    <row r="24" spans="10:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="24" spans="10:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="J24" s="3"/>
       <c r="K24" s="1"/>
     </row>
-    <row r="25" spans="10:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="10:11" x14ac:dyDescent="0.3">
       <c r="K25" s="1"/>
     </row>
-    <row r="26" spans="10:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="10:11" x14ac:dyDescent="0.3">
       <c r="K26" s="1"/>
     </row>
-    <row r="27" spans="10:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="10:11" x14ac:dyDescent="0.3">
       <c r="K27" s="1"/>
     </row>
-    <row r="28" spans="10:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="10:11" x14ac:dyDescent="0.3">
       <c r="K28" s="1"/>
     </row>
-    <row r="29" spans="10:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="10:11" x14ac:dyDescent="0.3">
       <c r="K29" s="1"/>
     </row>
-    <row r="30" spans="10:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="10:11" x14ac:dyDescent="0.3">
       <c r="K30" s="1"/>
     </row>
-    <row r="31" spans="10:11" x14ac:dyDescent="0.25">
+    <row r="31" spans="10:11" x14ac:dyDescent="0.3">
       <c r="K31" s="1"/>
     </row>
-    <row r="32" spans="10:11" x14ac:dyDescent="0.25">
+    <row r="32" spans="10:11" x14ac:dyDescent="0.3">
       <c r="K32" s="1"/>
     </row>
-    <row r="33" spans="11:11" x14ac:dyDescent="0.25">
+    <row r="33" spans="11:11" x14ac:dyDescent="0.3">
       <c r="K33" s="1"/>
     </row>
-    <row r="34" spans="11:11" x14ac:dyDescent="0.25">
+    <row r="34" spans="11:11" x14ac:dyDescent="0.3">
       <c r="K34" s="1"/>
     </row>
-    <row r="35" spans="11:11" x14ac:dyDescent="0.25">
+    <row r="35" spans="11:11" x14ac:dyDescent="0.3">
       <c r="K35" s="1"/>
     </row>
-    <row r="36" spans="11:11" x14ac:dyDescent="0.25">
+    <row r="36" spans="11:11" x14ac:dyDescent="0.3">
       <c r="K36" s="1"/>
     </row>
-    <row r="37" spans="11:11" x14ac:dyDescent="0.25">
+    <row r="37" spans="11:11" x14ac:dyDescent="0.3">
       <c r="K37" s="1"/>
     </row>
-    <row r="38" spans="11:11" x14ac:dyDescent="0.25">
+    <row r="38" spans="11:11" x14ac:dyDescent="0.3">
       <c r="K38" s="1"/>
     </row>
-    <row r="39" spans="11:11" x14ac:dyDescent="0.25">
+    <row r="39" spans="11:11" x14ac:dyDescent="0.3">
       <c r="K39" s="1"/>
     </row>
-    <row r="40" spans="11:11" x14ac:dyDescent="0.25">
+    <row r="40" spans="11:11" x14ac:dyDescent="0.3">
       <c r="K40" s="1"/>
     </row>
-    <row r="41" spans="11:11" x14ac:dyDescent="0.25">
+    <row r="41" spans="11:11" x14ac:dyDescent="0.3">
       <c r="K41" s="1"/>
     </row>
   </sheetData>
@@ -8031,7 +8022,7 @@
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="M2" r:id="rId1" xr:uid="{A111A7B2-D9C5-4F09-955C-F59643DB73F8}"/>
+    <hyperlink ref="M2" r:id="rId1" display="AutoTestUNIQUE@gmail.com" xr:uid="{A111A7B2-D9C5-4F09-955C-F59643DB73F8}"/>
   </hyperlinks>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0249999999999999" bottom="1.0249999999999999" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>

</xml_diff>

<commit_message>
Updated test cases and filter keywords
</commit_message>
<xml_diff>
--- a/Testdata/TestData.xlsx
+++ b/Testdata/TestData.xlsx
@@ -5,18 +5,29 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\QualiZeal\POC_project\TurtleMint\tm-auto-code\turtlemint\Testdata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\QualiZeal\POC_project\TurtleMint\result_validation\turtlemint\Testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98765EB1-144F-40F7-A0E3-AFA16DF1A292}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0035991E-4D66-4AE2-9699-09E599BE2048}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="policy" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
     </ext>
@@ -25,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="32">
   <si>
     <t>TC_01</t>
   </si>
@@ -113,12 +124,21 @@
   <si>
     <t>RANDOM_EMAILID</t>
   </si>
+  <si>
+    <t>Self</t>
+  </si>
+  <si>
+    <t>Self-30 years</t>
+  </si>
+  <si>
+    <t>TC_02</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -240,14 +260,6 @@
       <charset val="1"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF4EC9B0"/>
       <name val="Consolas"/>
@@ -355,7 +367,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="19">
+  <cellStyleXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
@@ -374,9 +386,8 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="14" fillId="9" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -384,17 +395,16 @@
     <xf numFmtId="49" fontId="14" fillId="10" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="17" fillId="0" borderId="2" xfId="18" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="15" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="19">
+  <cellStyles count="18">
     <cellStyle name="Accent 1 17" xfId="1" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
     <cellStyle name="Accent 16" xfId="2" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
     <cellStyle name="Accent 2 18" xfId="3" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
@@ -406,7 +416,6 @@
     <cellStyle name="Heading 1 4" xfId="9" xr:uid="{00000000-0005-0000-0000-000008000000}"/>
     <cellStyle name="Heading 2 5" xfId="10" xr:uid="{00000000-0005-0000-0000-000009000000}"/>
     <cellStyle name="Heading 3" xfId="11" xr:uid="{00000000-0005-0000-0000-00000A000000}"/>
-    <cellStyle name="Hyperlink" xfId="18" builtinId="8"/>
     <cellStyle name="Hyperlink 9" xfId="12" xr:uid="{00000000-0005-0000-0000-00000B000000}"/>
     <cellStyle name="Neutral 12" xfId="13" xr:uid="{00000000-0005-0000-0000-00000C000000}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -795,23 +804,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:ALH41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
-      <selection activeCell="L13" sqref="L13"/>
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
+      <selection activeCell="N10" sqref="N10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="11" style="1" customWidth="1"/>
     <col min="2" max="2" width="16.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="59.109375" style="6" customWidth="1"/>
+    <col min="3" max="3" width="59.109375" style="5" customWidth="1"/>
     <col min="4" max="4" width="38.109375" style="1" customWidth="1"/>
     <col min="5" max="5" width="17" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="27.88671875" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="27.88671875" style="1" customWidth="1"/>
     <col min="8" max="8" width="28.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11.44140625" style="1"/>
-    <col min="10" max="10" width="26.6640625" style="6" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="26.6640625" style="6" customWidth="1"/>
+    <col min="10" max="10" width="26.6640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="26.6640625" style="5" customWidth="1"/>
     <col min="12" max="12" width="25.88671875" style="1" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="31.88671875" style="1" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="25.33203125" style="1" bestFit="1" customWidth="1"/>
@@ -828,7 +837,7 @@
       <c r="B1" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="6" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="4" t="s">
@@ -879,17 +888,12 @@
         <v>6</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>8</v>
+        <v>29</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>9</v>
+        <v>30</v>
       </c>
-      <c r="F2" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>25</v>
-      </c>
+      <c r="G2" s="1"/>
       <c r="H2" s="3" t="s">
         <v>7</v>
       </c>
@@ -909,1010 +913,60 @@
         <v>28</v>
       </c>
       <c r="N2" s="3" t="s">
-        <v>20</v>
+        <v>29</v>
       </c>
       <c r="O2" s="3" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:996" s="9" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A3" s="3"/>
-      <c r="B3" s="3"/>
-      <c r="C3" s="5"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="8"/>
-      <c r="G3" s="1"/>
-      <c r="I3" s="1"/>
-      <c r="J3" s="3"/>
-      <c r="K3" s="1"/>
-      <c r="L3" s="1"/>
-      <c r="M3" s="1"/>
-      <c r="N3" s="1"/>
-      <c r="O3" s="1"/>
-      <c r="P3" s="1"/>
-      <c r="Q3" s="1"/>
-      <c r="R3" s="1"/>
-      <c r="S3" s="1"/>
-      <c r="T3" s="1"/>
-      <c r="U3" s="1"/>
-      <c r="V3" s="1"/>
-      <c r="W3" s="1"/>
-      <c r="X3" s="1"/>
-      <c r="Y3" s="1"/>
-      <c r="Z3" s="1"/>
-      <c r="AA3" s="1"/>
-      <c r="AB3" s="1"/>
-      <c r="AC3" s="1"/>
-      <c r="AD3" s="1"/>
-      <c r="AE3" s="1"/>
-      <c r="AF3" s="1"/>
-      <c r="AG3" s="1"/>
-      <c r="AH3" s="1"/>
-      <c r="AI3" s="1"/>
-      <c r="AJ3" s="1"/>
-      <c r="AK3" s="1"/>
-      <c r="AL3" s="1"/>
-      <c r="AM3" s="1"/>
-      <c r="AN3" s="1"/>
-      <c r="AO3" s="1"/>
-      <c r="AP3" s="1"/>
-      <c r="AQ3" s="1"/>
-      <c r="AR3" s="1"/>
-      <c r="AS3" s="1"/>
-      <c r="AT3" s="1"/>
-      <c r="AU3" s="1"/>
-      <c r="AV3" s="1"/>
-      <c r="AW3" s="1"/>
-      <c r="AX3" s="1"/>
-      <c r="AY3" s="1"/>
-      <c r="AZ3" s="1"/>
-      <c r="BA3" s="1"/>
-      <c r="BB3" s="1"/>
-      <c r="BC3" s="1"/>
-      <c r="BD3" s="1"/>
-      <c r="BE3" s="1"/>
-      <c r="BF3" s="1"/>
-      <c r="BG3" s="1"/>
-      <c r="BH3" s="1"/>
-      <c r="BI3" s="1"/>
-      <c r="BJ3" s="1"/>
-      <c r="BK3" s="1"/>
-      <c r="BL3" s="1"/>
-      <c r="BM3" s="1"/>
-      <c r="BN3" s="1"/>
-      <c r="BO3" s="1"/>
-      <c r="BP3" s="1"/>
-      <c r="BQ3" s="1"/>
-      <c r="BR3" s="1"/>
-      <c r="BS3" s="1"/>
-      <c r="BT3" s="1"/>
-      <c r="BU3" s="1"/>
-      <c r="BV3" s="1"/>
-      <c r="BW3" s="1"/>
-      <c r="BX3" s="1"/>
-      <c r="BY3" s="1"/>
-      <c r="BZ3" s="1"/>
-      <c r="CA3" s="1"/>
-      <c r="CB3" s="1"/>
-      <c r="CC3" s="1"/>
-      <c r="CD3" s="1"/>
-      <c r="CE3" s="1"/>
-      <c r="CF3" s="1"/>
-      <c r="CG3" s="1"/>
-      <c r="CH3" s="1"/>
-      <c r="CI3" s="1"/>
-      <c r="CJ3" s="1"/>
-      <c r="CK3" s="1"/>
-      <c r="CL3" s="1"/>
-      <c r="CM3" s="1"/>
-      <c r="CN3" s="1"/>
-      <c r="CO3" s="1"/>
-      <c r="CP3" s="1"/>
-      <c r="CQ3" s="1"/>
-      <c r="CR3" s="1"/>
-      <c r="CS3" s="1"/>
-      <c r="CT3" s="1"/>
-      <c r="CU3" s="1"/>
-      <c r="CV3" s="1"/>
-      <c r="CW3" s="1"/>
-      <c r="CX3" s="1"/>
-      <c r="CY3" s="1"/>
-      <c r="CZ3" s="1"/>
-      <c r="DA3" s="1"/>
-      <c r="DB3" s="1"/>
-      <c r="DC3" s="1"/>
-      <c r="DD3" s="1"/>
-      <c r="DE3" s="1"/>
-      <c r="DF3" s="1"/>
-      <c r="DG3" s="1"/>
-      <c r="DH3" s="1"/>
-      <c r="DI3" s="1"/>
-      <c r="DJ3" s="1"/>
-      <c r="DK3" s="1"/>
-      <c r="DL3" s="1"/>
-      <c r="DM3" s="1"/>
-      <c r="DN3" s="1"/>
-      <c r="DO3" s="1"/>
-      <c r="DP3" s="1"/>
-      <c r="DQ3" s="1"/>
-      <c r="DR3" s="1"/>
-      <c r="DS3" s="1"/>
-      <c r="DT3" s="1"/>
-      <c r="DU3" s="1"/>
-      <c r="DV3" s="1"/>
-      <c r="DW3" s="1"/>
-      <c r="DX3" s="1"/>
-      <c r="DY3" s="1"/>
-      <c r="DZ3" s="1"/>
-      <c r="EA3" s="1"/>
-      <c r="EB3" s="1"/>
-      <c r="EC3" s="1"/>
-      <c r="ED3" s="1"/>
-      <c r="EE3" s="1"/>
-      <c r="EF3" s="1"/>
-      <c r="EG3" s="1"/>
-      <c r="EH3" s="1"/>
-      <c r="EI3" s="1"/>
-      <c r="EJ3" s="1"/>
-      <c r="EK3" s="1"/>
-      <c r="EL3" s="1"/>
-      <c r="EM3" s="1"/>
-      <c r="EN3" s="1"/>
-      <c r="EO3" s="1"/>
-      <c r="EP3" s="1"/>
-      <c r="EQ3" s="1"/>
-      <c r="ER3" s="1"/>
-      <c r="ES3" s="1"/>
-      <c r="ET3" s="1"/>
-      <c r="EU3" s="1"/>
-      <c r="EV3" s="1"/>
-      <c r="EW3" s="1"/>
-      <c r="EX3" s="1"/>
-      <c r="EY3" s="1"/>
-      <c r="EZ3" s="1"/>
-      <c r="FA3" s="1"/>
-      <c r="FB3" s="1"/>
-      <c r="FC3" s="1"/>
-      <c r="FD3" s="1"/>
-      <c r="FE3" s="1"/>
-      <c r="FF3" s="1"/>
-      <c r="FG3" s="1"/>
-      <c r="FH3" s="1"/>
-      <c r="FI3" s="1"/>
-      <c r="FJ3" s="1"/>
-      <c r="FK3" s="1"/>
-      <c r="FL3" s="1"/>
-      <c r="FM3" s="1"/>
-      <c r="FN3" s="1"/>
-      <c r="FO3" s="1"/>
-      <c r="FP3" s="1"/>
-      <c r="FQ3" s="1"/>
-      <c r="FR3" s="1"/>
-      <c r="FS3" s="1"/>
-      <c r="FT3" s="1"/>
-      <c r="FU3" s="1"/>
-      <c r="FV3" s="1"/>
-      <c r="FW3" s="1"/>
-      <c r="FX3" s="1"/>
-      <c r="FY3" s="1"/>
-      <c r="FZ3" s="1"/>
-      <c r="GA3" s="1"/>
-      <c r="GB3" s="1"/>
-      <c r="GC3" s="1"/>
-      <c r="GD3" s="1"/>
-      <c r="GE3" s="1"/>
-      <c r="GF3" s="1"/>
-      <c r="GG3" s="1"/>
-      <c r="GH3" s="1"/>
-      <c r="GI3" s="1"/>
-      <c r="GJ3" s="1"/>
-      <c r="GK3" s="1"/>
-      <c r="GL3" s="1"/>
-      <c r="GM3" s="1"/>
-      <c r="GN3" s="1"/>
-      <c r="GO3" s="1"/>
-      <c r="GP3" s="1"/>
-      <c r="GQ3" s="1"/>
-      <c r="GR3" s="1"/>
-      <c r="GS3" s="1"/>
-      <c r="GT3" s="1"/>
-      <c r="GU3" s="1"/>
-      <c r="GV3" s="1"/>
-      <c r="GW3" s="1"/>
-      <c r="GX3" s="1"/>
-      <c r="GY3" s="1"/>
-      <c r="GZ3" s="1"/>
-      <c r="HA3" s="1"/>
-      <c r="HB3" s="1"/>
-      <c r="HC3" s="1"/>
-      <c r="HD3" s="1"/>
-      <c r="HE3" s="1"/>
-      <c r="HF3" s="1"/>
-      <c r="HG3" s="1"/>
-      <c r="HH3" s="1"/>
-      <c r="HI3" s="1"/>
-      <c r="HJ3" s="1"/>
-      <c r="HK3" s="1"/>
-      <c r="HL3" s="1"/>
-      <c r="HM3" s="1"/>
-      <c r="HN3" s="1"/>
-      <c r="HO3" s="1"/>
-      <c r="HP3" s="1"/>
-      <c r="HQ3" s="1"/>
-      <c r="HR3" s="1"/>
-      <c r="HS3" s="1"/>
-      <c r="HT3" s="1"/>
-      <c r="HU3" s="1"/>
-      <c r="HV3" s="1"/>
-      <c r="HW3" s="1"/>
-      <c r="HX3" s="1"/>
-      <c r="HY3" s="1"/>
-      <c r="HZ3" s="1"/>
-      <c r="IA3" s="1"/>
-      <c r="IB3" s="1"/>
-      <c r="IC3" s="1"/>
-      <c r="ID3" s="1"/>
-      <c r="IE3" s="1"/>
-      <c r="IF3" s="1"/>
-      <c r="IG3" s="1"/>
-      <c r="IH3" s="1"/>
-      <c r="II3" s="1"/>
-      <c r="IJ3" s="1"/>
-      <c r="IK3" s="1"/>
-      <c r="IL3" s="1"/>
-      <c r="IM3" s="1"/>
-      <c r="IN3" s="1"/>
-      <c r="IO3" s="1"/>
-      <c r="IP3" s="1"/>
-      <c r="IQ3" s="1"/>
-      <c r="IR3" s="1"/>
-      <c r="IS3" s="1"/>
-      <c r="IT3" s="1"/>
-      <c r="IU3" s="1"/>
-      <c r="IV3" s="1"/>
-      <c r="IW3" s="1"/>
-      <c r="IX3" s="1"/>
-      <c r="IY3" s="1"/>
-      <c r="IZ3" s="1"/>
-      <c r="JA3" s="1"/>
-      <c r="JB3" s="1"/>
-      <c r="JC3" s="1"/>
-      <c r="JD3" s="1"/>
-      <c r="JE3" s="1"/>
-      <c r="JF3" s="1"/>
-      <c r="JG3" s="1"/>
-      <c r="JH3" s="1"/>
-      <c r="JI3" s="1"/>
-      <c r="JJ3" s="1"/>
-      <c r="JK3" s="1"/>
-      <c r="JL3" s="1"/>
-      <c r="JM3" s="1"/>
-      <c r="JN3" s="1"/>
-      <c r="JO3" s="1"/>
-      <c r="JP3" s="1"/>
-      <c r="JQ3" s="1"/>
-      <c r="JR3" s="1"/>
-      <c r="JS3" s="1"/>
-      <c r="JT3" s="1"/>
-      <c r="JU3" s="1"/>
-      <c r="JV3" s="1"/>
-      <c r="JW3" s="1"/>
-      <c r="JX3" s="1"/>
-      <c r="JY3" s="1"/>
-      <c r="JZ3" s="1"/>
-      <c r="KA3" s="1"/>
-      <c r="KB3" s="1"/>
-      <c r="KC3" s="1"/>
-      <c r="KD3" s="1"/>
-      <c r="KE3" s="1"/>
-      <c r="KF3" s="1"/>
-      <c r="KG3" s="1"/>
-      <c r="KH3" s="1"/>
-      <c r="KI3" s="1"/>
-      <c r="KJ3" s="1"/>
-      <c r="KK3" s="1"/>
-      <c r="KL3" s="1"/>
-      <c r="KM3" s="1"/>
-      <c r="KN3" s="1"/>
-      <c r="KO3" s="1"/>
-      <c r="KP3" s="1"/>
-      <c r="KQ3" s="1"/>
-      <c r="KR3" s="1"/>
-      <c r="KS3" s="1"/>
-      <c r="KT3" s="1"/>
-      <c r="KU3" s="1"/>
-      <c r="KV3" s="1"/>
-      <c r="KW3" s="1"/>
-      <c r="KX3" s="1"/>
-      <c r="KY3" s="1"/>
-      <c r="KZ3" s="1"/>
-      <c r="LA3" s="1"/>
-      <c r="LB3" s="1"/>
-      <c r="LC3" s="1"/>
-      <c r="LD3" s="1"/>
-      <c r="LE3" s="1"/>
-      <c r="LF3" s="1"/>
-      <c r="LG3" s="1"/>
-      <c r="LH3" s="1"/>
-      <c r="LI3" s="1"/>
-      <c r="LJ3" s="1"/>
-      <c r="LK3" s="1"/>
-      <c r="LL3" s="1"/>
-      <c r="LM3" s="1"/>
-      <c r="LN3" s="1"/>
-      <c r="LO3" s="1"/>
-      <c r="LP3" s="1"/>
-      <c r="LQ3" s="1"/>
-      <c r="LR3" s="1"/>
-      <c r="LS3" s="1"/>
-      <c r="LT3" s="1"/>
-      <c r="LU3" s="1"/>
-      <c r="LV3" s="1"/>
-      <c r="LW3" s="1"/>
-      <c r="LX3" s="1"/>
-      <c r="LY3" s="1"/>
-      <c r="LZ3" s="1"/>
-      <c r="MA3" s="1"/>
-      <c r="MB3" s="1"/>
-      <c r="MC3" s="1"/>
-      <c r="MD3" s="1"/>
-      <c r="ME3" s="1"/>
-      <c r="MF3" s="1"/>
-      <c r="MG3" s="1"/>
-      <c r="MH3" s="1"/>
-      <c r="MI3" s="1"/>
-      <c r="MJ3" s="1"/>
-      <c r="MK3" s="1"/>
-      <c r="ML3" s="1"/>
-      <c r="MM3" s="1"/>
-      <c r="MN3" s="1"/>
-      <c r="MO3" s="1"/>
-      <c r="MP3" s="1"/>
-      <c r="MQ3" s="1"/>
-      <c r="MR3" s="1"/>
-      <c r="MS3" s="1"/>
-      <c r="MT3" s="1"/>
-      <c r="MU3" s="1"/>
-      <c r="MV3" s="1"/>
-      <c r="MW3" s="1"/>
-      <c r="MX3" s="1"/>
-      <c r="MY3" s="1"/>
-      <c r="MZ3" s="1"/>
-      <c r="NA3" s="1"/>
-      <c r="NB3" s="1"/>
-      <c r="NC3" s="1"/>
-      <c r="ND3" s="1"/>
-      <c r="NE3" s="1"/>
-      <c r="NF3" s="1"/>
-      <c r="NG3" s="1"/>
-      <c r="NH3" s="1"/>
-      <c r="NI3" s="1"/>
-      <c r="NJ3" s="1"/>
-      <c r="NK3" s="1"/>
-      <c r="NL3" s="1"/>
-      <c r="NM3" s="1"/>
-      <c r="NN3" s="1"/>
-      <c r="NO3" s="1"/>
-      <c r="NP3" s="1"/>
-      <c r="NQ3" s="1"/>
-      <c r="NR3" s="1"/>
-      <c r="NS3" s="1"/>
-      <c r="NT3" s="1"/>
-      <c r="NU3" s="1"/>
-      <c r="NV3" s="1"/>
-      <c r="NW3" s="1"/>
-      <c r="NX3" s="1"/>
-      <c r="NY3" s="1"/>
-      <c r="NZ3" s="1"/>
-      <c r="OA3" s="1"/>
-      <c r="OB3" s="1"/>
-      <c r="OC3" s="1"/>
-      <c r="OD3" s="1"/>
-      <c r="OE3" s="1"/>
-      <c r="OF3" s="1"/>
-      <c r="OG3" s="1"/>
-      <c r="OH3" s="1"/>
-      <c r="OI3" s="1"/>
-      <c r="OJ3" s="1"/>
-      <c r="OK3" s="1"/>
-      <c r="OL3" s="1"/>
-      <c r="OM3" s="1"/>
-      <c r="ON3" s="1"/>
-      <c r="OO3" s="1"/>
-      <c r="OP3" s="1"/>
-      <c r="OQ3" s="1"/>
-      <c r="OR3" s="1"/>
-      <c r="OS3" s="1"/>
-      <c r="OT3" s="1"/>
-      <c r="OU3" s="1"/>
-      <c r="OV3" s="1"/>
-      <c r="OW3" s="1"/>
-      <c r="OX3" s="1"/>
-      <c r="OY3" s="1"/>
-      <c r="OZ3" s="1"/>
-      <c r="PA3" s="1"/>
-      <c r="PB3" s="1"/>
-      <c r="PC3" s="1"/>
-      <c r="PD3" s="1"/>
-      <c r="PE3" s="1"/>
-      <c r="PF3" s="1"/>
-      <c r="PG3" s="1"/>
-      <c r="PH3" s="1"/>
-      <c r="PI3" s="1"/>
-      <c r="PJ3" s="1"/>
-      <c r="PK3" s="1"/>
-      <c r="PL3" s="1"/>
-      <c r="PM3" s="1"/>
-      <c r="PN3" s="1"/>
-      <c r="PO3" s="1"/>
-      <c r="PP3" s="1"/>
-      <c r="PQ3" s="1"/>
-      <c r="PR3" s="1"/>
-      <c r="PS3" s="1"/>
-      <c r="PT3" s="1"/>
-      <c r="PU3" s="1"/>
-      <c r="PV3" s="1"/>
-      <c r="PW3" s="1"/>
-      <c r="PX3" s="1"/>
-      <c r="PY3" s="1"/>
-      <c r="PZ3" s="1"/>
-      <c r="QA3" s="1"/>
-      <c r="QB3" s="1"/>
-      <c r="QC3" s="1"/>
-      <c r="QD3" s="1"/>
-      <c r="QE3" s="1"/>
-      <c r="QF3" s="1"/>
-      <c r="QG3" s="1"/>
-      <c r="QH3" s="1"/>
-      <c r="QI3" s="1"/>
-      <c r="QJ3" s="1"/>
-      <c r="QK3" s="1"/>
-      <c r="QL3" s="1"/>
-      <c r="QM3" s="1"/>
-      <c r="QN3" s="1"/>
-      <c r="QO3" s="1"/>
-      <c r="QP3" s="1"/>
-      <c r="QQ3" s="1"/>
-      <c r="QR3" s="1"/>
-      <c r="QS3" s="1"/>
-      <c r="QT3" s="1"/>
-      <c r="QU3" s="1"/>
-      <c r="QV3" s="1"/>
-      <c r="QW3" s="1"/>
-      <c r="QX3" s="1"/>
-      <c r="QY3" s="1"/>
-      <c r="QZ3" s="1"/>
-      <c r="RA3" s="1"/>
-      <c r="RB3" s="1"/>
-      <c r="RC3" s="1"/>
-      <c r="RD3" s="1"/>
-      <c r="RE3" s="1"/>
-      <c r="RF3" s="1"/>
-      <c r="RG3" s="1"/>
-      <c r="RH3" s="1"/>
-      <c r="RI3" s="1"/>
-      <c r="RJ3" s="1"/>
-      <c r="RK3" s="1"/>
-      <c r="RL3" s="1"/>
-      <c r="RM3" s="1"/>
-      <c r="RN3" s="1"/>
-      <c r="RO3" s="1"/>
-      <c r="RP3" s="1"/>
-      <c r="RQ3" s="1"/>
-      <c r="RR3" s="1"/>
-      <c r="RS3" s="1"/>
-      <c r="RT3" s="1"/>
-      <c r="RU3" s="1"/>
-      <c r="RV3" s="1"/>
-      <c r="RW3" s="1"/>
-      <c r="RX3" s="1"/>
-      <c r="RY3" s="1"/>
-      <c r="RZ3" s="1"/>
-      <c r="SA3" s="1"/>
-      <c r="SB3" s="1"/>
-      <c r="SC3" s="1"/>
-      <c r="SD3" s="1"/>
-      <c r="SE3" s="1"/>
-      <c r="SF3" s="1"/>
-      <c r="SG3" s="1"/>
-      <c r="SH3" s="1"/>
-      <c r="SI3" s="1"/>
-      <c r="SJ3" s="1"/>
-      <c r="SK3" s="1"/>
-      <c r="SL3" s="1"/>
-      <c r="SM3" s="1"/>
-      <c r="SN3" s="1"/>
-      <c r="SO3" s="1"/>
-      <c r="SP3" s="1"/>
-      <c r="SQ3" s="1"/>
-      <c r="SR3" s="1"/>
-      <c r="SS3" s="1"/>
-      <c r="ST3" s="1"/>
-      <c r="SU3" s="1"/>
-      <c r="SV3" s="1"/>
-      <c r="SW3" s="1"/>
-      <c r="SX3" s="1"/>
-      <c r="SY3" s="1"/>
-      <c r="SZ3" s="1"/>
-      <c r="TA3" s="1"/>
-      <c r="TB3" s="1"/>
-      <c r="TC3" s="1"/>
-      <c r="TD3" s="1"/>
-      <c r="TE3" s="1"/>
-      <c r="TF3" s="1"/>
-      <c r="TG3" s="1"/>
-      <c r="TH3" s="1"/>
-      <c r="TI3" s="1"/>
-      <c r="TJ3" s="1"/>
-      <c r="TK3" s="1"/>
-      <c r="TL3" s="1"/>
-      <c r="TM3" s="1"/>
-      <c r="TN3" s="1"/>
-      <c r="TO3" s="1"/>
-      <c r="TP3" s="1"/>
-      <c r="TQ3" s="1"/>
-      <c r="TR3" s="1"/>
-      <c r="TS3" s="1"/>
-      <c r="TT3" s="1"/>
-      <c r="TU3" s="1"/>
-      <c r="TV3" s="1"/>
-      <c r="TW3" s="1"/>
-      <c r="TX3" s="1"/>
-      <c r="TY3" s="1"/>
-      <c r="TZ3" s="1"/>
-      <c r="UA3" s="1"/>
-      <c r="UB3" s="1"/>
-      <c r="UC3" s="1"/>
-      <c r="UD3" s="1"/>
-      <c r="UE3" s="1"/>
-      <c r="UF3" s="1"/>
-      <c r="UG3" s="1"/>
-      <c r="UH3" s="1"/>
-      <c r="UI3" s="1"/>
-      <c r="UJ3" s="1"/>
-      <c r="UK3" s="1"/>
-      <c r="UL3" s="1"/>
-      <c r="UM3" s="1"/>
-      <c r="UN3" s="1"/>
-      <c r="UO3" s="1"/>
-      <c r="UP3" s="1"/>
-      <c r="UQ3" s="1"/>
-      <c r="UR3" s="1"/>
-      <c r="US3" s="1"/>
-      <c r="UT3" s="1"/>
-      <c r="UU3" s="1"/>
-      <c r="UV3" s="1"/>
-      <c r="UW3" s="1"/>
-      <c r="UX3" s="1"/>
-      <c r="UY3" s="1"/>
-      <c r="UZ3" s="1"/>
-      <c r="VA3" s="1"/>
-      <c r="VB3" s="1"/>
-      <c r="VC3" s="1"/>
-      <c r="VD3" s="1"/>
-      <c r="VE3" s="1"/>
-      <c r="VF3" s="1"/>
-      <c r="VG3" s="1"/>
-      <c r="VH3" s="1"/>
-      <c r="VI3" s="1"/>
-      <c r="VJ3" s="1"/>
-      <c r="VK3" s="1"/>
-      <c r="VL3" s="1"/>
-      <c r="VM3" s="1"/>
-      <c r="VN3" s="1"/>
-      <c r="VO3" s="1"/>
-      <c r="VP3" s="1"/>
-      <c r="VQ3" s="1"/>
-      <c r="VR3" s="1"/>
-      <c r="VS3" s="1"/>
-      <c r="VT3" s="1"/>
-      <c r="VU3" s="1"/>
-      <c r="VV3" s="1"/>
-      <c r="VW3" s="1"/>
-      <c r="VX3" s="1"/>
-      <c r="VY3" s="1"/>
-      <c r="VZ3" s="1"/>
-      <c r="WA3" s="1"/>
-      <c r="WB3" s="1"/>
-      <c r="WC3" s="1"/>
-      <c r="WD3" s="1"/>
-      <c r="WE3" s="1"/>
-      <c r="WF3" s="1"/>
-      <c r="WG3" s="1"/>
-      <c r="WH3" s="1"/>
-      <c r="WI3" s="1"/>
-      <c r="WJ3" s="1"/>
-      <c r="WK3" s="1"/>
-      <c r="WL3" s="1"/>
-      <c r="WM3" s="1"/>
-      <c r="WN3" s="1"/>
-      <c r="WO3" s="1"/>
-      <c r="WP3" s="1"/>
-      <c r="WQ3" s="1"/>
-      <c r="WR3" s="1"/>
-      <c r="WS3" s="1"/>
-      <c r="WT3" s="1"/>
-      <c r="WU3" s="1"/>
-      <c r="WV3" s="1"/>
-      <c r="WW3" s="1"/>
-      <c r="WX3" s="1"/>
-      <c r="WY3" s="1"/>
-      <c r="WZ3" s="1"/>
-      <c r="XA3" s="1"/>
-      <c r="XB3" s="1"/>
-      <c r="XC3" s="1"/>
-      <c r="XD3" s="1"/>
-      <c r="XE3" s="1"/>
-      <c r="XF3" s="1"/>
-      <c r="XG3" s="1"/>
-      <c r="XH3" s="1"/>
-      <c r="XI3" s="1"/>
-      <c r="XJ3" s="1"/>
-      <c r="XK3" s="1"/>
-      <c r="XL3" s="1"/>
-      <c r="XM3" s="1"/>
-      <c r="XN3" s="1"/>
-      <c r="XO3" s="1"/>
-      <c r="XP3" s="1"/>
-      <c r="XQ3" s="1"/>
-      <c r="XR3" s="1"/>
-      <c r="XS3" s="1"/>
-      <c r="XT3" s="1"/>
-      <c r="XU3" s="1"/>
-      <c r="XV3" s="1"/>
-      <c r="XW3" s="1"/>
-      <c r="XX3" s="1"/>
-      <c r="XY3" s="1"/>
-      <c r="XZ3" s="1"/>
-      <c r="YA3" s="1"/>
-      <c r="YB3" s="1"/>
-      <c r="YC3" s="1"/>
-      <c r="YD3" s="1"/>
-      <c r="YE3" s="1"/>
-      <c r="YF3" s="1"/>
-      <c r="YG3" s="1"/>
-      <c r="YH3" s="1"/>
-      <c r="YI3" s="1"/>
-      <c r="YJ3" s="1"/>
-      <c r="YK3" s="1"/>
-      <c r="YL3" s="1"/>
-      <c r="YM3" s="1"/>
-      <c r="YN3" s="1"/>
-      <c r="YO3" s="1"/>
-      <c r="YP3" s="1"/>
-      <c r="YQ3" s="1"/>
-      <c r="YR3" s="1"/>
-      <c r="YS3" s="1"/>
-      <c r="YT3" s="1"/>
-      <c r="YU3" s="1"/>
-      <c r="YV3" s="1"/>
-      <c r="YW3" s="1"/>
-      <c r="YX3" s="1"/>
-      <c r="YY3" s="1"/>
-      <c r="YZ3" s="1"/>
-      <c r="ZA3" s="1"/>
-      <c r="ZB3" s="1"/>
-      <c r="ZC3" s="1"/>
-      <c r="ZD3" s="1"/>
-      <c r="ZE3" s="1"/>
-      <c r="ZF3" s="1"/>
-      <c r="ZG3" s="1"/>
-      <c r="ZH3" s="1"/>
-      <c r="ZI3" s="1"/>
-      <c r="ZJ3" s="1"/>
-      <c r="ZK3" s="1"/>
-      <c r="ZL3" s="1"/>
-      <c r="ZM3" s="1"/>
-      <c r="ZN3" s="1"/>
-      <c r="ZO3" s="1"/>
-      <c r="ZP3" s="1"/>
-      <c r="ZQ3" s="1"/>
-      <c r="ZR3" s="1"/>
-      <c r="ZS3" s="1"/>
-      <c r="ZT3" s="1"/>
-      <c r="ZU3" s="1"/>
-      <c r="ZV3" s="1"/>
-      <c r="ZW3" s="1"/>
-      <c r="ZX3" s="1"/>
-      <c r="ZY3" s="1"/>
-      <c r="ZZ3" s="1"/>
-      <c r="AAA3" s="1"/>
-      <c r="AAB3" s="1"/>
-      <c r="AAC3" s="1"/>
-      <c r="AAD3" s="1"/>
-      <c r="AAE3" s="1"/>
-      <c r="AAF3" s="1"/>
-      <c r="AAG3" s="1"/>
-      <c r="AAH3" s="1"/>
-      <c r="AAI3" s="1"/>
-      <c r="AAJ3" s="1"/>
-      <c r="AAK3" s="1"/>
-      <c r="AAL3" s="1"/>
-      <c r="AAM3" s="1"/>
-      <c r="AAN3" s="1"/>
-      <c r="AAO3" s="1"/>
-      <c r="AAP3" s="1"/>
-      <c r="AAQ3" s="1"/>
-      <c r="AAR3" s="1"/>
-      <c r="AAS3" s="1"/>
-      <c r="AAT3" s="1"/>
-      <c r="AAU3" s="1"/>
-      <c r="AAV3" s="1"/>
-      <c r="AAW3" s="1"/>
-      <c r="AAX3" s="1"/>
-      <c r="AAY3" s="1"/>
-      <c r="AAZ3" s="1"/>
-      <c r="ABA3" s="1"/>
-      <c r="ABB3" s="1"/>
-      <c r="ABC3" s="1"/>
-      <c r="ABD3" s="1"/>
-      <c r="ABE3" s="1"/>
-      <c r="ABF3" s="1"/>
-      <c r="ABG3" s="1"/>
-      <c r="ABH3" s="1"/>
-      <c r="ABI3" s="1"/>
-      <c r="ABJ3" s="1"/>
-      <c r="ABK3" s="1"/>
-      <c r="ABL3" s="1"/>
-      <c r="ABM3" s="1"/>
-      <c r="ABN3" s="1"/>
-      <c r="ABO3" s="1"/>
-      <c r="ABP3" s="1"/>
-      <c r="ABQ3" s="1"/>
-      <c r="ABR3" s="1"/>
-      <c r="ABS3" s="1"/>
-      <c r="ABT3" s="1"/>
-      <c r="ABU3" s="1"/>
-      <c r="ABV3" s="1"/>
-      <c r="ABW3" s="1"/>
-      <c r="ABX3" s="1"/>
-      <c r="ABY3" s="1"/>
-      <c r="ABZ3" s="1"/>
-      <c r="ACA3" s="1"/>
-      <c r="ACB3" s="1"/>
-      <c r="ACC3" s="1"/>
-      <c r="ACD3" s="1"/>
-      <c r="ACE3" s="1"/>
-      <c r="ACF3" s="1"/>
-      <c r="ACG3" s="1"/>
-      <c r="ACH3" s="1"/>
-      <c r="ACI3" s="1"/>
-      <c r="ACJ3" s="1"/>
-      <c r="ACK3" s="1"/>
-      <c r="ACL3" s="1"/>
-      <c r="ACM3" s="1"/>
-      <c r="ACN3" s="1"/>
-      <c r="ACO3" s="1"/>
-      <c r="ACP3" s="1"/>
-      <c r="ACQ3" s="1"/>
-      <c r="ACR3" s="1"/>
-      <c r="ACS3" s="1"/>
-      <c r="ACT3" s="1"/>
-      <c r="ACU3" s="1"/>
-      <c r="ACV3" s="1"/>
-      <c r="ACW3" s="1"/>
-      <c r="ACX3" s="1"/>
-      <c r="ACY3" s="1"/>
-      <c r="ACZ3" s="1"/>
-      <c r="ADA3" s="1"/>
-      <c r="ADB3" s="1"/>
-      <c r="ADC3" s="1"/>
-      <c r="ADD3" s="1"/>
-      <c r="ADE3" s="1"/>
-      <c r="ADF3" s="1"/>
-      <c r="ADG3" s="1"/>
-      <c r="ADH3" s="1"/>
-      <c r="ADI3" s="1"/>
-      <c r="ADJ3" s="1"/>
-      <c r="ADK3" s="1"/>
-      <c r="ADL3" s="1"/>
-      <c r="ADM3" s="1"/>
-      <c r="ADN3" s="1"/>
-      <c r="ADO3" s="1"/>
-      <c r="ADP3" s="1"/>
-      <c r="ADQ3" s="1"/>
-      <c r="ADR3" s="1"/>
-      <c r="ADS3" s="1"/>
-      <c r="ADT3" s="1"/>
-      <c r="ADU3" s="1"/>
-      <c r="ADV3" s="1"/>
-      <c r="ADW3" s="1"/>
-      <c r="ADX3" s="1"/>
-      <c r="ADY3" s="1"/>
-      <c r="ADZ3" s="1"/>
-      <c r="AEA3" s="1"/>
-      <c r="AEB3" s="1"/>
-      <c r="AEC3" s="1"/>
-      <c r="AED3" s="1"/>
-      <c r="AEE3" s="1"/>
-      <c r="AEF3" s="1"/>
-      <c r="AEG3" s="1"/>
-      <c r="AEH3" s="1"/>
-      <c r="AEI3" s="1"/>
-      <c r="AEJ3" s="1"/>
-      <c r="AEK3" s="1"/>
-      <c r="AEL3" s="1"/>
-      <c r="AEM3" s="1"/>
-      <c r="AEN3" s="1"/>
-      <c r="AEO3" s="1"/>
-      <c r="AEP3" s="1"/>
-      <c r="AEQ3" s="1"/>
-      <c r="AER3" s="1"/>
-      <c r="AES3" s="1"/>
-      <c r="AET3" s="1"/>
-      <c r="AEU3" s="1"/>
-      <c r="AEV3" s="1"/>
-      <c r="AEW3" s="1"/>
-      <c r="AEX3" s="1"/>
-      <c r="AEY3" s="1"/>
-      <c r="AEZ3" s="1"/>
-      <c r="AFA3" s="1"/>
-      <c r="AFB3" s="1"/>
-      <c r="AFC3" s="1"/>
-      <c r="AFD3" s="1"/>
-      <c r="AFE3" s="1"/>
-      <c r="AFF3" s="1"/>
-      <c r="AFG3" s="1"/>
-      <c r="AFH3" s="1"/>
-      <c r="AFI3" s="1"/>
-      <c r="AFJ3" s="1"/>
-      <c r="AFK3" s="1"/>
-      <c r="AFL3" s="1"/>
-      <c r="AFM3" s="1"/>
-      <c r="AFN3" s="1"/>
-      <c r="AFO3" s="1"/>
-      <c r="AFP3" s="1"/>
-      <c r="AFQ3" s="1"/>
-      <c r="AFR3" s="1"/>
-      <c r="AFS3" s="1"/>
-      <c r="AFT3" s="1"/>
-      <c r="AFU3" s="1"/>
-      <c r="AFV3" s="1"/>
-      <c r="AFW3" s="1"/>
-      <c r="AFX3" s="1"/>
-      <c r="AFY3" s="1"/>
-      <c r="AFZ3" s="1"/>
-      <c r="AGA3" s="1"/>
-      <c r="AGB3" s="1"/>
-      <c r="AGC3" s="1"/>
-      <c r="AGD3" s="1"/>
-      <c r="AGE3" s="1"/>
-      <c r="AGF3" s="1"/>
-      <c r="AGG3" s="1"/>
-      <c r="AGH3" s="1"/>
-      <c r="AGI3" s="1"/>
-      <c r="AGJ3" s="1"/>
-      <c r="AGK3" s="1"/>
-      <c r="AGL3" s="1"/>
-      <c r="AGM3" s="1"/>
-      <c r="AGN3" s="1"/>
-      <c r="AGO3" s="1"/>
-      <c r="AGP3" s="1"/>
-      <c r="AGQ3" s="1"/>
-      <c r="AGR3" s="1"/>
-      <c r="AGS3" s="1"/>
-      <c r="AGT3" s="1"/>
-      <c r="AGU3" s="1"/>
-      <c r="AGV3" s="1"/>
-      <c r="AGW3" s="1"/>
-      <c r="AGX3" s="1"/>
-      <c r="AGY3" s="1"/>
-      <c r="AGZ3" s="1"/>
-      <c r="AHA3" s="1"/>
-      <c r="AHB3" s="1"/>
-      <c r="AHC3" s="1"/>
-      <c r="AHD3" s="1"/>
-      <c r="AHE3" s="1"/>
-      <c r="AHF3" s="1"/>
-      <c r="AHG3" s="1"/>
-      <c r="AHH3" s="1"/>
-      <c r="AHI3" s="1"/>
-      <c r="AHJ3" s="1"/>
-      <c r="AHK3" s="1"/>
-      <c r="AHL3" s="1"/>
-      <c r="AHM3" s="1"/>
-      <c r="AHN3" s="1"/>
-      <c r="AHO3" s="1"/>
-      <c r="AHP3" s="1"/>
-      <c r="AHQ3" s="1"/>
-      <c r="AHR3" s="1"/>
-      <c r="AHS3" s="1"/>
-      <c r="AHT3" s="1"/>
-      <c r="AHU3" s="1"/>
-      <c r="AHV3" s="1"/>
-      <c r="AHW3" s="1"/>
-      <c r="AHX3" s="1"/>
-      <c r="AHY3" s="1"/>
-      <c r="AHZ3" s="1"/>
-      <c r="AIA3" s="1"/>
-      <c r="AIB3" s="1"/>
-      <c r="AIC3" s="1"/>
-      <c r="AID3" s="1"/>
-      <c r="AIE3" s="1"/>
-      <c r="AIF3" s="1"/>
-      <c r="AIG3" s="1"/>
-      <c r="AIH3" s="1"/>
-      <c r="AII3" s="1"/>
-      <c r="AIJ3" s="1"/>
-      <c r="AIK3" s="1"/>
-      <c r="AIL3" s="1"/>
-      <c r="AIM3" s="1"/>
-      <c r="AIN3" s="1"/>
-      <c r="AIO3" s="1"/>
-      <c r="AIP3" s="1"/>
-      <c r="AIQ3" s="1"/>
-      <c r="AIR3" s="1"/>
-      <c r="AIS3" s="1"/>
-      <c r="AIT3" s="1"/>
-      <c r="AIU3" s="1"/>
-      <c r="AIV3" s="1"/>
-      <c r="AIW3" s="1"/>
-      <c r="AIX3" s="1"/>
-      <c r="AIY3" s="1"/>
-      <c r="AIZ3" s="1"/>
-      <c r="AJA3" s="1"/>
-      <c r="AJB3" s="1"/>
-      <c r="AJC3" s="1"/>
-      <c r="AJD3" s="1"/>
-      <c r="AJE3" s="1"/>
-      <c r="AJF3" s="1"/>
-      <c r="AJG3" s="1"/>
-      <c r="AJH3" s="1"/>
-      <c r="AJI3" s="1"/>
-      <c r="AJJ3" s="1"/>
-      <c r="AJK3" s="1"/>
-      <c r="AJL3" s="1"/>
-      <c r="AJM3" s="1"/>
-      <c r="AJN3" s="1"/>
-      <c r="AJO3" s="1"/>
-      <c r="AJP3" s="1"/>
-      <c r="AJQ3" s="1"/>
-      <c r="AJR3" s="1"/>
-      <c r="AJS3" s="1"/>
-      <c r="AJT3" s="1"/>
-      <c r="AJU3" s="1"/>
-      <c r="AJV3" s="1"/>
-      <c r="AJW3" s="1"/>
-      <c r="AJX3" s="1"/>
-      <c r="AJY3" s="1"/>
-      <c r="AJZ3" s="1"/>
-      <c r="AKA3" s="1"/>
-      <c r="AKB3" s="1"/>
-      <c r="AKC3" s="1"/>
-      <c r="AKD3" s="1"/>
-      <c r="AKE3" s="1"/>
-      <c r="AKF3" s="1"/>
-      <c r="AKG3" s="1"/>
-      <c r="AKH3" s="1"/>
-      <c r="AKI3" s="1"/>
-      <c r="AKJ3" s="1"/>
-      <c r="AKK3" s="1"/>
-      <c r="AKL3" s="1"/>
-      <c r="AKM3" s="1"/>
-      <c r="AKN3" s="1"/>
-      <c r="AKO3" s="1"/>
-      <c r="AKP3" s="1"/>
-      <c r="AKQ3" s="1"/>
-      <c r="AKR3" s="1"/>
-      <c r="AKS3" s="1"/>
-      <c r="AKT3" s="1"/>
-      <c r="AKU3" s="1"/>
-      <c r="AKV3" s="1"/>
-      <c r="AKW3" s="1"/>
-      <c r="AKX3" s="1"/>
-      <c r="AKY3" s="1"/>
-      <c r="AKZ3" s="1"/>
-      <c r="ALA3" s="1"/>
-      <c r="ALB3" s="1"/>
-      <c r="ALC3" s="1"/>
-      <c r="ALD3" s="1"/>
-      <c r="ALE3" s="1"/>
-      <c r="ALF3" s="1"/>
-      <c r="ALG3" s="1"/>
-      <c r="ALH3" s="1"/>
+    <row r="3" spans="1:996" s="3" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A3" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="K3" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="L3" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="M3" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="N3" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="O3" s="3" t="s">
+        <v>22</v>
+      </c>
     </row>
-    <row r="4" spans="1:996" s="9" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:996" s="8" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
@@ -2910,12 +1964,12 @@
       <c r="ALG4" s="1"/>
       <c r="ALH4" s="1"/>
     </row>
-    <row r="5" spans="1:996" s="9" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:996" s="8" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
-      <c r="E5" s="8"/>
+      <c r="E5" s="7"/>
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
@@ -3908,7 +2962,7 @@
       <c r="ALG5" s="1"/>
       <c r="ALH5" s="1"/>
     </row>
-    <row r="6" spans="1:996" s="9" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:996" s="8" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
@@ -4906,7 +3960,7 @@
       <c r="ALG6" s="1"/>
       <c r="ALH6" s="1"/>
     </row>
-    <row r="7" spans="1:996" s="9" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:996" s="8" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -4914,7 +3968,7 @@
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
-      <c r="H7" s="8"/>
+      <c r="H7" s="7"/>
       <c r="I7" s="1"/>
       <c r="J7" s="3"/>
       <c r="K7" s="1"/>
@@ -5904,7 +4958,7 @@
       <c r="ALG7" s="1"/>
       <c r="ALH7" s="1"/>
     </row>
-    <row r="8" spans="1:996" s="9" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:996" s="8" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
@@ -6902,7 +5956,7 @@
       <c r="ALG8" s="1"/>
       <c r="ALH8" s="1"/>
     </row>
-    <row r="9" spans="1:996" s="9" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:996" s="8" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
@@ -8023,9 +7077,10 @@
   </dataValidations>
   <hyperlinks>
     <hyperlink ref="M2" r:id="rId1" display="AutoTestUNIQUE@gmail.com" xr:uid="{A111A7B2-D9C5-4F09-955C-F59643DB73F8}"/>
+    <hyperlink ref="M3" r:id="rId2" display="AutoTestUNIQUE@gmail.com" xr:uid="{E03CF3A7-FFD0-4A31-A7BD-E78667BCB249}"/>
   </hyperlinks>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0249999999999999" bottom="1.0249999999999999" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+  <pageSetup orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300" r:id="rId3"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;"Arial,Regular"&amp;10&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Arial,Regular"&amp;10Page &amp;P</oddFooter>

</xml_diff>

<commit_message>
Added test data fro life
</commit_message>
<xml_diff>
--- a/Testdata/TestData.xlsx
+++ b/Testdata/TestData.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\poc_new\turtlemint\Testdata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\QualiZeal\POC_project\TurtleMint\result_validation\turtlemint\Testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4435B19F-1DE1-4327-BA2E-96AA8DF782EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCCCB3C3-508D-4C4D-9FFD-260536B4A0DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="health_policy" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="43">
   <si>
     <t>TC_01</t>
   </si>
@@ -85,9 +85,6 @@
     <t>name</t>
   </si>
   <si>
-    <t>AutoTestUNIQUE@gmail.com</t>
-  </si>
-  <si>
     <t>customize_policyheader</t>
   </si>
   <si>
@@ -100,16 +97,10 @@
     <t>5 Lakhs</t>
   </si>
   <si>
-    <t>UNIQUEphno</t>
-  </si>
-  <si>
     <t>500051</t>
   </si>
   <si>
     <t>UPTO10LAKHS</t>
-  </si>
-  <si>
-    <t>UNIQUEfullname</t>
   </si>
   <si>
     <t>IN1YR</t>
@@ -136,9 +127,6 @@
     <t>life_insurance_type</t>
   </si>
   <si>
-    <t>Yes</t>
-  </si>
-  <si>
     <t>assured_amount</t>
   </si>
   <si>
@@ -162,12 +150,18 @@
   <si>
     <t>RANDOM_EMAILID</t>
   </si>
+  <si>
+    <t>Self</t>
+  </si>
+  <si>
+    <t>Self-30 years</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -291,12 +285,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FF4EC9B0"/>
-      <name val="Consolas"/>
-      <family val="3"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9CDCFE"/>
       <name val="Consolas"/>
       <family val="3"/>
     </font>
@@ -427,7 +415,7 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="14" fillId="9" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -443,10 +431,7 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -850,33 +835,33 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:ALH40"/>
   <sheetViews>
-    <sheetView topLeftCell="H1" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView tabSelected="1" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="11" style="1" customWidth="1"/>
-    <col min="2" max="2" width="16.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="59.140625" style="5" customWidth="1"/>
-    <col min="4" max="4" width="38.140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="16.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="59.109375" style="5" customWidth="1"/>
+    <col min="4" max="4" width="38.109375" style="1" customWidth="1"/>
     <col min="5" max="5" width="17" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="27.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="27.85546875" style="1" customWidth="1"/>
-    <col min="8" max="8" width="28.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.42578125" style="1"/>
-    <col min="10" max="10" width="26.7109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="26.7109375" style="5" customWidth="1"/>
-    <col min="12" max="12" width="25.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="31.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="25.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="13.7109375" style="1" customWidth="1"/>
-    <col min="16" max="16" width="16.28515625" style="1" customWidth="1"/>
-    <col min="17" max="996" width="11.42578125" style="1"/>
-    <col min="997" max="1014" width="8.7109375" customWidth="1"/>
+    <col min="6" max="6" width="27.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="27.88671875" style="1" customWidth="1"/>
+    <col min="8" max="8" width="28.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.44140625" style="1"/>
+    <col min="10" max="10" width="26.6640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="26.6640625" style="5" customWidth="1"/>
+    <col min="12" max="12" width="25.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="31.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="25.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13.6640625" style="1" customWidth="1"/>
+    <col min="16" max="16" width="16.33203125" style="1" customWidth="1"/>
+    <col min="17" max="996" width="11.44140625" style="1"/>
+    <col min="997" max="1014" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:996" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:996" s="2" customFormat="1" ht="16.8" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>1</v>
       </c>
@@ -917,13 +902,13 @@
         <v>10</v>
       </c>
       <c r="N1" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="O1" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:996" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:996" s="3" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
@@ -934,1041 +919,85 @@
         <v>6</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>8</v>
+        <v>41</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>28</v>
-      </c>
+        <v>42</v>
+      </c>
+      <c r="G2" s="1"/>
       <c r="H2" s="3" t="s">
         <v>7</v>
       </c>
       <c r="I2" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="M2" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="N2" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="O2" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:996" s="3" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A3" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="G3" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="J2" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="L2" s="9" t="s">
+      <c r="H3" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="J3" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="M2" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="N2" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="O2" s="3" t="s">
-        <v>23</v>
+      <c r="K3" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="L3" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="M3" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="N3" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="O3" s="3" t="s">
+        <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:996" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="1"/>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
-      <c r="I3" s="1"/>
-      <c r="J3" s="3"/>
-      <c r="K3" s="1"/>
-      <c r="L3" s="1"/>
-      <c r="M3" s="1"/>
-      <c r="N3" s="1"/>
-      <c r="O3" s="1"/>
-      <c r="P3" s="1"/>
-      <c r="Q3" s="1"/>
-      <c r="R3" s="1"/>
-      <c r="S3" s="1"/>
-      <c r="T3" s="1"/>
-      <c r="U3" s="1"/>
-      <c r="V3" s="1"/>
-      <c r="W3" s="1"/>
-      <c r="X3" s="1"/>
-      <c r="Y3" s="1"/>
-      <c r="Z3" s="1"/>
-      <c r="AA3" s="1"/>
-      <c r="AB3" s="1"/>
-      <c r="AC3" s="1"/>
-      <c r="AD3" s="1"/>
-      <c r="AE3" s="1"/>
-      <c r="AF3" s="1"/>
-      <c r="AG3" s="1"/>
-      <c r="AH3" s="1"/>
-      <c r="AI3" s="1"/>
-      <c r="AJ3" s="1"/>
-      <c r="AK3" s="1"/>
-      <c r="AL3" s="1"/>
-      <c r="AM3" s="1"/>
-      <c r="AN3" s="1"/>
-      <c r="AO3" s="1"/>
-      <c r="AP3" s="1"/>
-      <c r="AQ3" s="1"/>
-      <c r="AR3" s="1"/>
-      <c r="AS3" s="1"/>
-      <c r="AT3" s="1"/>
-      <c r="AU3" s="1"/>
-      <c r="AV3" s="1"/>
-      <c r="AW3" s="1"/>
-      <c r="AX3" s="1"/>
-      <c r="AY3" s="1"/>
-      <c r="AZ3" s="1"/>
-      <c r="BA3" s="1"/>
-      <c r="BB3" s="1"/>
-      <c r="BC3" s="1"/>
-      <c r="BD3" s="1"/>
-      <c r="BE3" s="1"/>
-      <c r="BF3" s="1"/>
-      <c r="BG3" s="1"/>
-      <c r="BH3" s="1"/>
-      <c r="BI3" s="1"/>
-      <c r="BJ3" s="1"/>
-      <c r="BK3" s="1"/>
-      <c r="BL3" s="1"/>
-      <c r="BM3" s="1"/>
-      <c r="BN3" s="1"/>
-      <c r="BO3" s="1"/>
-      <c r="BP3" s="1"/>
-      <c r="BQ3" s="1"/>
-      <c r="BR3" s="1"/>
-      <c r="BS3" s="1"/>
-      <c r="BT3" s="1"/>
-      <c r="BU3" s="1"/>
-      <c r="BV3" s="1"/>
-      <c r="BW3" s="1"/>
-      <c r="BX3" s="1"/>
-      <c r="BY3" s="1"/>
-      <c r="BZ3" s="1"/>
-      <c r="CA3" s="1"/>
-      <c r="CB3" s="1"/>
-      <c r="CC3" s="1"/>
-      <c r="CD3" s="1"/>
-      <c r="CE3" s="1"/>
-      <c r="CF3" s="1"/>
-      <c r="CG3" s="1"/>
-      <c r="CH3" s="1"/>
-      <c r="CI3" s="1"/>
-      <c r="CJ3" s="1"/>
-      <c r="CK3" s="1"/>
-      <c r="CL3" s="1"/>
-      <c r="CM3" s="1"/>
-      <c r="CN3" s="1"/>
-      <c r="CO3" s="1"/>
-      <c r="CP3" s="1"/>
-      <c r="CQ3" s="1"/>
-      <c r="CR3" s="1"/>
-      <c r="CS3" s="1"/>
-      <c r="CT3" s="1"/>
-      <c r="CU3" s="1"/>
-      <c r="CV3" s="1"/>
-      <c r="CW3" s="1"/>
-      <c r="CX3" s="1"/>
-      <c r="CY3" s="1"/>
-      <c r="CZ3" s="1"/>
-      <c r="DA3" s="1"/>
-      <c r="DB3" s="1"/>
-      <c r="DC3" s="1"/>
-      <c r="DD3" s="1"/>
-      <c r="DE3" s="1"/>
-      <c r="DF3" s="1"/>
-      <c r="DG3" s="1"/>
-      <c r="DH3" s="1"/>
-      <c r="DI3" s="1"/>
-      <c r="DJ3" s="1"/>
-      <c r="DK3" s="1"/>
-      <c r="DL3" s="1"/>
-      <c r="DM3" s="1"/>
-      <c r="DN3" s="1"/>
-      <c r="DO3" s="1"/>
-      <c r="DP3" s="1"/>
-      <c r="DQ3" s="1"/>
-      <c r="DR3" s="1"/>
-      <c r="DS3" s="1"/>
-      <c r="DT3" s="1"/>
-      <c r="DU3" s="1"/>
-      <c r="DV3" s="1"/>
-      <c r="DW3" s="1"/>
-      <c r="DX3" s="1"/>
-      <c r="DY3" s="1"/>
-      <c r="DZ3" s="1"/>
-      <c r="EA3" s="1"/>
-      <c r="EB3" s="1"/>
-      <c r="EC3" s="1"/>
-      <c r="ED3" s="1"/>
-      <c r="EE3" s="1"/>
-      <c r="EF3" s="1"/>
-      <c r="EG3" s="1"/>
-      <c r="EH3" s="1"/>
-      <c r="EI3" s="1"/>
-      <c r="EJ3" s="1"/>
-      <c r="EK3" s="1"/>
-      <c r="EL3" s="1"/>
-      <c r="EM3" s="1"/>
-      <c r="EN3" s="1"/>
-      <c r="EO3" s="1"/>
-      <c r="EP3" s="1"/>
-      <c r="EQ3" s="1"/>
-      <c r="ER3" s="1"/>
-      <c r="ES3" s="1"/>
-      <c r="ET3" s="1"/>
-      <c r="EU3" s="1"/>
-      <c r="EV3" s="1"/>
-      <c r="EW3" s="1"/>
-      <c r="EX3" s="1"/>
-      <c r="EY3" s="1"/>
-      <c r="EZ3" s="1"/>
-      <c r="FA3" s="1"/>
-      <c r="FB3" s="1"/>
-      <c r="FC3" s="1"/>
-      <c r="FD3" s="1"/>
-      <c r="FE3" s="1"/>
-      <c r="FF3" s="1"/>
-      <c r="FG3" s="1"/>
-      <c r="FH3" s="1"/>
-      <c r="FI3" s="1"/>
-      <c r="FJ3" s="1"/>
-      <c r="FK3" s="1"/>
-      <c r="FL3" s="1"/>
-      <c r="FM3" s="1"/>
-      <c r="FN3" s="1"/>
-      <c r="FO3" s="1"/>
-      <c r="FP3" s="1"/>
-      <c r="FQ3" s="1"/>
-      <c r="FR3" s="1"/>
-      <c r="FS3" s="1"/>
-      <c r="FT3" s="1"/>
-      <c r="FU3" s="1"/>
-      <c r="FV3" s="1"/>
-      <c r="FW3" s="1"/>
-      <c r="FX3" s="1"/>
-      <c r="FY3" s="1"/>
-      <c r="FZ3" s="1"/>
-      <c r="GA3" s="1"/>
-      <c r="GB3" s="1"/>
-      <c r="GC3" s="1"/>
-      <c r="GD3" s="1"/>
-      <c r="GE3" s="1"/>
-      <c r="GF3" s="1"/>
-      <c r="GG3" s="1"/>
-      <c r="GH3" s="1"/>
-      <c r="GI3" s="1"/>
-      <c r="GJ3" s="1"/>
-      <c r="GK3" s="1"/>
-      <c r="GL3" s="1"/>
-      <c r="GM3" s="1"/>
-      <c r="GN3" s="1"/>
-      <c r="GO3" s="1"/>
-      <c r="GP3" s="1"/>
-      <c r="GQ3" s="1"/>
-      <c r="GR3" s="1"/>
-      <c r="GS3" s="1"/>
-      <c r="GT3" s="1"/>
-      <c r="GU3" s="1"/>
-      <c r="GV3" s="1"/>
-      <c r="GW3" s="1"/>
-      <c r="GX3" s="1"/>
-      <c r="GY3" s="1"/>
-      <c r="GZ3" s="1"/>
-      <c r="HA3" s="1"/>
-      <c r="HB3" s="1"/>
-      <c r="HC3" s="1"/>
-      <c r="HD3" s="1"/>
-      <c r="HE3" s="1"/>
-      <c r="HF3" s="1"/>
-      <c r="HG3" s="1"/>
-      <c r="HH3" s="1"/>
-      <c r="HI3" s="1"/>
-      <c r="HJ3" s="1"/>
-      <c r="HK3" s="1"/>
-      <c r="HL3" s="1"/>
-      <c r="HM3" s="1"/>
-      <c r="HN3" s="1"/>
-      <c r="HO3" s="1"/>
-      <c r="HP3" s="1"/>
-      <c r="HQ3" s="1"/>
-      <c r="HR3" s="1"/>
-      <c r="HS3" s="1"/>
-      <c r="HT3" s="1"/>
-      <c r="HU3" s="1"/>
-      <c r="HV3" s="1"/>
-      <c r="HW3" s="1"/>
-      <c r="HX3" s="1"/>
-      <c r="HY3" s="1"/>
-      <c r="HZ3" s="1"/>
-      <c r="IA3" s="1"/>
-      <c r="IB3" s="1"/>
-      <c r="IC3" s="1"/>
-      <c r="ID3" s="1"/>
-      <c r="IE3" s="1"/>
-      <c r="IF3" s="1"/>
-      <c r="IG3" s="1"/>
-      <c r="IH3" s="1"/>
-      <c r="II3" s="1"/>
-      <c r="IJ3" s="1"/>
-      <c r="IK3" s="1"/>
-      <c r="IL3" s="1"/>
-      <c r="IM3" s="1"/>
-      <c r="IN3" s="1"/>
-      <c r="IO3" s="1"/>
-      <c r="IP3" s="1"/>
-      <c r="IQ3" s="1"/>
-      <c r="IR3" s="1"/>
-      <c r="IS3" s="1"/>
-      <c r="IT3" s="1"/>
-      <c r="IU3" s="1"/>
-      <c r="IV3" s="1"/>
-      <c r="IW3" s="1"/>
-      <c r="IX3" s="1"/>
-      <c r="IY3" s="1"/>
-      <c r="IZ3" s="1"/>
-      <c r="JA3" s="1"/>
-      <c r="JB3" s="1"/>
-      <c r="JC3" s="1"/>
-      <c r="JD3" s="1"/>
-      <c r="JE3" s="1"/>
-      <c r="JF3" s="1"/>
-      <c r="JG3" s="1"/>
-      <c r="JH3" s="1"/>
-      <c r="JI3" s="1"/>
-      <c r="JJ3" s="1"/>
-      <c r="JK3" s="1"/>
-      <c r="JL3" s="1"/>
-      <c r="JM3" s="1"/>
-      <c r="JN3" s="1"/>
-      <c r="JO3" s="1"/>
-      <c r="JP3" s="1"/>
-      <c r="JQ3" s="1"/>
-      <c r="JR3" s="1"/>
-      <c r="JS3" s="1"/>
-      <c r="JT3" s="1"/>
-      <c r="JU3" s="1"/>
-      <c r="JV3" s="1"/>
-      <c r="JW3" s="1"/>
-      <c r="JX3" s="1"/>
-      <c r="JY3" s="1"/>
-      <c r="JZ3" s="1"/>
-      <c r="KA3" s="1"/>
-      <c r="KB3" s="1"/>
-      <c r="KC3" s="1"/>
-      <c r="KD3" s="1"/>
-      <c r="KE3" s="1"/>
-      <c r="KF3" s="1"/>
-      <c r="KG3" s="1"/>
-      <c r="KH3" s="1"/>
-      <c r="KI3" s="1"/>
-      <c r="KJ3" s="1"/>
-      <c r="KK3" s="1"/>
-      <c r="KL3" s="1"/>
-      <c r="KM3" s="1"/>
-      <c r="KN3" s="1"/>
-      <c r="KO3" s="1"/>
-      <c r="KP3" s="1"/>
-      <c r="KQ3" s="1"/>
-      <c r="KR3" s="1"/>
-      <c r="KS3" s="1"/>
-      <c r="KT3" s="1"/>
-      <c r="KU3" s="1"/>
-      <c r="KV3" s="1"/>
-      <c r="KW3" s="1"/>
-      <c r="KX3" s="1"/>
-      <c r="KY3" s="1"/>
-      <c r="KZ3" s="1"/>
-      <c r="LA3" s="1"/>
-      <c r="LB3" s="1"/>
-      <c r="LC3" s="1"/>
-      <c r="LD3" s="1"/>
-      <c r="LE3" s="1"/>
-      <c r="LF3" s="1"/>
-      <c r="LG3" s="1"/>
-      <c r="LH3" s="1"/>
-      <c r="LI3" s="1"/>
-      <c r="LJ3" s="1"/>
-      <c r="LK3" s="1"/>
-      <c r="LL3" s="1"/>
-      <c r="LM3" s="1"/>
-      <c r="LN3" s="1"/>
-      <c r="LO3" s="1"/>
-      <c r="LP3" s="1"/>
-      <c r="LQ3" s="1"/>
-      <c r="LR3" s="1"/>
-      <c r="LS3" s="1"/>
-      <c r="LT3" s="1"/>
-      <c r="LU3" s="1"/>
-      <c r="LV3" s="1"/>
-      <c r="LW3" s="1"/>
-      <c r="LX3" s="1"/>
-      <c r="LY3" s="1"/>
-      <c r="LZ3" s="1"/>
-      <c r="MA3" s="1"/>
-      <c r="MB3" s="1"/>
-      <c r="MC3" s="1"/>
-      <c r="MD3" s="1"/>
-      <c r="ME3" s="1"/>
-      <c r="MF3" s="1"/>
-      <c r="MG3" s="1"/>
-      <c r="MH3" s="1"/>
-      <c r="MI3" s="1"/>
-      <c r="MJ3" s="1"/>
-      <c r="MK3" s="1"/>
-      <c r="ML3" s="1"/>
-      <c r="MM3" s="1"/>
-      <c r="MN3" s="1"/>
-      <c r="MO3" s="1"/>
-      <c r="MP3" s="1"/>
-      <c r="MQ3" s="1"/>
-      <c r="MR3" s="1"/>
-      <c r="MS3" s="1"/>
-      <c r="MT3" s="1"/>
-      <c r="MU3" s="1"/>
-      <c r="MV3" s="1"/>
-      <c r="MW3" s="1"/>
-      <c r="MX3" s="1"/>
-      <c r="MY3" s="1"/>
-      <c r="MZ3" s="1"/>
-      <c r="NA3" s="1"/>
-      <c r="NB3" s="1"/>
-      <c r="NC3" s="1"/>
-      <c r="ND3" s="1"/>
-      <c r="NE3" s="1"/>
-      <c r="NF3" s="1"/>
-      <c r="NG3" s="1"/>
-      <c r="NH3" s="1"/>
-      <c r="NI3" s="1"/>
-      <c r="NJ3" s="1"/>
-      <c r="NK3" s="1"/>
-      <c r="NL3" s="1"/>
-      <c r="NM3" s="1"/>
-      <c r="NN3" s="1"/>
-      <c r="NO3" s="1"/>
-      <c r="NP3" s="1"/>
-      <c r="NQ3" s="1"/>
-      <c r="NR3" s="1"/>
-      <c r="NS3" s="1"/>
-      <c r="NT3" s="1"/>
-      <c r="NU3" s="1"/>
-      <c r="NV3" s="1"/>
-      <c r="NW3" s="1"/>
-      <c r="NX3" s="1"/>
-      <c r="NY3" s="1"/>
-      <c r="NZ3" s="1"/>
-      <c r="OA3" s="1"/>
-      <c r="OB3" s="1"/>
-      <c r="OC3" s="1"/>
-      <c r="OD3" s="1"/>
-      <c r="OE3" s="1"/>
-      <c r="OF3" s="1"/>
-      <c r="OG3" s="1"/>
-      <c r="OH3" s="1"/>
-      <c r="OI3" s="1"/>
-      <c r="OJ3" s="1"/>
-      <c r="OK3" s="1"/>
-      <c r="OL3" s="1"/>
-      <c r="OM3" s="1"/>
-      <c r="ON3" s="1"/>
-      <c r="OO3" s="1"/>
-      <c r="OP3" s="1"/>
-      <c r="OQ3" s="1"/>
-      <c r="OR3" s="1"/>
-      <c r="OS3" s="1"/>
-      <c r="OT3" s="1"/>
-      <c r="OU3" s="1"/>
-      <c r="OV3" s="1"/>
-      <c r="OW3" s="1"/>
-      <c r="OX3" s="1"/>
-      <c r="OY3" s="1"/>
-      <c r="OZ3" s="1"/>
-      <c r="PA3" s="1"/>
-      <c r="PB3" s="1"/>
-      <c r="PC3" s="1"/>
-      <c r="PD3" s="1"/>
-      <c r="PE3" s="1"/>
-      <c r="PF3" s="1"/>
-      <c r="PG3" s="1"/>
-      <c r="PH3" s="1"/>
-      <c r="PI3" s="1"/>
-      <c r="PJ3" s="1"/>
-      <c r="PK3" s="1"/>
-      <c r="PL3" s="1"/>
-      <c r="PM3" s="1"/>
-      <c r="PN3" s="1"/>
-      <c r="PO3" s="1"/>
-      <c r="PP3" s="1"/>
-      <c r="PQ3" s="1"/>
-      <c r="PR3" s="1"/>
-      <c r="PS3" s="1"/>
-      <c r="PT3" s="1"/>
-      <c r="PU3" s="1"/>
-      <c r="PV3" s="1"/>
-      <c r="PW3" s="1"/>
-      <c r="PX3" s="1"/>
-      <c r="PY3" s="1"/>
-      <c r="PZ3" s="1"/>
-      <c r="QA3" s="1"/>
-      <c r="QB3" s="1"/>
-      <c r="QC3" s="1"/>
-      <c r="QD3" s="1"/>
-      <c r="QE3" s="1"/>
-      <c r="QF3" s="1"/>
-      <c r="QG3" s="1"/>
-      <c r="QH3" s="1"/>
-      <c r="QI3" s="1"/>
-      <c r="QJ3" s="1"/>
-      <c r="QK3" s="1"/>
-      <c r="QL3" s="1"/>
-      <c r="QM3" s="1"/>
-      <c r="QN3" s="1"/>
-      <c r="QO3" s="1"/>
-      <c r="QP3" s="1"/>
-      <c r="QQ3" s="1"/>
-      <c r="QR3" s="1"/>
-      <c r="QS3" s="1"/>
-      <c r="QT3" s="1"/>
-      <c r="QU3" s="1"/>
-      <c r="QV3" s="1"/>
-      <c r="QW3" s="1"/>
-      <c r="QX3" s="1"/>
-      <c r="QY3" s="1"/>
-      <c r="QZ3" s="1"/>
-      <c r="RA3" s="1"/>
-      <c r="RB3" s="1"/>
-      <c r="RC3" s="1"/>
-      <c r="RD3" s="1"/>
-      <c r="RE3" s="1"/>
-      <c r="RF3" s="1"/>
-      <c r="RG3" s="1"/>
-      <c r="RH3" s="1"/>
-      <c r="RI3" s="1"/>
-      <c r="RJ3" s="1"/>
-      <c r="RK3" s="1"/>
-      <c r="RL3" s="1"/>
-      <c r="RM3" s="1"/>
-      <c r="RN3" s="1"/>
-      <c r="RO3" s="1"/>
-      <c r="RP3" s="1"/>
-      <c r="RQ3" s="1"/>
-      <c r="RR3" s="1"/>
-      <c r="RS3" s="1"/>
-      <c r="RT3" s="1"/>
-      <c r="RU3" s="1"/>
-      <c r="RV3" s="1"/>
-      <c r="RW3" s="1"/>
-      <c r="RX3" s="1"/>
-      <c r="RY3" s="1"/>
-      <c r="RZ3" s="1"/>
-      <c r="SA3" s="1"/>
-      <c r="SB3" s="1"/>
-      <c r="SC3" s="1"/>
-      <c r="SD3" s="1"/>
-      <c r="SE3" s="1"/>
-      <c r="SF3" s="1"/>
-      <c r="SG3" s="1"/>
-      <c r="SH3" s="1"/>
-      <c r="SI3" s="1"/>
-      <c r="SJ3" s="1"/>
-      <c r="SK3" s="1"/>
-      <c r="SL3" s="1"/>
-      <c r="SM3" s="1"/>
-      <c r="SN3" s="1"/>
-      <c r="SO3" s="1"/>
-      <c r="SP3" s="1"/>
-      <c r="SQ3" s="1"/>
-      <c r="SR3" s="1"/>
-      <c r="SS3" s="1"/>
-      <c r="ST3" s="1"/>
-      <c r="SU3" s="1"/>
-      <c r="SV3" s="1"/>
-      <c r="SW3" s="1"/>
-      <c r="SX3" s="1"/>
-      <c r="SY3" s="1"/>
-      <c r="SZ3" s="1"/>
-      <c r="TA3" s="1"/>
-      <c r="TB3" s="1"/>
-      <c r="TC3" s="1"/>
-      <c r="TD3" s="1"/>
-      <c r="TE3" s="1"/>
-      <c r="TF3" s="1"/>
-      <c r="TG3" s="1"/>
-      <c r="TH3" s="1"/>
-      <c r="TI3" s="1"/>
-      <c r="TJ3" s="1"/>
-      <c r="TK3" s="1"/>
-      <c r="TL3" s="1"/>
-      <c r="TM3" s="1"/>
-      <c r="TN3" s="1"/>
-      <c r="TO3" s="1"/>
-      <c r="TP3" s="1"/>
-      <c r="TQ3" s="1"/>
-      <c r="TR3" s="1"/>
-      <c r="TS3" s="1"/>
-      <c r="TT3" s="1"/>
-      <c r="TU3" s="1"/>
-      <c r="TV3" s="1"/>
-      <c r="TW3" s="1"/>
-      <c r="TX3" s="1"/>
-      <c r="TY3" s="1"/>
-      <c r="TZ3" s="1"/>
-      <c r="UA3" s="1"/>
-      <c r="UB3" s="1"/>
-      <c r="UC3" s="1"/>
-      <c r="UD3" s="1"/>
-      <c r="UE3" s="1"/>
-      <c r="UF3" s="1"/>
-      <c r="UG3" s="1"/>
-      <c r="UH3" s="1"/>
-      <c r="UI3" s="1"/>
-      <c r="UJ3" s="1"/>
-      <c r="UK3" s="1"/>
-      <c r="UL3" s="1"/>
-      <c r="UM3" s="1"/>
-      <c r="UN3" s="1"/>
-      <c r="UO3" s="1"/>
-      <c r="UP3" s="1"/>
-      <c r="UQ3" s="1"/>
-      <c r="UR3" s="1"/>
-      <c r="US3" s="1"/>
-      <c r="UT3" s="1"/>
-      <c r="UU3" s="1"/>
-      <c r="UV3" s="1"/>
-      <c r="UW3" s="1"/>
-      <c r="UX3" s="1"/>
-      <c r="UY3" s="1"/>
-      <c r="UZ3" s="1"/>
-      <c r="VA3" s="1"/>
-      <c r="VB3" s="1"/>
-      <c r="VC3" s="1"/>
-      <c r="VD3" s="1"/>
-      <c r="VE3" s="1"/>
-      <c r="VF3" s="1"/>
-      <c r="VG3" s="1"/>
-      <c r="VH3" s="1"/>
-      <c r="VI3" s="1"/>
-      <c r="VJ3" s="1"/>
-      <c r="VK3" s="1"/>
-      <c r="VL3" s="1"/>
-      <c r="VM3" s="1"/>
-      <c r="VN3" s="1"/>
-      <c r="VO3" s="1"/>
-      <c r="VP3" s="1"/>
-      <c r="VQ3" s="1"/>
-      <c r="VR3" s="1"/>
-      <c r="VS3" s="1"/>
-      <c r="VT3" s="1"/>
-      <c r="VU3" s="1"/>
-      <c r="VV3" s="1"/>
-      <c r="VW3" s="1"/>
-      <c r="VX3" s="1"/>
-      <c r="VY3" s="1"/>
-      <c r="VZ3" s="1"/>
-      <c r="WA3" s="1"/>
-      <c r="WB3" s="1"/>
-      <c r="WC3" s="1"/>
-      <c r="WD3" s="1"/>
-      <c r="WE3" s="1"/>
-      <c r="WF3" s="1"/>
-      <c r="WG3" s="1"/>
-      <c r="WH3" s="1"/>
-      <c r="WI3" s="1"/>
-      <c r="WJ3" s="1"/>
-      <c r="WK3" s="1"/>
-      <c r="WL3" s="1"/>
-      <c r="WM3" s="1"/>
-      <c r="WN3" s="1"/>
-      <c r="WO3" s="1"/>
-      <c r="WP3" s="1"/>
-      <c r="WQ3" s="1"/>
-      <c r="WR3" s="1"/>
-      <c r="WS3" s="1"/>
-      <c r="WT3" s="1"/>
-      <c r="WU3" s="1"/>
-      <c r="WV3" s="1"/>
-      <c r="WW3" s="1"/>
-      <c r="WX3" s="1"/>
-      <c r="WY3" s="1"/>
-      <c r="WZ3" s="1"/>
-      <c r="XA3" s="1"/>
-      <c r="XB3" s="1"/>
-      <c r="XC3" s="1"/>
-      <c r="XD3" s="1"/>
-      <c r="XE3" s="1"/>
-      <c r="XF3" s="1"/>
-      <c r="XG3" s="1"/>
-      <c r="XH3" s="1"/>
-      <c r="XI3" s="1"/>
-      <c r="XJ3" s="1"/>
-      <c r="XK3" s="1"/>
-      <c r="XL3" s="1"/>
-      <c r="XM3" s="1"/>
-      <c r="XN3" s="1"/>
-      <c r="XO3" s="1"/>
-      <c r="XP3" s="1"/>
-      <c r="XQ3" s="1"/>
-      <c r="XR3" s="1"/>
-      <c r="XS3" s="1"/>
-      <c r="XT3" s="1"/>
-      <c r="XU3" s="1"/>
-      <c r="XV3" s="1"/>
-      <c r="XW3" s="1"/>
-      <c r="XX3" s="1"/>
-      <c r="XY3" s="1"/>
-      <c r="XZ3" s="1"/>
-      <c r="YA3" s="1"/>
-      <c r="YB3" s="1"/>
-      <c r="YC3" s="1"/>
-      <c r="YD3" s="1"/>
-      <c r="YE3" s="1"/>
-      <c r="YF3" s="1"/>
-      <c r="YG3" s="1"/>
-      <c r="YH3" s="1"/>
-      <c r="YI3" s="1"/>
-      <c r="YJ3" s="1"/>
-      <c r="YK3" s="1"/>
-      <c r="YL3" s="1"/>
-      <c r="YM3" s="1"/>
-      <c r="YN3" s="1"/>
-      <c r="YO3" s="1"/>
-      <c r="YP3" s="1"/>
-      <c r="YQ3" s="1"/>
-      <c r="YR3" s="1"/>
-      <c r="YS3" s="1"/>
-      <c r="YT3" s="1"/>
-      <c r="YU3" s="1"/>
-      <c r="YV3" s="1"/>
-      <c r="YW3" s="1"/>
-      <c r="YX3" s="1"/>
-      <c r="YY3" s="1"/>
-      <c r="YZ3" s="1"/>
-      <c r="ZA3" s="1"/>
-      <c r="ZB3" s="1"/>
-      <c r="ZC3" s="1"/>
-      <c r="ZD3" s="1"/>
-      <c r="ZE3" s="1"/>
-      <c r="ZF3" s="1"/>
-      <c r="ZG3" s="1"/>
-      <c r="ZH3" s="1"/>
-      <c r="ZI3" s="1"/>
-      <c r="ZJ3" s="1"/>
-      <c r="ZK3" s="1"/>
-      <c r="ZL3" s="1"/>
-      <c r="ZM3" s="1"/>
-      <c r="ZN3" s="1"/>
-      <c r="ZO3" s="1"/>
-      <c r="ZP3" s="1"/>
-      <c r="ZQ3" s="1"/>
-      <c r="ZR3" s="1"/>
-      <c r="ZS3" s="1"/>
-      <c r="ZT3" s="1"/>
-      <c r="ZU3" s="1"/>
-      <c r="ZV3" s="1"/>
-      <c r="ZW3" s="1"/>
-      <c r="ZX3" s="1"/>
-      <c r="ZY3" s="1"/>
-      <c r="ZZ3" s="1"/>
-      <c r="AAA3" s="1"/>
-      <c r="AAB3" s="1"/>
-      <c r="AAC3" s="1"/>
-      <c r="AAD3" s="1"/>
-      <c r="AAE3" s="1"/>
-      <c r="AAF3" s="1"/>
-      <c r="AAG3" s="1"/>
-      <c r="AAH3" s="1"/>
-      <c r="AAI3" s="1"/>
-      <c r="AAJ3" s="1"/>
-      <c r="AAK3" s="1"/>
-      <c r="AAL3" s="1"/>
-      <c r="AAM3" s="1"/>
-      <c r="AAN3" s="1"/>
-      <c r="AAO3" s="1"/>
-      <c r="AAP3" s="1"/>
-      <c r="AAQ3" s="1"/>
-      <c r="AAR3" s="1"/>
-      <c r="AAS3" s="1"/>
-      <c r="AAT3" s="1"/>
-      <c r="AAU3" s="1"/>
-      <c r="AAV3" s="1"/>
-      <c r="AAW3" s="1"/>
-      <c r="AAX3" s="1"/>
-      <c r="AAY3" s="1"/>
-      <c r="AAZ3" s="1"/>
-      <c r="ABA3" s="1"/>
-      <c r="ABB3" s="1"/>
-      <c r="ABC3" s="1"/>
-      <c r="ABD3" s="1"/>
-      <c r="ABE3" s="1"/>
-      <c r="ABF3" s="1"/>
-      <c r="ABG3" s="1"/>
-      <c r="ABH3" s="1"/>
-      <c r="ABI3" s="1"/>
-      <c r="ABJ3" s="1"/>
-      <c r="ABK3" s="1"/>
-      <c r="ABL3" s="1"/>
-      <c r="ABM3" s="1"/>
-      <c r="ABN3" s="1"/>
-      <c r="ABO3" s="1"/>
-      <c r="ABP3" s="1"/>
-      <c r="ABQ3" s="1"/>
-      <c r="ABR3" s="1"/>
-      <c r="ABS3" s="1"/>
-      <c r="ABT3" s="1"/>
-      <c r="ABU3" s="1"/>
-      <c r="ABV3" s="1"/>
-      <c r="ABW3" s="1"/>
-      <c r="ABX3" s="1"/>
-      <c r="ABY3" s="1"/>
-      <c r="ABZ3" s="1"/>
-      <c r="ACA3" s="1"/>
-      <c r="ACB3" s="1"/>
-      <c r="ACC3" s="1"/>
-      <c r="ACD3" s="1"/>
-      <c r="ACE3" s="1"/>
-      <c r="ACF3" s="1"/>
-      <c r="ACG3" s="1"/>
-      <c r="ACH3" s="1"/>
-      <c r="ACI3" s="1"/>
-      <c r="ACJ3" s="1"/>
-      <c r="ACK3" s="1"/>
-      <c r="ACL3" s="1"/>
-      <c r="ACM3" s="1"/>
-      <c r="ACN3" s="1"/>
-      <c r="ACO3" s="1"/>
-      <c r="ACP3" s="1"/>
-      <c r="ACQ3" s="1"/>
-      <c r="ACR3" s="1"/>
-      <c r="ACS3" s="1"/>
-      <c r="ACT3" s="1"/>
-      <c r="ACU3" s="1"/>
-      <c r="ACV3" s="1"/>
-      <c r="ACW3" s="1"/>
-      <c r="ACX3" s="1"/>
-      <c r="ACY3" s="1"/>
-      <c r="ACZ3" s="1"/>
-      <c r="ADA3" s="1"/>
-      <c r="ADB3" s="1"/>
-      <c r="ADC3" s="1"/>
-      <c r="ADD3" s="1"/>
-      <c r="ADE3" s="1"/>
-      <c r="ADF3" s="1"/>
-      <c r="ADG3" s="1"/>
-      <c r="ADH3" s="1"/>
-      <c r="ADI3" s="1"/>
-      <c r="ADJ3" s="1"/>
-      <c r="ADK3" s="1"/>
-      <c r="ADL3" s="1"/>
-      <c r="ADM3" s="1"/>
-      <c r="ADN3" s="1"/>
-      <c r="ADO3" s="1"/>
-      <c r="ADP3" s="1"/>
-      <c r="ADQ3" s="1"/>
-      <c r="ADR3" s="1"/>
-      <c r="ADS3" s="1"/>
-      <c r="ADT3" s="1"/>
-      <c r="ADU3" s="1"/>
-      <c r="ADV3" s="1"/>
-      <c r="ADW3" s="1"/>
-      <c r="ADX3" s="1"/>
-      <c r="ADY3" s="1"/>
-      <c r="ADZ3" s="1"/>
-      <c r="AEA3" s="1"/>
-      <c r="AEB3" s="1"/>
-      <c r="AEC3" s="1"/>
-      <c r="AED3" s="1"/>
-      <c r="AEE3" s="1"/>
-      <c r="AEF3" s="1"/>
-      <c r="AEG3" s="1"/>
-      <c r="AEH3" s="1"/>
-      <c r="AEI3" s="1"/>
-      <c r="AEJ3" s="1"/>
-      <c r="AEK3" s="1"/>
-      <c r="AEL3" s="1"/>
-      <c r="AEM3" s="1"/>
-      <c r="AEN3" s="1"/>
-      <c r="AEO3" s="1"/>
-      <c r="AEP3" s="1"/>
-      <c r="AEQ3" s="1"/>
-      <c r="AER3" s="1"/>
-      <c r="AES3" s="1"/>
-      <c r="AET3" s="1"/>
-      <c r="AEU3" s="1"/>
-      <c r="AEV3" s="1"/>
-      <c r="AEW3" s="1"/>
-      <c r="AEX3" s="1"/>
-      <c r="AEY3" s="1"/>
-      <c r="AEZ3" s="1"/>
-      <c r="AFA3" s="1"/>
-      <c r="AFB3" s="1"/>
-      <c r="AFC3" s="1"/>
-      <c r="AFD3" s="1"/>
-      <c r="AFE3" s="1"/>
-      <c r="AFF3" s="1"/>
-      <c r="AFG3" s="1"/>
-      <c r="AFH3" s="1"/>
-      <c r="AFI3" s="1"/>
-      <c r="AFJ3" s="1"/>
-      <c r="AFK3" s="1"/>
-      <c r="AFL3" s="1"/>
-      <c r="AFM3" s="1"/>
-      <c r="AFN3" s="1"/>
-      <c r="AFO3" s="1"/>
-      <c r="AFP3" s="1"/>
-      <c r="AFQ3" s="1"/>
-      <c r="AFR3" s="1"/>
-      <c r="AFS3" s="1"/>
-      <c r="AFT3" s="1"/>
-      <c r="AFU3" s="1"/>
-      <c r="AFV3" s="1"/>
-      <c r="AFW3" s="1"/>
-      <c r="AFX3" s="1"/>
-      <c r="AFY3" s="1"/>
-      <c r="AFZ3" s="1"/>
-      <c r="AGA3" s="1"/>
-      <c r="AGB3" s="1"/>
-      <c r="AGC3" s="1"/>
-      <c r="AGD3" s="1"/>
-      <c r="AGE3" s="1"/>
-      <c r="AGF3" s="1"/>
-      <c r="AGG3" s="1"/>
-      <c r="AGH3" s="1"/>
-      <c r="AGI3" s="1"/>
-      <c r="AGJ3" s="1"/>
-      <c r="AGK3" s="1"/>
-      <c r="AGL3" s="1"/>
-      <c r="AGM3" s="1"/>
-      <c r="AGN3" s="1"/>
-      <c r="AGO3" s="1"/>
-      <c r="AGP3" s="1"/>
-      <c r="AGQ3" s="1"/>
-      <c r="AGR3" s="1"/>
-      <c r="AGS3" s="1"/>
-      <c r="AGT3" s="1"/>
-      <c r="AGU3" s="1"/>
-      <c r="AGV3" s="1"/>
-      <c r="AGW3" s="1"/>
-      <c r="AGX3" s="1"/>
-      <c r="AGY3" s="1"/>
-      <c r="AGZ3" s="1"/>
-      <c r="AHA3" s="1"/>
-      <c r="AHB3" s="1"/>
-      <c r="AHC3" s="1"/>
-      <c r="AHD3" s="1"/>
-      <c r="AHE3" s="1"/>
-      <c r="AHF3" s="1"/>
-      <c r="AHG3" s="1"/>
-      <c r="AHH3" s="1"/>
-      <c r="AHI3" s="1"/>
-      <c r="AHJ3" s="1"/>
-      <c r="AHK3" s="1"/>
-      <c r="AHL3" s="1"/>
-      <c r="AHM3" s="1"/>
-      <c r="AHN3" s="1"/>
-      <c r="AHO3" s="1"/>
-      <c r="AHP3" s="1"/>
-      <c r="AHQ3" s="1"/>
-      <c r="AHR3" s="1"/>
-      <c r="AHS3" s="1"/>
-      <c r="AHT3" s="1"/>
-      <c r="AHU3" s="1"/>
-      <c r="AHV3" s="1"/>
-      <c r="AHW3" s="1"/>
-      <c r="AHX3" s="1"/>
-      <c r="AHY3" s="1"/>
-      <c r="AHZ3" s="1"/>
-      <c r="AIA3" s="1"/>
-      <c r="AIB3" s="1"/>
-      <c r="AIC3" s="1"/>
-      <c r="AID3" s="1"/>
-      <c r="AIE3" s="1"/>
-      <c r="AIF3" s="1"/>
-      <c r="AIG3" s="1"/>
-      <c r="AIH3" s="1"/>
-      <c r="AII3" s="1"/>
-      <c r="AIJ3" s="1"/>
-      <c r="AIK3" s="1"/>
-      <c r="AIL3" s="1"/>
-      <c r="AIM3" s="1"/>
-      <c r="AIN3" s="1"/>
-      <c r="AIO3" s="1"/>
-      <c r="AIP3" s="1"/>
-      <c r="AIQ3" s="1"/>
-      <c r="AIR3" s="1"/>
-      <c r="AIS3" s="1"/>
-      <c r="AIT3" s="1"/>
-      <c r="AIU3" s="1"/>
-      <c r="AIV3" s="1"/>
-      <c r="AIW3" s="1"/>
-      <c r="AIX3" s="1"/>
-      <c r="AIY3" s="1"/>
-      <c r="AIZ3" s="1"/>
-      <c r="AJA3" s="1"/>
-      <c r="AJB3" s="1"/>
-      <c r="AJC3" s="1"/>
-      <c r="AJD3" s="1"/>
-      <c r="AJE3" s="1"/>
-      <c r="AJF3" s="1"/>
-      <c r="AJG3" s="1"/>
-      <c r="AJH3" s="1"/>
-      <c r="AJI3" s="1"/>
-      <c r="AJJ3" s="1"/>
-      <c r="AJK3" s="1"/>
-      <c r="AJL3" s="1"/>
-      <c r="AJM3" s="1"/>
-      <c r="AJN3" s="1"/>
-      <c r="AJO3" s="1"/>
-      <c r="AJP3" s="1"/>
-      <c r="AJQ3" s="1"/>
-      <c r="AJR3" s="1"/>
-      <c r="AJS3" s="1"/>
-      <c r="AJT3" s="1"/>
-      <c r="AJU3" s="1"/>
-      <c r="AJV3" s="1"/>
-      <c r="AJW3" s="1"/>
-      <c r="AJX3" s="1"/>
-      <c r="AJY3" s="1"/>
-      <c r="AJZ3" s="1"/>
-      <c r="AKA3" s="1"/>
-      <c r="AKB3" s="1"/>
-      <c r="AKC3" s="1"/>
-      <c r="AKD3" s="1"/>
-      <c r="AKE3" s="1"/>
-      <c r="AKF3" s="1"/>
-      <c r="AKG3" s="1"/>
-      <c r="AKH3" s="1"/>
-      <c r="AKI3" s="1"/>
-      <c r="AKJ3" s="1"/>
-      <c r="AKK3" s="1"/>
-      <c r="AKL3" s="1"/>
-      <c r="AKM3" s="1"/>
-      <c r="AKN3" s="1"/>
-      <c r="AKO3" s="1"/>
-      <c r="AKP3" s="1"/>
-      <c r="AKQ3" s="1"/>
-      <c r="AKR3" s="1"/>
-      <c r="AKS3" s="1"/>
-      <c r="AKT3" s="1"/>
-      <c r="AKU3" s="1"/>
-      <c r="AKV3" s="1"/>
-      <c r="AKW3" s="1"/>
-      <c r="AKX3" s="1"/>
-      <c r="AKY3" s="1"/>
-      <c r="AKZ3" s="1"/>
-      <c r="ALA3" s="1"/>
-      <c r="ALB3" s="1"/>
-      <c r="ALC3" s="1"/>
-      <c r="ALD3" s="1"/>
-      <c r="ALE3" s="1"/>
-      <c r="ALF3" s="1"/>
-      <c r="ALG3" s="1"/>
-      <c r="ALH3" s="1"/>
-    </row>
-    <row r="4" spans="1:996" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:996" s="8" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
@@ -2966,7 +1995,7 @@
       <c r="ALG4" s="1"/>
       <c r="ALH4" s="1"/>
     </row>
-    <row r="5" spans="1:996" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:996" s="8" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
@@ -3964,7 +2993,7 @@
       <c r="ALG5" s="1"/>
       <c r="ALH5" s="1"/>
     </row>
-    <row r="6" spans="1:996" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:996" s="8" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
@@ -4962,7 +3991,7 @@
       <c r="ALG6" s="1"/>
       <c r="ALH6" s="1"/>
     </row>
-    <row r="7" spans="1:996" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:996" s="8" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -5960,7 +4989,7 @@
       <c r="ALG7" s="1"/>
       <c r="ALH7" s="1"/>
     </row>
-    <row r="8" spans="1:996" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:996" s="8" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
@@ -6958,115 +5987,115 @@
       <c r="ALG8" s="1"/>
       <c r="ALH8" s="1"/>
     </row>
-    <row r="9" spans="1:996" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:996" ht="15.6" x14ac:dyDescent="0.3">
       <c r="J9" s="3"/>
       <c r="K9" s="1"/>
     </row>
-    <row r="10" spans="1:996" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:996" ht="15.6" x14ac:dyDescent="0.3">
       <c r="J10" s="3"/>
       <c r="K10" s="1"/>
     </row>
-    <row r="11" spans="1:996" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:996" ht="15.6" x14ac:dyDescent="0.3">
       <c r="J11" s="3"/>
       <c r="K11" s="1"/>
     </row>
-    <row r="12" spans="1:996" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:996" ht="15.6" x14ac:dyDescent="0.3">
       <c r="J12" s="3"/>
       <c r="K12" s="1"/>
     </row>
-    <row r="13" spans="1:996" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:996" ht="15.6" x14ac:dyDescent="0.3">
       <c r="J13" s="3"/>
       <c r="K13" s="1"/>
     </row>
-    <row r="14" spans="1:996" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:996" ht="15.6" x14ac:dyDescent="0.3">
       <c r="J14" s="3"/>
       <c r="K14" s="1"/>
     </row>
-    <row r="15" spans="1:996" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:996" ht="15.6" x14ac:dyDescent="0.3">
       <c r="J15" s="3"/>
       <c r="K15" s="1"/>
     </row>
-    <row r="16" spans="1:996" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:996" ht="15.6" x14ac:dyDescent="0.3">
       <c r="J16" s="3"/>
       <c r="K16" s="1"/>
     </row>
-    <row r="17" spans="10:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="17" spans="10:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="J17" s="3"/>
       <c r="K17" s="1"/>
     </row>
-    <row r="18" spans="10:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="18" spans="10:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="J18" s="3"/>
       <c r="K18" s="1"/>
     </row>
-    <row r="19" spans="10:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="19" spans="10:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="J19" s="3"/>
       <c r="K19" s="1"/>
     </row>
-    <row r="20" spans="10:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="20" spans="10:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="J20" s="3"/>
       <c r="K20" s="1"/>
     </row>
-    <row r="21" spans="10:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="21" spans="10:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="J21" s="3"/>
       <c r="K21" s="1"/>
     </row>
-    <row r="22" spans="10:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="22" spans="10:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="J22" s="3"/>
       <c r="K22" s="1"/>
     </row>
-    <row r="23" spans="10:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="23" spans="10:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="J23" s="3"/>
       <c r="K23" s="1"/>
     </row>
-    <row r="24" spans="10:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="10:11" x14ac:dyDescent="0.3">
       <c r="K24" s="1"/>
     </row>
-    <row r="25" spans="10:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="10:11" x14ac:dyDescent="0.3">
       <c r="K25" s="1"/>
     </row>
-    <row r="26" spans="10:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="10:11" x14ac:dyDescent="0.3">
       <c r="K26" s="1"/>
     </row>
-    <row r="27" spans="10:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="10:11" x14ac:dyDescent="0.3">
       <c r="K27" s="1"/>
     </row>
-    <row r="28" spans="10:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="10:11" x14ac:dyDescent="0.3">
       <c r="K28" s="1"/>
     </row>
-    <row r="29" spans="10:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="10:11" x14ac:dyDescent="0.3">
       <c r="K29" s="1"/>
     </row>
-    <row r="30" spans="10:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="10:11" x14ac:dyDescent="0.3">
       <c r="K30" s="1"/>
     </row>
-    <row r="31" spans="10:11" x14ac:dyDescent="0.25">
+    <row r="31" spans="10:11" x14ac:dyDescent="0.3">
       <c r="K31" s="1"/>
     </row>
-    <row r="32" spans="10:11" x14ac:dyDescent="0.25">
+    <row r="32" spans="10:11" x14ac:dyDescent="0.3">
       <c r="K32" s="1"/>
     </row>
-    <row r="33" spans="11:11" x14ac:dyDescent="0.25">
+    <row r="33" spans="11:11" x14ac:dyDescent="0.3">
       <c r="K33" s="1"/>
     </row>
-    <row r="34" spans="11:11" x14ac:dyDescent="0.25">
+    <row r="34" spans="11:11" x14ac:dyDescent="0.3">
       <c r="K34" s="1"/>
     </row>
-    <row r="35" spans="11:11" x14ac:dyDescent="0.25">
+    <row r="35" spans="11:11" x14ac:dyDescent="0.3">
       <c r="K35" s="1"/>
     </row>
-    <row r="36" spans="11:11" x14ac:dyDescent="0.25">
+    <row r="36" spans="11:11" x14ac:dyDescent="0.3">
       <c r="K36" s="1"/>
     </row>
-    <row r="37" spans="11:11" x14ac:dyDescent="0.25">
+    <row r="37" spans="11:11" x14ac:dyDescent="0.3">
       <c r="K37" s="1"/>
     </row>
-    <row r="38" spans="11:11" x14ac:dyDescent="0.25">
+    <row r="38" spans="11:11" x14ac:dyDescent="0.3">
       <c r="K38" s="1"/>
     </row>
-    <row r="39" spans="11:11" x14ac:dyDescent="0.25">
+    <row r="39" spans="11:11" x14ac:dyDescent="0.3">
       <c r="K39" s="1"/>
     </row>
-    <row r="40" spans="11:11" x14ac:dyDescent="0.25">
+    <row r="40" spans="11:11" x14ac:dyDescent="0.3">
       <c r="K40" s="1"/>
     </row>
   </sheetData>
@@ -7080,10 +6109,11 @@
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="M2" r:id="rId1" xr:uid="{A111A7B2-D9C5-4F09-955C-F59643DB73F8}"/>
+    <hyperlink ref="M2" r:id="rId1" display="AutoTestUNIQUE@gmail.com" xr:uid="{A2B6AFF1-BB2F-474B-AC43-AD97DD11409E}"/>
+    <hyperlink ref="M3" r:id="rId2" display="AutoTestUNIQUE@gmail.com" xr:uid="{6844504D-A967-411E-A0B7-19BE15FA6F52}"/>
   </hyperlinks>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0249999999999999" bottom="1.0249999999999999" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+  <pageSetup orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300" r:id="rId3"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;"Arial,Regular"&amp;10&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Arial,Regular"&amp;10Page &amp;P</oddFooter>
@@ -7095,25 +6125,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82133CBD-184A-4904-91FF-20FD4A9F3DA6}">
   <dimension ref="A1:Q4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="K4" sqref="K4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.44140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="24" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="23.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="31.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="23.88671875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="31.44140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.88671875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="22" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="31.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="31.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>1</v>
       </c>
@@ -7121,22 +6151,22 @@
         <v>12</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D1" s="6" t="s">
         <v>2</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="F1" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="H1" s="4" t="s">
         <v>33</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="H1" s="4" t="s">
-        <v>37</v>
       </c>
       <c r="I1" s="4" t="s">
         <v>18</v>
@@ -7148,65 +6178,65 @@
         <v>10</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="M1" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="N1" s="2"/>
       <c r="O1" s="2"/>
       <c r="P1" s="2"/>
       <c r="Q1" s="2"/>
     </row>
-    <row r="2" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>32</v>
-      </c>
       <c r="D2" s="3" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>7</v>
       </c>
       <c r="G2" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="J2" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="H2" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="J2" s="10" t="s">
-        <v>43</v>
-      </c>
       <c r="K2" s="3" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="L2" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="M2" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="N2" s="3"/>
       <c r="O2" s="3"/>
       <c r="P2" s="3"/>
       <c r="Q2" s="3"/>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
       <c r="G3" s="8"/>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
       <c r="G4" s="8"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated life policy keywprds
</commit_message>
<xml_diff>
--- a/Testdata/TestData.xlsx
+++ b/Testdata/TestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\poc_new\turtlemint\Testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4435B19F-1DE1-4327-BA2E-96AA8DF782EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCEBC18C-7225-422D-8950-71DF38CBF556}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="44">
   <si>
     <t>TC_01</t>
   </si>
@@ -113,9 +113,6 @@
   </si>
   <si>
     <t>IN1YR</t>
-  </si>
-  <si>
-    <t>TC_02</t>
   </si>
   <si>
     <t>Life</t>
@@ -940,7 +937,7 @@
         <v>9</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>28</v>
@@ -7095,8 +7092,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82133CBD-184A-4904-91FF-20FD4A9F3DA6}">
   <dimension ref="A1:Q4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="K4" sqref="K4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7121,22 +7118,22 @@
         <v>12</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D1" s="6" t="s">
         <v>2</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F1" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="G1" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="G1" s="4" t="s">
-        <v>34</v>
-      </c>
       <c r="H1" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="I1" s="4" t="s">
         <v>18</v>
@@ -7160,37 +7157,37 @@
     </row>
     <row r="2" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="C2" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>31</v>
-      </c>
       <c r="E2" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>7</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I2" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="J2" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="J2" s="10" t="s">
+      <c r="K2" s="3" t="s">
         <v>43</v>
-      </c>
-      <c r="K2" s="3" t="s">
-        <v>44</v>
       </c>
       <c r="L2" s="3" t="s">
         <v>21</v>

</xml_diff>

<commit_message>
Added health compare keywords and test case
</commit_message>
<xml_diff>
--- a/Testdata/TestData.xlsx
+++ b/Testdata/TestData.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\poc_new\turtlemint\Testdata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\QualiZeal\POC_project\TurtleMint\result_validation\turtlemint\Testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47E7CA54-A26B-415A-A35C-82CF7771C2EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E1E47B3-961E-46A2-9134-74D0EFA4524C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="health_policy" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="56">
   <si>
     <t>TC_01</t>
   </si>
@@ -85,9 +85,6 @@
     <t>name</t>
   </si>
   <si>
-    <t>AutoTestUNIQUE@gmail.com</t>
-  </si>
-  <si>
     <t>customize_policyheader</t>
   </si>
   <si>
@@ -100,18 +97,12 @@
     <t>5 Lakhs</t>
   </si>
   <si>
-    <t>UNIQUEphno</t>
-  </si>
-  <si>
     <t>500051</t>
   </si>
   <si>
     <t>UPTO10LAKHS</t>
   </si>
   <si>
-    <t>UNIQUEfullname</t>
-  </si>
-  <si>
     <t>IN1YR</t>
   </si>
   <si>
@@ -160,12 +151,6 @@
     <t>RANDOM_EMAILID</t>
   </si>
   <si>
-    <t>Yearly</t>
-  </si>
-  <si>
-    <t>payment_frequency</t>
-  </si>
-  <si>
     <t>₹</t>
   </si>
   <si>
@@ -173,13 +158,49 @@
   </si>
   <si>
     <t>Waiver of Premium</t>
+  </si>
+  <si>
+    <t>Critical Illness - 22 Illness</t>
+  </si>
+  <si>
+    <t>TC_02</t>
+  </si>
+  <si>
+    <t>12-Oct-1988</t>
+  </si>
+  <si>
+    <t>7 Lac to 10 Lac</t>
+  </si>
+  <si>
+    <t>40 Lakhs</t>
+  </si>
+  <si>
+    <t>Self;Father;Mother</t>
+  </si>
+  <si>
+    <t>Self-25 years;Father-65 years;Mother-58 years</t>
+  </si>
+  <si>
+    <t>UPTO5LAKHS</t>
+  </si>
+  <si>
+    <t>All members</t>
+  </si>
+  <si>
+    <t>Self</t>
+  </si>
+  <si>
+    <t>TC_03</t>
+  </si>
+  <si>
+    <t>Self-30 years</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -303,12 +324,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FF4EC9B0"/>
-      <name val="Consolas"/>
-      <family val="3"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9CDCFE"/>
       <name val="Consolas"/>
       <family val="3"/>
     </font>
@@ -439,7 +454,7 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="14" fillId="9" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -455,10 +470,7 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -862,33 +874,33 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:ALH40"/>
   <sheetViews>
-    <sheetView topLeftCell="H1" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView tabSelected="1" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="11" style="1" customWidth="1"/>
-    <col min="2" max="2" width="16.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="59.140625" style="5" customWidth="1"/>
-    <col min="4" max="4" width="38.140625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="17" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="27.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="27.85546875" style="1" customWidth="1"/>
-    <col min="8" max="8" width="28.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.42578125" style="1"/>
-    <col min="10" max="10" width="26.7109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="26.7109375" style="5" customWidth="1"/>
-    <col min="12" max="12" width="25.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="31.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="25.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="13.7109375" style="1" customWidth="1"/>
-    <col min="16" max="16" width="16.28515625" style="1" customWidth="1"/>
-    <col min="17" max="996" width="11.42578125" style="1"/>
-    <col min="997" max="1014" width="8.7109375" customWidth="1"/>
+    <col min="2" max="2" width="16.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="59.109375" style="5" customWidth="1"/>
+    <col min="4" max="4" width="38.109375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="36.109375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="27.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="27.88671875" style="1" customWidth="1"/>
+    <col min="8" max="8" width="28.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.44140625" style="1"/>
+    <col min="10" max="10" width="26.6640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="26.6640625" style="5" customWidth="1"/>
+    <col min="12" max="12" width="25.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="31.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="25.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="18.109375" style="1" customWidth="1"/>
+    <col min="16" max="16" width="16.33203125" style="1" customWidth="1"/>
+    <col min="17" max="996" width="11.44140625" style="1"/>
+    <col min="997" max="1014" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:996" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:996" s="2" customFormat="1" ht="16.8" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>1</v>
       </c>
@@ -929,13 +941,13 @@
         <v>10</v>
       </c>
       <c r="N1" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="O1" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:996" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:996" s="3" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
@@ -946,2039 +958,127 @@
         <v>6</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>8</v>
+        <v>49</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>28</v>
-      </c>
+        <v>50</v>
+      </c>
+      <c r="G2" s="1"/>
       <c r="H2" s="3" t="s">
         <v>7</v>
       </c>
       <c r="I2" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="L2" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="M2" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="N2" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="O2" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:996" s="3" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A3" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="G3" s="1"/>
+      <c r="H3" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="L3" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="M3" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="N3" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="O3" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:996" s="3" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A4" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="G4" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="J2" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="L2" s="9" t="s">
+      <c r="H4" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="J4" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="M2" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="N2" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="O2" s="3" t="s">
-        <v>23</v>
+      <c r="K4" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="L4" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="M4" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="N4" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="O4" s="3" t="s">
+        <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:996" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="1"/>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
-      <c r="I3" s="1"/>
-      <c r="J3" s="3"/>
-      <c r="K3" s="1"/>
-      <c r="L3" s="1"/>
-      <c r="M3" s="1"/>
-      <c r="N3" s="1"/>
-      <c r="O3" s="1"/>
-      <c r="P3" s="1"/>
-      <c r="Q3" s="1"/>
-      <c r="R3" s="1"/>
-      <c r="S3" s="1"/>
-      <c r="T3" s="1"/>
-      <c r="U3" s="1"/>
-      <c r="V3" s="1"/>
-      <c r="W3" s="1"/>
-      <c r="X3" s="1"/>
-      <c r="Y3" s="1"/>
-      <c r="Z3" s="1"/>
-      <c r="AA3" s="1"/>
-      <c r="AB3" s="1"/>
-      <c r="AC3" s="1"/>
-      <c r="AD3" s="1"/>
-      <c r="AE3" s="1"/>
-      <c r="AF3" s="1"/>
-      <c r="AG3" s="1"/>
-      <c r="AH3" s="1"/>
-      <c r="AI3" s="1"/>
-      <c r="AJ3" s="1"/>
-      <c r="AK3" s="1"/>
-      <c r="AL3" s="1"/>
-      <c r="AM3" s="1"/>
-      <c r="AN3" s="1"/>
-      <c r="AO3" s="1"/>
-      <c r="AP3" s="1"/>
-      <c r="AQ3" s="1"/>
-      <c r="AR3" s="1"/>
-      <c r="AS3" s="1"/>
-      <c r="AT3" s="1"/>
-      <c r="AU3" s="1"/>
-      <c r="AV3" s="1"/>
-      <c r="AW3" s="1"/>
-      <c r="AX3" s="1"/>
-      <c r="AY3" s="1"/>
-      <c r="AZ3" s="1"/>
-      <c r="BA3" s="1"/>
-      <c r="BB3" s="1"/>
-      <c r="BC3" s="1"/>
-      <c r="BD3" s="1"/>
-      <c r="BE3" s="1"/>
-      <c r="BF3" s="1"/>
-      <c r="BG3" s="1"/>
-      <c r="BH3" s="1"/>
-      <c r="BI3" s="1"/>
-      <c r="BJ3" s="1"/>
-      <c r="BK3" s="1"/>
-      <c r="BL3" s="1"/>
-      <c r="BM3" s="1"/>
-      <c r="BN3" s="1"/>
-      <c r="BO3" s="1"/>
-      <c r="BP3" s="1"/>
-      <c r="BQ3" s="1"/>
-      <c r="BR3" s="1"/>
-      <c r="BS3" s="1"/>
-      <c r="BT3" s="1"/>
-      <c r="BU3" s="1"/>
-      <c r="BV3" s="1"/>
-      <c r="BW3" s="1"/>
-      <c r="BX3" s="1"/>
-      <c r="BY3" s="1"/>
-      <c r="BZ3" s="1"/>
-      <c r="CA3" s="1"/>
-      <c r="CB3" s="1"/>
-      <c r="CC3" s="1"/>
-      <c r="CD3" s="1"/>
-      <c r="CE3" s="1"/>
-      <c r="CF3" s="1"/>
-      <c r="CG3" s="1"/>
-      <c r="CH3" s="1"/>
-      <c r="CI3" s="1"/>
-      <c r="CJ3" s="1"/>
-      <c r="CK3" s="1"/>
-      <c r="CL3" s="1"/>
-      <c r="CM3" s="1"/>
-      <c r="CN3" s="1"/>
-      <c r="CO3" s="1"/>
-      <c r="CP3" s="1"/>
-      <c r="CQ3" s="1"/>
-      <c r="CR3" s="1"/>
-      <c r="CS3" s="1"/>
-      <c r="CT3" s="1"/>
-      <c r="CU3" s="1"/>
-      <c r="CV3" s="1"/>
-      <c r="CW3" s="1"/>
-      <c r="CX3" s="1"/>
-      <c r="CY3" s="1"/>
-      <c r="CZ3" s="1"/>
-      <c r="DA3" s="1"/>
-      <c r="DB3" s="1"/>
-      <c r="DC3" s="1"/>
-      <c r="DD3" s="1"/>
-      <c r="DE3" s="1"/>
-      <c r="DF3" s="1"/>
-      <c r="DG3" s="1"/>
-      <c r="DH3" s="1"/>
-      <c r="DI3" s="1"/>
-      <c r="DJ3" s="1"/>
-      <c r="DK3" s="1"/>
-      <c r="DL3" s="1"/>
-      <c r="DM3" s="1"/>
-      <c r="DN3" s="1"/>
-      <c r="DO3" s="1"/>
-      <c r="DP3" s="1"/>
-      <c r="DQ3" s="1"/>
-      <c r="DR3" s="1"/>
-      <c r="DS3" s="1"/>
-      <c r="DT3" s="1"/>
-      <c r="DU3" s="1"/>
-      <c r="DV3" s="1"/>
-      <c r="DW3" s="1"/>
-      <c r="DX3" s="1"/>
-      <c r="DY3" s="1"/>
-      <c r="DZ3" s="1"/>
-      <c r="EA3" s="1"/>
-      <c r="EB3" s="1"/>
-      <c r="EC3" s="1"/>
-      <c r="ED3" s="1"/>
-      <c r="EE3" s="1"/>
-      <c r="EF3" s="1"/>
-      <c r="EG3" s="1"/>
-      <c r="EH3" s="1"/>
-      <c r="EI3" s="1"/>
-      <c r="EJ3" s="1"/>
-      <c r="EK3" s="1"/>
-      <c r="EL3" s="1"/>
-      <c r="EM3" s="1"/>
-      <c r="EN3" s="1"/>
-      <c r="EO3" s="1"/>
-      <c r="EP3" s="1"/>
-      <c r="EQ3" s="1"/>
-      <c r="ER3" s="1"/>
-      <c r="ES3" s="1"/>
-      <c r="ET3" s="1"/>
-      <c r="EU3" s="1"/>
-      <c r="EV3" s="1"/>
-      <c r="EW3" s="1"/>
-      <c r="EX3" s="1"/>
-      <c r="EY3" s="1"/>
-      <c r="EZ3" s="1"/>
-      <c r="FA3" s="1"/>
-      <c r="FB3" s="1"/>
-      <c r="FC3" s="1"/>
-      <c r="FD3" s="1"/>
-      <c r="FE3" s="1"/>
-      <c r="FF3" s="1"/>
-      <c r="FG3" s="1"/>
-      <c r="FH3" s="1"/>
-      <c r="FI3" s="1"/>
-      <c r="FJ3" s="1"/>
-      <c r="FK3" s="1"/>
-      <c r="FL3" s="1"/>
-      <c r="FM3" s="1"/>
-      <c r="FN3" s="1"/>
-      <c r="FO3" s="1"/>
-      <c r="FP3" s="1"/>
-      <c r="FQ3" s="1"/>
-      <c r="FR3" s="1"/>
-      <c r="FS3" s="1"/>
-      <c r="FT3" s="1"/>
-      <c r="FU3" s="1"/>
-      <c r="FV3" s="1"/>
-      <c r="FW3" s="1"/>
-      <c r="FX3" s="1"/>
-      <c r="FY3" s="1"/>
-      <c r="FZ3" s="1"/>
-      <c r="GA3" s="1"/>
-      <c r="GB3" s="1"/>
-      <c r="GC3" s="1"/>
-      <c r="GD3" s="1"/>
-      <c r="GE3" s="1"/>
-      <c r="GF3" s="1"/>
-      <c r="GG3" s="1"/>
-      <c r="GH3" s="1"/>
-      <c r="GI3" s="1"/>
-      <c r="GJ3" s="1"/>
-      <c r="GK3" s="1"/>
-      <c r="GL3" s="1"/>
-      <c r="GM3" s="1"/>
-      <c r="GN3" s="1"/>
-      <c r="GO3" s="1"/>
-      <c r="GP3" s="1"/>
-      <c r="GQ3" s="1"/>
-      <c r="GR3" s="1"/>
-      <c r="GS3" s="1"/>
-      <c r="GT3" s="1"/>
-      <c r="GU3" s="1"/>
-      <c r="GV3" s="1"/>
-      <c r="GW3" s="1"/>
-      <c r="GX3" s="1"/>
-      <c r="GY3" s="1"/>
-      <c r="GZ3" s="1"/>
-      <c r="HA3" s="1"/>
-      <c r="HB3" s="1"/>
-      <c r="HC3" s="1"/>
-      <c r="HD3" s="1"/>
-      <c r="HE3" s="1"/>
-      <c r="HF3" s="1"/>
-      <c r="HG3" s="1"/>
-      <c r="HH3" s="1"/>
-      <c r="HI3" s="1"/>
-      <c r="HJ3" s="1"/>
-      <c r="HK3" s="1"/>
-      <c r="HL3" s="1"/>
-      <c r="HM3" s="1"/>
-      <c r="HN3" s="1"/>
-      <c r="HO3" s="1"/>
-      <c r="HP3" s="1"/>
-      <c r="HQ3" s="1"/>
-      <c r="HR3" s="1"/>
-      <c r="HS3" s="1"/>
-      <c r="HT3" s="1"/>
-      <c r="HU3" s="1"/>
-      <c r="HV3" s="1"/>
-      <c r="HW3" s="1"/>
-      <c r="HX3" s="1"/>
-      <c r="HY3" s="1"/>
-      <c r="HZ3" s="1"/>
-      <c r="IA3" s="1"/>
-      <c r="IB3" s="1"/>
-      <c r="IC3" s="1"/>
-      <c r="ID3" s="1"/>
-      <c r="IE3" s="1"/>
-      <c r="IF3" s="1"/>
-      <c r="IG3" s="1"/>
-      <c r="IH3" s="1"/>
-      <c r="II3" s="1"/>
-      <c r="IJ3" s="1"/>
-      <c r="IK3" s="1"/>
-      <c r="IL3" s="1"/>
-      <c r="IM3" s="1"/>
-      <c r="IN3" s="1"/>
-      <c r="IO3" s="1"/>
-      <c r="IP3" s="1"/>
-      <c r="IQ3" s="1"/>
-      <c r="IR3" s="1"/>
-      <c r="IS3" s="1"/>
-      <c r="IT3" s="1"/>
-      <c r="IU3" s="1"/>
-      <c r="IV3" s="1"/>
-      <c r="IW3" s="1"/>
-      <c r="IX3" s="1"/>
-      <c r="IY3" s="1"/>
-      <c r="IZ3" s="1"/>
-      <c r="JA3" s="1"/>
-      <c r="JB3" s="1"/>
-      <c r="JC3" s="1"/>
-      <c r="JD3" s="1"/>
-      <c r="JE3" s="1"/>
-      <c r="JF3" s="1"/>
-      <c r="JG3" s="1"/>
-      <c r="JH3" s="1"/>
-      <c r="JI3" s="1"/>
-      <c r="JJ3" s="1"/>
-      <c r="JK3" s="1"/>
-      <c r="JL3" s="1"/>
-      <c r="JM3" s="1"/>
-      <c r="JN3" s="1"/>
-      <c r="JO3" s="1"/>
-      <c r="JP3" s="1"/>
-      <c r="JQ3" s="1"/>
-      <c r="JR3" s="1"/>
-      <c r="JS3" s="1"/>
-      <c r="JT3" s="1"/>
-      <c r="JU3" s="1"/>
-      <c r="JV3" s="1"/>
-      <c r="JW3" s="1"/>
-      <c r="JX3" s="1"/>
-      <c r="JY3" s="1"/>
-      <c r="JZ3" s="1"/>
-      <c r="KA3" s="1"/>
-      <c r="KB3" s="1"/>
-      <c r="KC3" s="1"/>
-      <c r="KD3" s="1"/>
-      <c r="KE3" s="1"/>
-      <c r="KF3" s="1"/>
-      <c r="KG3" s="1"/>
-      <c r="KH3" s="1"/>
-      <c r="KI3" s="1"/>
-      <c r="KJ3" s="1"/>
-      <c r="KK3" s="1"/>
-      <c r="KL3" s="1"/>
-      <c r="KM3" s="1"/>
-      <c r="KN3" s="1"/>
-      <c r="KO3" s="1"/>
-      <c r="KP3" s="1"/>
-      <c r="KQ3" s="1"/>
-      <c r="KR3" s="1"/>
-      <c r="KS3" s="1"/>
-      <c r="KT3" s="1"/>
-      <c r="KU3" s="1"/>
-      <c r="KV3" s="1"/>
-      <c r="KW3" s="1"/>
-      <c r="KX3" s="1"/>
-      <c r="KY3" s="1"/>
-      <c r="KZ3" s="1"/>
-      <c r="LA3" s="1"/>
-      <c r="LB3" s="1"/>
-      <c r="LC3" s="1"/>
-      <c r="LD3" s="1"/>
-      <c r="LE3" s="1"/>
-      <c r="LF3" s="1"/>
-      <c r="LG3" s="1"/>
-      <c r="LH3" s="1"/>
-      <c r="LI3" s="1"/>
-      <c r="LJ3" s="1"/>
-      <c r="LK3" s="1"/>
-      <c r="LL3" s="1"/>
-      <c r="LM3" s="1"/>
-      <c r="LN3" s="1"/>
-      <c r="LO3" s="1"/>
-      <c r="LP3" s="1"/>
-      <c r="LQ3" s="1"/>
-      <c r="LR3" s="1"/>
-      <c r="LS3" s="1"/>
-      <c r="LT3" s="1"/>
-      <c r="LU3" s="1"/>
-      <c r="LV3" s="1"/>
-      <c r="LW3" s="1"/>
-      <c r="LX3" s="1"/>
-      <c r="LY3" s="1"/>
-      <c r="LZ3" s="1"/>
-      <c r="MA3" s="1"/>
-      <c r="MB3" s="1"/>
-      <c r="MC3" s="1"/>
-      <c r="MD3" s="1"/>
-      <c r="ME3" s="1"/>
-      <c r="MF3" s="1"/>
-      <c r="MG3" s="1"/>
-      <c r="MH3" s="1"/>
-      <c r="MI3" s="1"/>
-      <c r="MJ3" s="1"/>
-      <c r="MK3" s="1"/>
-      <c r="ML3" s="1"/>
-      <c r="MM3" s="1"/>
-      <c r="MN3" s="1"/>
-      <c r="MO3" s="1"/>
-      <c r="MP3" s="1"/>
-      <c r="MQ3" s="1"/>
-      <c r="MR3" s="1"/>
-      <c r="MS3" s="1"/>
-      <c r="MT3" s="1"/>
-      <c r="MU3" s="1"/>
-      <c r="MV3" s="1"/>
-      <c r="MW3" s="1"/>
-      <c r="MX3" s="1"/>
-      <c r="MY3" s="1"/>
-      <c r="MZ3" s="1"/>
-      <c r="NA3" s="1"/>
-      <c r="NB3" s="1"/>
-      <c r="NC3" s="1"/>
-      <c r="ND3" s="1"/>
-      <c r="NE3" s="1"/>
-      <c r="NF3" s="1"/>
-      <c r="NG3" s="1"/>
-      <c r="NH3" s="1"/>
-      <c r="NI3" s="1"/>
-      <c r="NJ3" s="1"/>
-      <c r="NK3" s="1"/>
-      <c r="NL3" s="1"/>
-      <c r="NM3" s="1"/>
-      <c r="NN3" s="1"/>
-      <c r="NO3" s="1"/>
-      <c r="NP3" s="1"/>
-      <c r="NQ3" s="1"/>
-      <c r="NR3" s="1"/>
-      <c r="NS3" s="1"/>
-      <c r="NT3" s="1"/>
-      <c r="NU3" s="1"/>
-      <c r="NV3" s="1"/>
-      <c r="NW3" s="1"/>
-      <c r="NX3" s="1"/>
-      <c r="NY3" s="1"/>
-      <c r="NZ3" s="1"/>
-      <c r="OA3" s="1"/>
-      <c r="OB3" s="1"/>
-      <c r="OC3" s="1"/>
-      <c r="OD3" s="1"/>
-      <c r="OE3" s="1"/>
-      <c r="OF3" s="1"/>
-      <c r="OG3" s="1"/>
-      <c r="OH3" s="1"/>
-      <c r="OI3" s="1"/>
-      <c r="OJ3" s="1"/>
-      <c r="OK3" s="1"/>
-      <c r="OL3" s="1"/>
-      <c r="OM3" s="1"/>
-      <c r="ON3" s="1"/>
-      <c r="OO3" s="1"/>
-      <c r="OP3" s="1"/>
-      <c r="OQ3" s="1"/>
-      <c r="OR3" s="1"/>
-      <c r="OS3" s="1"/>
-      <c r="OT3" s="1"/>
-      <c r="OU3" s="1"/>
-      <c r="OV3" s="1"/>
-      <c r="OW3" s="1"/>
-      <c r="OX3" s="1"/>
-      <c r="OY3" s="1"/>
-      <c r="OZ3" s="1"/>
-      <c r="PA3" s="1"/>
-      <c r="PB3" s="1"/>
-      <c r="PC3" s="1"/>
-      <c r="PD3" s="1"/>
-      <c r="PE3" s="1"/>
-      <c r="PF3" s="1"/>
-      <c r="PG3" s="1"/>
-      <c r="PH3" s="1"/>
-      <c r="PI3" s="1"/>
-      <c r="PJ3" s="1"/>
-      <c r="PK3" s="1"/>
-      <c r="PL3" s="1"/>
-      <c r="PM3" s="1"/>
-      <c r="PN3" s="1"/>
-      <c r="PO3" s="1"/>
-      <c r="PP3" s="1"/>
-      <c r="PQ3" s="1"/>
-      <c r="PR3" s="1"/>
-      <c r="PS3" s="1"/>
-      <c r="PT3" s="1"/>
-      <c r="PU3" s="1"/>
-      <c r="PV3" s="1"/>
-      <c r="PW3" s="1"/>
-      <c r="PX3" s="1"/>
-      <c r="PY3" s="1"/>
-      <c r="PZ3" s="1"/>
-      <c r="QA3" s="1"/>
-      <c r="QB3" s="1"/>
-      <c r="QC3" s="1"/>
-      <c r="QD3" s="1"/>
-      <c r="QE3" s="1"/>
-      <c r="QF3" s="1"/>
-      <c r="QG3" s="1"/>
-      <c r="QH3" s="1"/>
-      <c r="QI3" s="1"/>
-      <c r="QJ3" s="1"/>
-      <c r="QK3" s="1"/>
-      <c r="QL3" s="1"/>
-      <c r="QM3" s="1"/>
-      <c r="QN3" s="1"/>
-      <c r="QO3" s="1"/>
-      <c r="QP3" s="1"/>
-      <c r="QQ3" s="1"/>
-      <c r="QR3" s="1"/>
-      <c r="QS3" s="1"/>
-      <c r="QT3" s="1"/>
-      <c r="QU3" s="1"/>
-      <c r="QV3" s="1"/>
-      <c r="QW3" s="1"/>
-      <c r="QX3" s="1"/>
-      <c r="QY3" s="1"/>
-      <c r="QZ3" s="1"/>
-      <c r="RA3" s="1"/>
-      <c r="RB3" s="1"/>
-      <c r="RC3" s="1"/>
-      <c r="RD3" s="1"/>
-      <c r="RE3" s="1"/>
-      <c r="RF3" s="1"/>
-      <c r="RG3" s="1"/>
-      <c r="RH3" s="1"/>
-      <c r="RI3" s="1"/>
-      <c r="RJ3" s="1"/>
-      <c r="RK3" s="1"/>
-      <c r="RL3" s="1"/>
-      <c r="RM3" s="1"/>
-      <c r="RN3" s="1"/>
-      <c r="RO3" s="1"/>
-      <c r="RP3" s="1"/>
-      <c r="RQ3" s="1"/>
-      <c r="RR3" s="1"/>
-      <c r="RS3" s="1"/>
-      <c r="RT3" s="1"/>
-      <c r="RU3" s="1"/>
-      <c r="RV3" s="1"/>
-      <c r="RW3" s="1"/>
-      <c r="RX3" s="1"/>
-      <c r="RY3" s="1"/>
-      <c r="RZ3" s="1"/>
-      <c r="SA3" s="1"/>
-      <c r="SB3" s="1"/>
-      <c r="SC3" s="1"/>
-      <c r="SD3" s="1"/>
-      <c r="SE3" s="1"/>
-      <c r="SF3" s="1"/>
-      <c r="SG3" s="1"/>
-      <c r="SH3" s="1"/>
-      <c r="SI3" s="1"/>
-      <c r="SJ3" s="1"/>
-      <c r="SK3" s="1"/>
-      <c r="SL3" s="1"/>
-      <c r="SM3" s="1"/>
-      <c r="SN3" s="1"/>
-      <c r="SO3" s="1"/>
-      <c r="SP3" s="1"/>
-      <c r="SQ3" s="1"/>
-      <c r="SR3" s="1"/>
-      <c r="SS3" s="1"/>
-      <c r="ST3" s="1"/>
-      <c r="SU3" s="1"/>
-      <c r="SV3" s="1"/>
-      <c r="SW3" s="1"/>
-      <c r="SX3" s="1"/>
-      <c r="SY3" s="1"/>
-      <c r="SZ3" s="1"/>
-      <c r="TA3" s="1"/>
-      <c r="TB3" s="1"/>
-      <c r="TC3" s="1"/>
-      <c r="TD3" s="1"/>
-      <c r="TE3" s="1"/>
-      <c r="TF3" s="1"/>
-      <c r="TG3" s="1"/>
-      <c r="TH3" s="1"/>
-      <c r="TI3" s="1"/>
-      <c r="TJ3" s="1"/>
-      <c r="TK3" s="1"/>
-      <c r="TL3" s="1"/>
-      <c r="TM3" s="1"/>
-      <c r="TN3" s="1"/>
-      <c r="TO3" s="1"/>
-      <c r="TP3" s="1"/>
-      <c r="TQ3" s="1"/>
-      <c r="TR3" s="1"/>
-      <c r="TS3" s="1"/>
-      <c r="TT3" s="1"/>
-      <c r="TU3" s="1"/>
-      <c r="TV3" s="1"/>
-      <c r="TW3" s="1"/>
-      <c r="TX3" s="1"/>
-      <c r="TY3" s="1"/>
-      <c r="TZ3" s="1"/>
-      <c r="UA3" s="1"/>
-      <c r="UB3" s="1"/>
-      <c r="UC3" s="1"/>
-      <c r="UD3" s="1"/>
-      <c r="UE3" s="1"/>
-      <c r="UF3" s="1"/>
-      <c r="UG3" s="1"/>
-      <c r="UH3" s="1"/>
-      <c r="UI3" s="1"/>
-      <c r="UJ3" s="1"/>
-      <c r="UK3" s="1"/>
-      <c r="UL3" s="1"/>
-      <c r="UM3" s="1"/>
-      <c r="UN3" s="1"/>
-      <c r="UO3" s="1"/>
-      <c r="UP3" s="1"/>
-      <c r="UQ3" s="1"/>
-      <c r="UR3" s="1"/>
-      <c r="US3" s="1"/>
-      <c r="UT3" s="1"/>
-      <c r="UU3" s="1"/>
-      <c r="UV3" s="1"/>
-      <c r="UW3" s="1"/>
-      <c r="UX3" s="1"/>
-      <c r="UY3" s="1"/>
-      <c r="UZ3" s="1"/>
-      <c r="VA3" s="1"/>
-      <c r="VB3" s="1"/>
-      <c r="VC3" s="1"/>
-      <c r="VD3" s="1"/>
-      <c r="VE3" s="1"/>
-      <c r="VF3" s="1"/>
-      <c r="VG3" s="1"/>
-      <c r="VH3" s="1"/>
-      <c r="VI3" s="1"/>
-      <c r="VJ3" s="1"/>
-      <c r="VK3" s="1"/>
-      <c r="VL3" s="1"/>
-      <c r="VM3" s="1"/>
-      <c r="VN3" s="1"/>
-      <c r="VO3" s="1"/>
-      <c r="VP3" s="1"/>
-      <c r="VQ3" s="1"/>
-      <c r="VR3" s="1"/>
-      <c r="VS3" s="1"/>
-      <c r="VT3" s="1"/>
-      <c r="VU3" s="1"/>
-      <c r="VV3" s="1"/>
-      <c r="VW3" s="1"/>
-      <c r="VX3" s="1"/>
-      <c r="VY3" s="1"/>
-      <c r="VZ3" s="1"/>
-      <c r="WA3" s="1"/>
-      <c r="WB3" s="1"/>
-      <c r="WC3" s="1"/>
-      <c r="WD3" s="1"/>
-      <c r="WE3" s="1"/>
-      <c r="WF3" s="1"/>
-      <c r="WG3" s="1"/>
-      <c r="WH3" s="1"/>
-      <c r="WI3" s="1"/>
-      <c r="WJ3" s="1"/>
-      <c r="WK3" s="1"/>
-      <c r="WL3" s="1"/>
-      <c r="WM3" s="1"/>
-      <c r="WN3" s="1"/>
-      <c r="WO3" s="1"/>
-      <c r="WP3" s="1"/>
-      <c r="WQ3" s="1"/>
-      <c r="WR3" s="1"/>
-      <c r="WS3" s="1"/>
-      <c r="WT3" s="1"/>
-      <c r="WU3" s="1"/>
-      <c r="WV3" s="1"/>
-      <c r="WW3" s="1"/>
-      <c r="WX3" s="1"/>
-      <c r="WY3" s="1"/>
-      <c r="WZ3" s="1"/>
-      <c r="XA3" s="1"/>
-      <c r="XB3" s="1"/>
-      <c r="XC3" s="1"/>
-      <c r="XD3" s="1"/>
-      <c r="XE3" s="1"/>
-      <c r="XF3" s="1"/>
-      <c r="XG3" s="1"/>
-      <c r="XH3" s="1"/>
-      <c r="XI3" s="1"/>
-      <c r="XJ3" s="1"/>
-      <c r="XK3" s="1"/>
-      <c r="XL3" s="1"/>
-      <c r="XM3" s="1"/>
-      <c r="XN3" s="1"/>
-      <c r="XO3" s="1"/>
-      <c r="XP3" s="1"/>
-      <c r="XQ3" s="1"/>
-      <c r="XR3" s="1"/>
-      <c r="XS3" s="1"/>
-      <c r="XT3" s="1"/>
-      <c r="XU3" s="1"/>
-      <c r="XV3" s="1"/>
-      <c r="XW3" s="1"/>
-      <c r="XX3" s="1"/>
-      <c r="XY3" s="1"/>
-      <c r="XZ3" s="1"/>
-      <c r="YA3" s="1"/>
-      <c r="YB3" s="1"/>
-      <c r="YC3" s="1"/>
-      <c r="YD3" s="1"/>
-      <c r="YE3" s="1"/>
-      <c r="YF3" s="1"/>
-      <c r="YG3" s="1"/>
-      <c r="YH3" s="1"/>
-      <c r="YI3" s="1"/>
-      <c r="YJ3" s="1"/>
-      <c r="YK3" s="1"/>
-      <c r="YL3" s="1"/>
-      <c r="YM3" s="1"/>
-      <c r="YN3" s="1"/>
-      <c r="YO3" s="1"/>
-      <c r="YP3" s="1"/>
-      <c r="YQ3" s="1"/>
-      <c r="YR3" s="1"/>
-      <c r="YS3" s="1"/>
-      <c r="YT3" s="1"/>
-      <c r="YU3" s="1"/>
-      <c r="YV3" s="1"/>
-      <c r="YW3" s="1"/>
-      <c r="YX3" s="1"/>
-      <c r="YY3" s="1"/>
-      <c r="YZ3" s="1"/>
-      <c r="ZA3" s="1"/>
-      <c r="ZB3" s="1"/>
-      <c r="ZC3" s="1"/>
-      <c r="ZD3" s="1"/>
-      <c r="ZE3" s="1"/>
-      <c r="ZF3" s="1"/>
-      <c r="ZG3" s="1"/>
-      <c r="ZH3" s="1"/>
-      <c r="ZI3" s="1"/>
-      <c r="ZJ3" s="1"/>
-      <c r="ZK3" s="1"/>
-      <c r="ZL3" s="1"/>
-      <c r="ZM3" s="1"/>
-      <c r="ZN3" s="1"/>
-      <c r="ZO3" s="1"/>
-      <c r="ZP3" s="1"/>
-      <c r="ZQ3" s="1"/>
-      <c r="ZR3" s="1"/>
-      <c r="ZS3" s="1"/>
-      <c r="ZT3" s="1"/>
-      <c r="ZU3" s="1"/>
-      <c r="ZV3" s="1"/>
-      <c r="ZW3" s="1"/>
-      <c r="ZX3" s="1"/>
-      <c r="ZY3" s="1"/>
-      <c r="ZZ3" s="1"/>
-      <c r="AAA3" s="1"/>
-      <c r="AAB3" s="1"/>
-      <c r="AAC3" s="1"/>
-      <c r="AAD3" s="1"/>
-      <c r="AAE3" s="1"/>
-      <c r="AAF3" s="1"/>
-      <c r="AAG3" s="1"/>
-      <c r="AAH3" s="1"/>
-      <c r="AAI3" s="1"/>
-      <c r="AAJ3" s="1"/>
-      <c r="AAK3" s="1"/>
-      <c r="AAL3" s="1"/>
-      <c r="AAM3" s="1"/>
-      <c r="AAN3" s="1"/>
-      <c r="AAO3" s="1"/>
-      <c r="AAP3" s="1"/>
-      <c r="AAQ3" s="1"/>
-      <c r="AAR3" s="1"/>
-      <c r="AAS3" s="1"/>
-      <c r="AAT3" s="1"/>
-      <c r="AAU3" s="1"/>
-      <c r="AAV3" s="1"/>
-      <c r="AAW3" s="1"/>
-      <c r="AAX3" s="1"/>
-      <c r="AAY3" s="1"/>
-      <c r="AAZ3" s="1"/>
-      <c r="ABA3" s="1"/>
-      <c r="ABB3" s="1"/>
-      <c r="ABC3" s="1"/>
-      <c r="ABD3" s="1"/>
-      <c r="ABE3" s="1"/>
-      <c r="ABF3" s="1"/>
-      <c r="ABG3" s="1"/>
-      <c r="ABH3" s="1"/>
-      <c r="ABI3" s="1"/>
-      <c r="ABJ3" s="1"/>
-      <c r="ABK3" s="1"/>
-      <c r="ABL3" s="1"/>
-      <c r="ABM3" s="1"/>
-      <c r="ABN3" s="1"/>
-      <c r="ABO3" s="1"/>
-      <c r="ABP3" s="1"/>
-      <c r="ABQ3" s="1"/>
-      <c r="ABR3" s="1"/>
-      <c r="ABS3" s="1"/>
-      <c r="ABT3" s="1"/>
-      <c r="ABU3" s="1"/>
-      <c r="ABV3" s="1"/>
-      <c r="ABW3" s="1"/>
-      <c r="ABX3" s="1"/>
-      <c r="ABY3" s="1"/>
-      <c r="ABZ3" s="1"/>
-      <c r="ACA3" s="1"/>
-      <c r="ACB3" s="1"/>
-      <c r="ACC3" s="1"/>
-      <c r="ACD3" s="1"/>
-      <c r="ACE3" s="1"/>
-      <c r="ACF3" s="1"/>
-      <c r="ACG3" s="1"/>
-      <c r="ACH3" s="1"/>
-      <c r="ACI3" s="1"/>
-      <c r="ACJ3" s="1"/>
-      <c r="ACK3" s="1"/>
-      <c r="ACL3" s="1"/>
-      <c r="ACM3" s="1"/>
-      <c r="ACN3" s="1"/>
-      <c r="ACO3" s="1"/>
-      <c r="ACP3" s="1"/>
-      <c r="ACQ3" s="1"/>
-      <c r="ACR3" s="1"/>
-      <c r="ACS3" s="1"/>
-      <c r="ACT3" s="1"/>
-      <c r="ACU3" s="1"/>
-      <c r="ACV3" s="1"/>
-      <c r="ACW3" s="1"/>
-      <c r="ACX3" s="1"/>
-      <c r="ACY3" s="1"/>
-      <c r="ACZ3" s="1"/>
-      <c r="ADA3" s="1"/>
-      <c r="ADB3" s="1"/>
-      <c r="ADC3" s="1"/>
-      <c r="ADD3" s="1"/>
-      <c r="ADE3" s="1"/>
-      <c r="ADF3" s="1"/>
-      <c r="ADG3" s="1"/>
-      <c r="ADH3" s="1"/>
-      <c r="ADI3" s="1"/>
-      <c r="ADJ3" s="1"/>
-      <c r="ADK3" s="1"/>
-      <c r="ADL3" s="1"/>
-      <c r="ADM3" s="1"/>
-      <c r="ADN3" s="1"/>
-      <c r="ADO3" s="1"/>
-      <c r="ADP3" s="1"/>
-      <c r="ADQ3" s="1"/>
-      <c r="ADR3" s="1"/>
-      <c r="ADS3" s="1"/>
-      <c r="ADT3" s="1"/>
-      <c r="ADU3" s="1"/>
-      <c r="ADV3" s="1"/>
-      <c r="ADW3" s="1"/>
-      <c r="ADX3" s="1"/>
-      <c r="ADY3" s="1"/>
-      <c r="ADZ3" s="1"/>
-      <c r="AEA3" s="1"/>
-      <c r="AEB3" s="1"/>
-      <c r="AEC3" s="1"/>
-      <c r="AED3" s="1"/>
-      <c r="AEE3" s="1"/>
-      <c r="AEF3" s="1"/>
-      <c r="AEG3" s="1"/>
-      <c r="AEH3" s="1"/>
-      <c r="AEI3" s="1"/>
-      <c r="AEJ3" s="1"/>
-      <c r="AEK3" s="1"/>
-      <c r="AEL3" s="1"/>
-      <c r="AEM3" s="1"/>
-      <c r="AEN3" s="1"/>
-      <c r="AEO3" s="1"/>
-      <c r="AEP3" s="1"/>
-      <c r="AEQ3" s="1"/>
-      <c r="AER3" s="1"/>
-      <c r="AES3" s="1"/>
-      <c r="AET3" s="1"/>
-      <c r="AEU3" s="1"/>
-      <c r="AEV3" s="1"/>
-      <c r="AEW3" s="1"/>
-      <c r="AEX3" s="1"/>
-      <c r="AEY3" s="1"/>
-      <c r="AEZ3" s="1"/>
-      <c r="AFA3" s="1"/>
-      <c r="AFB3" s="1"/>
-      <c r="AFC3" s="1"/>
-      <c r="AFD3" s="1"/>
-      <c r="AFE3" s="1"/>
-      <c r="AFF3" s="1"/>
-      <c r="AFG3" s="1"/>
-      <c r="AFH3" s="1"/>
-      <c r="AFI3" s="1"/>
-      <c r="AFJ3" s="1"/>
-      <c r="AFK3" s="1"/>
-      <c r="AFL3" s="1"/>
-      <c r="AFM3" s="1"/>
-      <c r="AFN3" s="1"/>
-      <c r="AFO3" s="1"/>
-      <c r="AFP3" s="1"/>
-      <c r="AFQ3" s="1"/>
-      <c r="AFR3" s="1"/>
-      <c r="AFS3" s="1"/>
-      <c r="AFT3" s="1"/>
-      <c r="AFU3" s="1"/>
-      <c r="AFV3" s="1"/>
-      <c r="AFW3" s="1"/>
-      <c r="AFX3" s="1"/>
-      <c r="AFY3" s="1"/>
-      <c r="AFZ3" s="1"/>
-      <c r="AGA3" s="1"/>
-      <c r="AGB3" s="1"/>
-      <c r="AGC3" s="1"/>
-      <c r="AGD3" s="1"/>
-      <c r="AGE3" s="1"/>
-      <c r="AGF3" s="1"/>
-      <c r="AGG3" s="1"/>
-      <c r="AGH3" s="1"/>
-      <c r="AGI3" s="1"/>
-      <c r="AGJ3" s="1"/>
-      <c r="AGK3" s="1"/>
-      <c r="AGL3" s="1"/>
-      <c r="AGM3" s="1"/>
-      <c r="AGN3" s="1"/>
-      <c r="AGO3" s="1"/>
-      <c r="AGP3" s="1"/>
-      <c r="AGQ3" s="1"/>
-      <c r="AGR3" s="1"/>
-      <c r="AGS3" s="1"/>
-      <c r="AGT3" s="1"/>
-      <c r="AGU3" s="1"/>
-      <c r="AGV3" s="1"/>
-      <c r="AGW3" s="1"/>
-      <c r="AGX3" s="1"/>
-      <c r="AGY3" s="1"/>
-      <c r="AGZ3" s="1"/>
-      <c r="AHA3" s="1"/>
-      <c r="AHB3" s="1"/>
-      <c r="AHC3" s="1"/>
-      <c r="AHD3" s="1"/>
-      <c r="AHE3" s="1"/>
-      <c r="AHF3" s="1"/>
-      <c r="AHG3" s="1"/>
-      <c r="AHH3" s="1"/>
-      <c r="AHI3" s="1"/>
-      <c r="AHJ3" s="1"/>
-      <c r="AHK3" s="1"/>
-      <c r="AHL3" s="1"/>
-      <c r="AHM3" s="1"/>
-      <c r="AHN3" s="1"/>
-      <c r="AHO3" s="1"/>
-      <c r="AHP3" s="1"/>
-      <c r="AHQ3" s="1"/>
-      <c r="AHR3" s="1"/>
-      <c r="AHS3" s="1"/>
-      <c r="AHT3" s="1"/>
-      <c r="AHU3" s="1"/>
-      <c r="AHV3" s="1"/>
-      <c r="AHW3" s="1"/>
-      <c r="AHX3" s="1"/>
-      <c r="AHY3" s="1"/>
-      <c r="AHZ3" s="1"/>
-      <c r="AIA3" s="1"/>
-      <c r="AIB3" s="1"/>
-      <c r="AIC3" s="1"/>
-      <c r="AID3" s="1"/>
-      <c r="AIE3" s="1"/>
-      <c r="AIF3" s="1"/>
-      <c r="AIG3" s="1"/>
-      <c r="AIH3" s="1"/>
-      <c r="AII3" s="1"/>
-      <c r="AIJ3" s="1"/>
-      <c r="AIK3" s="1"/>
-      <c r="AIL3" s="1"/>
-      <c r="AIM3" s="1"/>
-      <c r="AIN3" s="1"/>
-      <c r="AIO3" s="1"/>
-      <c r="AIP3" s="1"/>
-      <c r="AIQ3" s="1"/>
-      <c r="AIR3" s="1"/>
-      <c r="AIS3" s="1"/>
-      <c r="AIT3" s="1"/>
-      <c r="AIU3" s="1"/>
-      <c r="AIV3" s="1"/>
-      <c r="AIW3" s="1"/>
-      <c r="AIX3" s="1"/>
-      <c r="AIY3" s="1"/>
-      <c r="AIZ3" s="1"/>
-      <c r="AJA3" s="1"/>
-      <c r="AJB3" s="1"/>
-      <c r="AJC3" s="1"/>
-      <c r="AJD3" s="1"/>
-      <c r="AJE3" s="1"/>
-      <c r="AJF3" s="1"/>
-      <c r="AJG3" s="1"/>
-      <c r="AJH3" s="1"/>
-      <c r="AJI3" s="1"/>
-      <c r="AJJ3" s="1"/>
-      <c r="AJK3" s="1"/>
-      <c r="AJL3" s="1"/>
-      <c r="AJM3" s="1"/>
-      <c r="AJN3" s="1"/>
-      <c r="AJO3" s="1"/>
-      <c r="AJP3" s="1"/>
-      <c r="AJQ3" s="1"/>
-      <c r="AJR3" s="1"/>
-      <c r="AJS3" s="1"/>
-      <c r="AJT3" s="1"/>
-      <c r="AJU3" s="1"/>
-      <c r="AJV3" s="1"/>
-      <c r="AJW3" s="1"/>
-      <c r="AJX3" s="1"/>
-      <c r="AJY3" s="1"/>
-      <c r="AJZ3" s="1"/>
-      <c r="AKA3" s="1"/>
-      <c r="AKB3" s="1"/>
-      <c r="AKC3" s="1"/>
-      <c r="AKD3" s="1"/>
-      <c r="AKE3" s="1"/>
-      <c r="AKF3" s="1"/>
-      <c r="AKG3" s="1"/>
-      <c r="AKH3" s="1"/>
-      <c r="AKI3" s="1"/>
-      <c r="AKJ3" s="1"/>
-      <c r="AKK3" s="1"/>
-      <c r="AKL3" s="1"/>
-      <c r="AKM3" s="1"/>
-      <c r="AKN3" s="1"/>
-      <c r="AKO3" s="1"/>
-      <c r="AKP3" s="1"/>
-      <c r="AKQ3" s="1"/>
-      <c r="AKR3" s="1"/>
-      <c r="AKS3" s="1"/>
-      <c r="AKT3" s="1"/>
-      <c r="AKU3" s="1"/>
-      <c r="AKV3" s="1"/>
-      <c r="AKW3" s="1"/>
-      <c r="AKX3" s="1"/>
-      <c r="AKY3" s="1"/>
-      <c r="AKZ3" s="1"/>
-      <c r="ALA3" s="1"/>
-      <c r="ALB3" s="1"/>
-      <c r="ALC3" s="1"/>
-      <c r="ALD3" s="1"/>
-      <c r="ALE3" s="1"/>
-      <c r="ALF3" s="1"/>
-      <c r="ALG3" s="1"/>
-      <c r="ALH3" s="1"/>
-    </row>
-    <row r="4" spans="1:996" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="1"/>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="7"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
-      <c r="H4" s="1"/>
-      <c r="I4" s="1"/>
-      <c r="J4" s="3"/>
-      <c r="K4" s="1"/>
-      <c r="L4" s="1"/>
-      <c r="M4" s="1"/>
-      <c r="N4" s="1"/>
-      <c r="O4" s="1"/>
-      <c r="P4" s="1"/>
-      <c r="Q4" s="1"/>
-      <c r="R4" s="1"/>
-      <c r="S4" s="1"/>
-      <c r="T4" s="1"/>
-      <c r="U4" s="1"/>
-      <c r="V4" s="1"/>
-      <c r="W4" s="1"/>
-      <c r="X4" s="1"/>
-      <c r="Y4" s="1"/>
-      <c r="Z4" s="1"/>
-      <c r="AA4" s="1"/>
-      <c r="AB4" s="1"/>
-      <c r="AC4" s="1"/>
-      <c r="AD4" s="1"/>
-      <c r="AE4" s="1"/>
-      <c r="AF4" s="1"/>
-      <c r="AG4" s="1"/>
-      <c r="AH4" s="1"/>
-      <c r="AI4" s="1"/>
-      <c r="AJ4" s="1"/>
-      <c r="AK4" s="1"/>
-      <c r="AL4" s="1"/>
-      <c r="AM4" s="1"/>
-      <c r="AN4" s="1"/>
-      <c r="AO4" s="1"/>
-      <c r="AP4" s="1"/>
-      <c r="AQ4" s="1"/>
-      <c r="AR4" s="1"/>
-      <c r="AS4" s="1"/>
-      <c r="AT4" s="1"/>
-      <c r="AU4" s="1"/>
-      <c r="AV4" s="1"/>
-      <c r="AW4" s="1"/>
-      <c r="AX4" s="1"/>
-      <c r="AY4" s="1"/>
-      <c r="AZ4" s="1"/>
-      <c r="BA4" s="1"/>
-      <c r="BB4" s="1"/>
-      <c r="BC4" s="1"/>
-      <c r="BD4" s="1"/>
-      <c r="BE4" s="1"/>
-      <c r="BF4" s="1"/>
-      <c r="BG4" s="1"/>
-      <c r="BH4" s="1"/>
-      <c r="BI4" s="1"/>
-      <c r="BJ4" s="1"/>
-      <c r="BK4" s="1"/>
-      <c r="BL4" s="1"/>
-      <c r="BM4" s="1"/>
-      <c r="BN4" s="1"/>
-      <c r="BO4" s="1"/>
-      <c r="BP4" s="1"/>
-      <c r="BQ4" s="1"/>
-      <c r="BR4" s="1"/>
-      <c r="BS4" s="1"/>
-      <c r="BT4" s="1"/>
-      <c r="BU4" s="1"/>
-      <c r="BV4" s="1"/>
-      <c r="BW4" s="1"/>
-      <c r="BX4" s="1"/>
-      <c r="BY4" s="1"/>
-      <c r="BZ4" s="1"/>
-      <c r="CA4" s="1"/>
-      <c r="CB4" s="1"/>
-      <c r="CC4" s="1"/>
-      <c r="CD4" s="1"/>
-      <c r="CE4" s="1"/>
-      <c r="CF4" s="1"/>
-      <c r="CG4" s="1"/>
-      <c r="CH4" s="1"/>
-      <c r="CI4" s="1"/>
-      <c r="CJ4" s="1"/>
-      <c r="CK4" s="1"/>
-      <c r="CL4" s="1"/>
-      <c r="CM4" s="1"/>
-      <c r="CN4" s="1"/>
-      <c r="CO4" s="1"/>
-      <c r="CP4" s="1"/>
-      <c r="CQ4" s="1"/>
-      <c r="CR4" s="1"/>
-      <c r="CS4" s="1"/>
-      <c r="CT4" s="1"/>
-      <c r="CU4" s="1"/>
-      <c r="CV4" s="1"/>
-      <c r="CW4" s="1"/>
-      <c r="CX4" s="1"/>
-      <c r="CY4" s="1"/>
-      <c r="CZ4" s="1"/>
-      <c r="DA4" s="1"/>
-      <c r="DB4" s="1"/>
-      <c r="DC4" s="1"/>
-      <c r="DD4" s="1"/>
-      <c r="DE4" s="1"/>
-      <c r="DF4" s="1"/>
-      <c r="DG4" s="1"/>
-      <c r="DH4" s="1"/>
-      <c r="DI4" s="1"/>
-      <c r="DJ4" s="1"/>
-      <c r="DK4" s="1"/>
-      <c r="DL4" s="1"/>
-      <c r="DM4" s="1"/>
-      <c r="DN4" s="1"/>
-      <c r="DO4" s="1"/>
-      <c r="DP4" s="1"/>
-      <c r="DQ4" s="1"/>
-      <c r="DR4" s="1"/>
-      <c r="DS4" s="1"/>
-      <c r="DT4" s="1"/>
-      <c r="DU4" s="1"/>
-      <c r="DV4" s="1"/>
-      <c r="DW4" s="1"/>
-      <c r="DX4" s="1"/>
-      <c r="DY4" s="1"/>
-      <c r="DZ4" s="1"/>
-      <c r="EA4" s="1"/>
-      <c r="EB4" s="1"/>
-      <c r="EC4" s="1"/>
-      <c r="ED4" s="1"/>
-      <c r="EE4" s="1"/>
-      <c r="EF4" s="1"/>
-      <c r="EG4" s="1"/>
-      <c r="EH4" s="1"/>
-      <c r="EI4" s="1"/>
-      <c r="EJ4" s="1"/>
-      <c r="EK4" s="1"/>
-      <c r="EL4" s="1"/>
-      <c r="EM4" s="1"/>
-      <c r="EN4" s="1"/>
-      <c r="EO4" s="1"/>
-      <c r="EP4" s="1"/>
-      <c r="EQ4" s="1"/>
-      <c r="ER4" s="1"/>
-      <c r="ES4" s="1"/>
-      <c r="ET4" s="1"/>
-      <c r="EU4" s="1"/>
-      <c r="EV4" s="1"/>
-      <c r="EW4" s="1"/>
-      <c r="EX4" s="1"/>
-      <c r="EY4" s="1"/>
-      <c r="EZ4" s="1"/>
-      <c r="FA4" s="1"/>
-      <c r="FB4" s="1"/>
-      <c r="FC4" s="1"/>
-      <c r="FD4" s="1"/>
-      <c r="FE4" s="1"/>
-      <c r="FF4" s="1"/>
-      <c r="FG4" s="1"/>
-      <c r="FH4" s="1"/>
-      <c r="FI4" s="1"/>
-      <c r="FJ4" s="1"/>
-      <c r="FK4" s="1"/>
-      <c r="FL4" s="1"/>
-      <c r="FM4" s="1"/>
-      <c r="FN4" s="1"/>
-      <c r="FO4" s="1"/>
-      <c r="FP4" s="1"/>
-      <c r="FQ4" s="1"/>
-      <c r="FR4" s="1"/>
-      <c r="FS4" s="1"/>
-      <c r="FT4" s="1"/>
-      <c r="FU4" s="1"/>
-      <c r="FV4" s="1"/>
-      <c r="FW4" s="1"/>
-      <c r="FX4" s="1"/>
-      <c r="FY4" s="1"/>
-      <c r="FZ4" s="1"/>
-      <c r="GA4" s="1"/>
-      <c r="GB4" s="1"/>
-      <c r="GC4" s="1"/>
-      <c r="GD4" s="1"/>
-      <c r="GE4" s="1"/>
-      <c r="GF4" s="1"/>
-      <c r="GG4" s="1"/>
-      <c r="GH4" s="1"/>
-      <c r="GI4" s="1"/>
-      <c r="GJ4" s="1"/>
-      <c r="GK4" s="1"/>
-      <c r="GL4" s="1"/>
-      <c r="GM4" s="1"/>
-      <c r="GN4" s="1"/>
-      <c r="GO4" s="1"/>
-      <c r="GP4" s="1"/>
-      <c r="GQ4" s="1"/>
-      <c r="GR4" s="1"/>
-      <c r="GS4" s="1"/>
-      <c r="GT4" s="1"/>
-      <c r="GU4" s="1"/>
-      <c r="GV4" s="1"/>
-      <c r="GW4" s="1"/>
-      <c r="GX4" s="1"/>
-      <c r="GY4" s="1"/>
-      <c r="GZ4" s="1"/>
-      <c r="HA4" s="1"/>
-      <c r="HB4" s="1"/>
-      <c r="HC4" s="1"/>
-      <c r="HD4" s="1"/>
-      <c r="HE4" s="1"/>
-      <c r="HF4" s="1"/>
-      <c r="HG4" s="1"/>
-      <c r="HH4" s="1"/>
-      <c r="HI4" s="1"/>
-      <c r="HJ4" s="1"/>
-      <c r="HK4" s="1"/>
-      <c r="HL4" s="1"/>
-      <c r="HM4" s="1"/>
-      <c r="HN4" s="1"/>
-      <c r="HO4" s="1"/>
-      <c r="HP4" s="1"/>
-      <c r="HQ4" s="1"/>
-      <c r="HR4" s="1"/>
-      <c r="HS4" s="1"/>
-      <c r="HT4" s="1"/>
-      <c r="HU4" s="1"/>
-      <c r="HV4" s="1"/>
-      <c r="HW4" s="1"/>
-      <c r="HX4" s="1"/>
-      <c r="HY4" s="1"/>
-      <c r="HZ4" s="1"/>
-      <c r="IA4" s="1"/>
-      <c r="IB4" s="1"/>
-      <c r="IC4" s="1"/>
-      <c r="ID4" s="1"/>
-      <c r="IE4" s="1"/>
-      <c r="IF4" s="1"/>
-      <c r="IG4" s="1"/>
-      <c r="IH4" s="1"/>
-      <c r="II4" s="1"/>
-      <c r="IJ4" s="1"/>
-      <c r="IK4" s="1"/>
-      <c r="IL4" s="1"/>
-      <c r="IM4" s="1"/>
-      <c r="IN4" s="1"/>
-      <c r="IO4" s="1"/>
-      <c r="IP4" s="1"/>
-      <c r="IQ4" s="1"/>
-      <c r="IR4" s="1"/>
-      <c r="IS4" s="1"/>
-      <c r="IT4" s="1"/>
-      <c r="IU4" s="1"/>
-      <c r="IV4" s="1"/>
-      <c r="IW4" s="1"/>
-      <c r="IX4" s="1"/>
-      <c r="IY4" s="1"/>
-      <c r="IZ4" s="1"/>
-      <c r="JA4" s="1"/>
-      <c r="JB4" s="1"/>
-      <c r="JC4" s="1"/>
-      <c r="JD4" s="1"/>
-      <c r="JE4" s="1"/>
-      <c r="JF4" s="1"/>
-      <c r="JG4" s="1"/>
-      <c r="JH4" s="1"/>
-      <c r="JI4" s="1"/>
-      <c r="JJ4" s="1"/>
-      <c r="JK4" s="1"/>
-      <c r="JL4" s="1"/>
-      <c r="JM4" s="1"/>
-      <c r="JN4" s="1"/>
-      <c r="JO4" s="1"/>
-      <c r="JP4" s="1"/>
-      <c r="JQ4" s="1"/>
-      <c r="JR4" s="1"/>
-      <c r="JS4" s="1"/>
-      <c r="JT4" s="1"/>
-      <c r="JU4" s="1"/>
-      <c r="JV4" s="1"/>
-      <c r="JW4" s="1"/>
-      <c r="JX4" s="1"/>
-      <c r="JY4" s="1"/>
-      <c r="JZ4" s="1"/>
-      <c r="KA4" s="1"/>
-      <c r="KB4" s="1"/>
-      <c r="KC4" s="1"/>
-      <c r="KD4" s="1"/>
-      <c r="KE4" s="1"/>
-      <c r="KF4" s="1"/>
-      <c r="KG4" s="1"/>
-      <c r="KH4" s="1"/>
-      <c r="KI4" s="1"/>
-      <c r="KJ4" s="1"/>
-      <c r="KK4" s="1"/>
-      <c r="KL4" s="1"/>
-      <c r="KM4" s="1"/>
-      <c r="KN4" s="1"/>
-      <c r="KO4" s="1"/>
-      <c r="KP4" s="1"/>
-      <c r="KQ4" s="1"/>
-      <c r="KR4" s="1"/>
-      <c r="KS4" s="1"/>
-      <c r="KT4" s="1"/>
-      <c r="KU4" s="1"/>
-      <c r="KV4" s="1"/>
-      <c r="KW4" s="1"/>
-      <c r="KX4" s="1"/>
-      <c r="KY4" s="1"/>
-      <c r="KZ4" s="1"/>
-      <c r="LA4" s="1"/>
-      <c r="LB4" s="1"/>
-      <c r="LC4" s="1"/>
-      <c r="LD4" s="1"/>
-      <c r="LE4" s="1"/>
-      <c r="LF4" s="1"/>
-      <c r="LG4" s="1"/>
-      <c r="LH4" s="1"/>
-      <c r="LI4" s="1"/>
-      <c r="LJ4" s="1"/>
-      <c r="LK4" s="1"/>
-      <c r="LL4" s="1"/>
-      <c r="LM4" s="1"/>
-      <c r="LN4" s="1"/>
-      <c r="LO4" s="1"/>
-      <c r="LP4" s="1"/>
-      <c r="LQ4" s="1"/>
-      <c r="LR4" s="1"/>
-      <c r="LS4" s="1"/>
-      <c r="LT4" s="1"/>
-      <c r="LU4" s="1"/>
-      <c r="LV4" s="1"/>
-      <c r="LW4" s="1"/>
-      <c r="LX4" s="1"/>
-      <c r="LY4" s="1"/>
-      <c r="LZ4" s="1"/>
-      <c r="MA4" s="1"/>
-      <c r="MB4" s="1"/>
-      <c r="MC4" s="1"/>
-      <c r="MD4" s="1"/>
-      <c r="ME4" s="1"/>
-      <c r="MF4" s="1"/>
-      <c r="MG4" s="1"/>
-      <c r="MH4" s="1"/>
-      <c r="MI4" s="1"/>
-      <c r="MJ4" s="1"/>
-      <c r="MK4" s="1"/>
-      <c r="ML4" s="1"/>
-      <c r="MM4" s="1"/>
-      <c r="MN4" s="1"/>
-      <c r="MO4" s="1"/>
-      <c r="MP4" s="1"/>
-      <c r="MQ4" s="1"/>
-      <c r="MR4" s="1"/>
-      <c r="MS4" s="1"/>
-      <c r="MT4" s="1"/>
-      <c r="MU4" s="1"/>
-      <c r="MV4" s="1"/>
-      <c r="MW4" s="1"/>
-      <c r="MX4" s="1"/>
-      <c r="MY4" s="1"/>
-      <c r="MZ4" s="1"/>
-      <c r="NA4" s="1"/>
-      <c r="NB4" s="1"/>
-      <c r="NC4" s="1"/>
-      <c r="ND4" s="1"/>
-      <c r="NE4" s="1"/>
-      <c r="NF4" s="1"/>
-      <c r="NG4" s="1"/>
-      <c r="NH4" s="1"/>
-      <c r="NI4" s="1"/>
-      <c r="NJ4" s="1"/>
-      <c r="NK4" s="1"/>
-      <c r="NL4" s="1"/>
-      <c r="NM4" s="1"/>
-      <c r="NN4" s="1"/>
-      <c r="NO4" s="1"/>
-      <c r="NP4" s="1"/>
-      <c r="NQ4" s="1"/>
-      <c r="NR4" s="1"/>
-      <c r="NS4" s="1"/>
-      <c r="NT4" s="1"/>
-      <c r="NU4" s="1"/>
-      <c r="NV4" s="1"/>
-      <c r="NW4" s="1"/>
-      <c r="NX4" s="1"/>
-      <c r="NY4" s="1"/>
-      <c r="NZ4" s="1"/>
-      <c r="OA4" s="1"/>
-      <c r="OB4" s="1"/>
-      <c r="OC4" s="1"/>
-      <c r="OD4" s="1"/>
-      <c r="OE4" s="1"/>
-      <c r="OF4" s="1"/>
-      <c r="OG4" s="1"/>
-      <c r="OH4" s="1"/>
-      <c r="OI4" s="1"/>
-      <c r="OJ4" s="1"/>
-      <c r="OK4" s="1"/>
-      <c r="OL4" s="1"/>
-      <c r="OM4" s="1"/>
-      <c r="ON4" s="1"/>
-      <c r="OO4" s="1"/>
-      <c r="OP4" s="1"/>
-      <c r="OQ4" s="1"/>
-      <c r="OR4" s="1"/>
-      <c r="OS4" s="1"/>
-      <c r="OT4" s="1"/>
-      <c r="OU4" s="1"/>
-      <c r="OV4" s="1"/>
-      <c r="OW4" s="1"/>
-      <c r="OX4" s="1"/>
-      <c r="OY4" s="1"/>
-      <c r="OZ4" s="1"/>
-      <c r="PA4" s="1"/>
-      <c r="PB4" s="1"/>
-      <c r="PC4" s="1"/>
-      <c r="PD4" s="1"/>
-      <c r="PE4" s="1"/>
-      <c r="PF4" s="1"/>
-      <c r="PG4" s="1"/>
-      <c r="PH4" s="1"/>
-      <c r="PI4" s="1"/>
-      <c r="PJ4" s="1"/>
-      <c r="PK4" s="1"/>
-      <c r="PL4" s="1"/>
-      <c r="PM4" s="1"/>
-      <c r="PN4" s="1"/>
-      <c r="PO4" s="1"/>
-      <c r="PP4" s="1"/>
-      <c r="PQ4" s="1"/>
-      <c r="PR4" s="1"/>
-      <c r="PS4" s="1"/>
-      <c r="PT4" s="1"/>
-      <c r="PU4" s="1"/>
-      <c r="PV4" s="1"/>
-      <c r="PW4" s="1"/>
-      <c r="PX4" s="1"/>
-      <c r="PY4" s="1"/>
-      <c r="PZ4" s="1"/>
-      <c r="QA4" s="1"/>
-      <c r="QB4" s="1"/>
-      <c r="QC4" s="1"/>
-      <c r="QD4" s="1"/>
-      <c r="QE4" s="1"/>
-      <c r="QF4" s="1"/>
-      <c r="QG4" s="1"/>
-      <c r="QH4" s="1"/>
-      <c r="QI4" s="1"/>
-      <c r="QJ4" s="1"/>
-      <c r="QK4" s="1"/>
-      <c r="QL4" s="1"/>
-      <c r="QM4" s="1"/>
-      <c r="QN4" s="1"/>
-      <c r="QO4" s="1"/>
-      <c r="QP4" s="1"/>
-      <c r="QQ4" s="1"/>
-      <c r="QR4" s="1"/>
-      <c r="QS4" s="1"/>
-      <c r="QT4" s="1"/>
-      <c r="QU4" s="1"/>
-      <c r="QV4" s="1"/>
-      <c r="QW4" s="1"/>
-      <c r="QX4" s="1"/>
-      <c r="QY4" s="1"/>
-      <c r="QZ4" s="1"/>
-      <c r="RA4" s="1"/>
-      <c r="RB4" s="1"/>
-      <c r="RC4" s="1"/>
-      <c r="RD4" s="1"/>
-      <c r="RE4" s="1"/>
-      <c r="RF4" s="1"/>
-      <c r="RG4" s="1"/>
-      <c r="RH4" s="1"/>
-      <c r="RI4" s="1"/>
-      <c r="RJ4" s="1"/>
-      <c r="RK4" s="1"/>
-      <c r="RL4" s="1"/>
-      <c r="RM4" s="1"/>
-      <c r="RN4" s="1"/>
-      <c r="RO4" s="1"/>
-      <c r="RP4" s="1"/>
-      <c r="RQ4" s="1"/>
-      <c r="RR4" s="1"/>
-      <c r="RS4" s="1"/>
-      <c r="RT4" s="1"/>
-      <c r="RU4" s="1"/>
-      <c r="RV4" s="1"/>
-      <c r="RW4" s="1"/>
-      <c r="RX4" s="1"/>
-      <c r="RY4" s="1"/>
-      <c r="RZ4" s="1"/>
-      <c r="SA4" s="1"/>
-      <c r="SB4" s="1"/>
-      <c r="SC4" s="1"/>
-      <c r="SD4" s="1"/>
-      <c r="SE4" s="1"/>
-      <c r="SF4" s="1"/>
-      <c r="SG4" s="1"/>
-      <c r="SH4" s="1"/>
-      <c r="SI4" s="1"/>
-      <c r="SJ4" s="1"/>
-      <c r="SK4" s="1"/>
-      <c r="SL4" s="1"/>
-      <c r="SM4" s="1"/>
-      <c r="SN4" s="1"/>
-      <c r="SO4" s="1"/>
-      <c r="SP4" s="1"/>
-      <c r="SQ4" s="1"/>
-      <c r="SR4" s="1"/>
-      <c r="SS4" s="1"/>
-      <c r="ST4" s="1"/>
-      <c r="SU4" s="1"/>
-      <c r="SV4" s="1"/>
-      <c r="SW4" s="1"/>
-      <c r="SX4" s="1"/>
-      <c r="SY4" s="1"/>
-      <c r="SZ4" s="1"/>
-      <c r="TA4" s="1"/>
-      <c r="TB4" s="1"/>
-      <c r="TC4" s="1"/>
-      <c r="TD4" s="1"/>
-      <c r="TE4" s="1"/>
-      <c r="TF4" s="1"/>
-      <c r="TG4" s="1"/>
-      <c r="TH4" s="1"/>
-      <c r="TI4" s="1"/>
-      <c r="TJ4" s="1"/>
-      <c r="TK4" s="1"/>
-      <c r="TL4" s="1"/>
-      <c r="TM4" s="1"/>
-      <c r="TN4" s="1"/>
-      <c r="TO4" s="1"/>
-      <c r="TP4" s="1"/>
-      <c r="TQ4" s="1"/>
-      <c r="TR4" s="1"/>
-      <c r="TS4" s="1"/>
-      <c r="TT4" s="1"/>
-      <c r="TU4" s="1"/>
-      <c r="TV4" s="1"/>
-      <c r="TW4" s="1"/>
-      <c r="TX4" s="1"/>
-      <c r="TY4" s="1"/>
-      <c r="TZ4" s="1"/>
-      <c r="UA4" s="1"/>
-      <c r="UB4" s="1"/>
-      <c r="UC4" s="1"/>
-      <c r="UD4" s="1"/>
-      <c r="UE4" s="1"/>
-      <c r="UF4" s="1"/>
-      <c r="UG4" s="1"/>
-      <c r="UH4" s="1"/>
-      <c r="UI4" s="1"/>
-      <c r="UJ4" s="1"/>
-      <c r="UK4" s="1"/>
-      <c r="UL4" s="1"/>
-      <c r="UM4" s="1"/>
-      <c r="UN4" s="1"/>
-      <c r="UO4" s="1"/>
-      <c r="UP4" s="1"/>
-      <c r="UQ4" s="1"/>
-      <c r="UR4" s="1"/>
-      <c r="US4" s="1"/>
-      <c r="UT4" s="1"/>
-      <c r="UU4" s="1"/>
-      <c r="UV4" s="1"/>
-      <c r="UW4" s="1"/>
-      <c r="UX4" s="1"/>
-      <c r="UY4" s="1"/>
-      <c r="UZ4" s="1"/>
-      <c r="VA4" s="1"/>
-      <c r="VB4" s="1"/>
-      <c r="VC4" s="1"/>
-      <c r="VD4" s="1"/>
-      <c r="VE4" s="1"/>
-      <c r="VF4" s="1"/>
-      <c r="VG4" s="1"/>
-      <c r="VH4" s="1"/>
-      <c r="VI4" s="1"/>
-      <c r="VJ4" s="1"/>
-      <c r="VK4" s="1"/>
-      <c r="VL4" s="1"/>
-      <c r="VM4" s="1"/>
-      <c r="VN4" s="1"/>
-      <c r="VO4" s="1"/>
-      <c r="VP4" s="1"/>
-      <c r="VQ4" s="1"/>
-      <c r="VR4" s="1"/>
-      <c r="VS4" s="1"/>
-      <c r="VT4" s="1"/>
-      <c r="VU4" s="1"/>
-      <c r="VV4" s="1"/>
-      <c r="VW4" s="1"/>
-      <c r="VX4" s="1"/>
-      <c r="VY4" s="1"/>
-      <c r="VZ4" s="1"/>
-      <c r="WA4" s="1"/>
-      <c r="WB4" s="1"/>
-      <c r="WC4" s="1"/>
-      <c r="WD4" s="1"/>
-      <c r="WE4" s="1"/>
-      <c r="WF4" s="1"/>
-      <c r="WG4" s="1"/>
-      <c r="WH4" s="1"/>
-      <c r="WI4" s="1"/>
-      <c r="WJ4" s="1"/>
-      <c r="WK4" s="1"/>
-      <c r="WL4" s="1"/>
-      <c r="WM4" s="1"/>
-      <c r="WN4" s="1"/>
-      <c r="WO4" s="1"/>
-      <c r="WP4" s="1"/>
-      <c r="WQ4" s="1"/>
-      <c r="WR4" s="1"/>
-      <c r="WS4" s="1"/>
-      <c r="WT4" s="1"/>
-      <c r="WU4" s="1"/>
-      <c r="WV4" s="1"/>
-      <c r="WW4" s="1"/>
-      <c r="WX4" s="1"/>
-      <c r="WY4" s="1"/>
-      <c r="WZ4" s="1"/>
-      <c r="XA4" s="1"/>
-      <c r="XB4" s="1"/>
-      <c r="XC4" s="1"/>
-      <c r="XD4" s="1"/>
-      <c r="XE4" s="1"/>
-      <c r="XF4" s="1"/>
-      <c r="XG4" s="1"/>
-      <c r="XH4" s="1"/>
-      <c r="XI4" s="1"/>
-      <c r="XJ4" s="1"/>
-      <c r="XK4" s="1"/>
-      <c r="XL4" s="1"/>
-      <c r="XM4" s="1"/>
-      <c r="XN4" s="1"/>
-      <c r="XO4" s="1"/>
-      <c r="XP4" s="1"/>
-      <c r="XQ4" s="1"/>
-      <c r="XR4" s="1"/>
-      <c r="XS4" s="1"/>
-      <c r="XT4" s="1"/>
-      <c r="XU4" s="1"/>
-      <c r="XV4" s="1"/>
-      <c r="XW4" s="1"/>
-      <c r="XX4" s="1"/>
-      <c r="XY4" s="1"/>
-      <c r="XZ4" s="1"/>
-      <c r="YA4" s="1"/>
-      <c r="YB4" s="1"/>
-      <c r="YC4" s="1"/>
-      <c r="YD4" s="1"/>
-      <c r="YE4" s="1"/>
-      <c r="YF4" s="1"/>
-      <c r="YG4" s="1"/>
-      <c r="YH4" s="1"/>
-      <c r="YI4" s="1"/>
-      <c r="YJ4" s="1"/>
-      <c r="YK4" s="1"/>
-      <c r="YL4" s="1"/>
-      <c r="YM4" s="1"/>
-      <c r="YN4" s="1"/>
-      <c r="YO4" s="1"/>
-      <c r="YP4" s="1"/>
-      <c r="YQ4" s="1"/>
-      <c r="YR4" s="1"/>
-      <c r="YS4" s="1"/>
-      <c r="YT4" s="1"/>
-      <c r="YU4" s="1"/>
-      <c r="YV4" s="1"/>
-      <c r="YW4" s="1"/>
-      <c r="YX4" s="1"/>
-      <c r="YY4" s="1"/>
-      <c r="YZ4" s="1"/>
-      <c r="ZA4" s="1"/>
-      <c r="ZB4" s="1"/>
-      <c r="ZC4" s="1"/>
-      <c r="ZD4" s="1"/>
-      <c r="ZE4" s="1"/>
-      <c r="ZF4" s="1"/>
-      <c r="ZG4" s="1"/>
-      <c r="ZH4" s="1"/>
-      <c r="ZI4" s="1"/>
-      <c r="ZJ4" s="1"/>
-      <c r="ZK4" s="1"/>
-      <c r="ZL4" s="1"/>
-      <c r="ZM4" s="1"/>
-      <c r="ZN4" s="1"/>
-      <c r="ZO4" s="1"/>
-      <c r="ZP4" s="1"/>
-      <c r="ZQ4" s="1"/>
-      <c r="ZR4" s="1"/>
-      <c r="ZS4" s="1"/>
-      <c r="ZT4" s="1"/>
-      <c r="ZU4" s="1"/>
-      <c r="ZV4" s="1"/>
-      <c r="ZW4" s="1"/>
-      <c r="ZX4" s="1"/>
-      <c r="ZY4" s="1"/>
-      <c r="ZZ4" s="1"/>
-      <c r="AAA4" s="1"/>
-      <c r="AAB4" s="1"/>
-      <c r="AAC4" s="1"/>
-      <c r="AAD4" s="1"/>
-      <c r="AAE4" s="1"/>
-      <c r="AAF4" s="1"/>
-      <c r="AAG4" s="1"/>
-      <c r="AAH4" s="1"/>
-      <c r="AAI4" s="1"/>
-      <c r="AAJ4" s="1"/>
-      <c r="AAK4" s="1"/>
-      <c r="AAL4" s="1"/>
-      <c r="AAM4" s="1"/>
-      <c r="AAN4" s="1"/>
-      <c r="AAO4" s="1"/>
-      <c r="AAP4" s="1"/>
-      <c r="AAQ4" s="1"/>
-      <c r="AAR4" s="1"/>
-      <c r="AAS4" s="1"/>
-      <c r="AAT4" s="1"/>
-      <c r="AAU4" s="1"/>
-      <c r="AAV4" s="1"/>
-      <c r="AAW4" s="1"/>
-      <c r="AAX4" s="1"/>
-      <c r="AAY4" s="1"/>
-      <c r="AAZ4" s="1"/>
-      <c r="ABA4" s="1"/>
-      <c r="ABB4" s="1"/>
-      <c r="ABC4" s="1"/>
-      <c r="ABD4" s="1"/>
-      <c r="ABE4" s="1"/>
-      <c r="ABF4" s="1"/>
-      <c r="ABG4" s="1"/>
-      <c r="ABH4" s="1"/>
-      <c r="ABI4" s="1"/>
-      <c r="ABJ4" s="1"/>
-      <c r="ABK4" s="1"/>
-      <c r="ABL4" s="1"/>
-      <c r="ABM4" s="1"/>
-      <c r="ABN4" s="1"/>
-      <c r="ABO4" s="1"/>
-      <c r="ABP4" s="1"/>
-      <c r="ABQ4" s="1"/>
-      <c r="ABR4" s="1"/>
-      <c r="ABS4" s="1"/>
-      <c r="ABT4" s="1"/>
-      <c r="ABU4" s="1"/>
-      <c r="ABV4" s="1"/>
-      <c r="ABW4" s="1"/>
-      <c r="ABX4" s="1"/>
-      <c r="ABY4" s="1"/>
-      <c r="ABZ4" s="1"/>
-      <c r="ACA4" s="1"/>
-      <c r="ACB4" s="1"/>
-      <c r="ACC4" s="1"/>
-      <c r="ACD4" s="1"/>
-      <c r="ACE4" s="1"/>
-      <c r="ACF4" s="1"/>
-      <c r="ACG4" s="1"/>
-      <c r="ACH4" s="1"/>
-      <c r="ACI4" s="1"/>
-      <c r="ACJ4" s="1"/>
-      <c r="ACK4" s="1"/>
-      <c r="ACL4" s="1"/>
-      <c r="ACM4" s="1"/>
-      <c r="ACN4" s="1"/>
-      <c r="ACO4" s="1"/>
-      <c r="ACP4" s="1"/>
-      <c r="ACQ4" s="1"/>
-      <c r="ACR4" s="1"/>
-      <c r="ACS4" s="1"/>
-      <c r="ACT4" s="1"/>
-      <c r="ACU4" s="1"/>
-      <c r="ACV4" s="1"/>
-      <c r="ACW4" s="1"/>
-      <c r="ACX4" s="1"/>
-      <c r="ACY4" s="1"/>
-      <c r="ACZ4" s="1"/>
-      <c r="ADA4" s="1"/>
-      <c r="ADB4" s="1"/>
-      <c r="ADC4" s="1"/>
-      <c r="ADD4" s="1"/>
-      <c r="ADE4" s="1"/>
-      <c r="ADF4" s="1"/>
-      <c r="ADG4" s="1"/>
-      <c r="ADH4" s="1"/>
-      <c r="ADI4" s="1"/>
-      <c r="ADJ4" s="1"/>
-      <c r="ADK4" s="1"/>
-      <c r="ADL4" s="1"/>
-      <c r="ADM4" s="1"/>
-      <c r="ADN4" s="1"/>
-      <c r="ADO4" s="1"/>
-      <c r="ADP4" s="1"/>
-      <c r="ADQ4" s="1"/>
-      <c r="ADR4" s="1"/>
-      <c r="ADS4" s="1"/>
-      <c r="ADT4" s="1"/>
-      <c r="ADU4" s="1"/>
-      <c r="ADV4" s="1"/>
-      <c r="ADW4" s="1"/>
-      <c r="ADX4" s="1"/>
-      <c r="ADY4" s="1"/>
-      <c r="ADZ4" s="1"/>
-      <c r="AEA4" s="1"/>
-      <c r="AEB4" s="1"/>
-      <c r="AEC4" s="1"/>
-      <c r="AED4" s="1"/>
-      <c r="AEE4" s="1"/>
-      <c r="AEF4" s="1"/>
-      <c r="AEG4" s="1"/>
-      <c r="AEH4" s="1"/>
-      <c r="AEI4" s="1"/>
-      <c r="AEJ4" s="1"/>
-      <c r="AEK4" s="1"/>
-      <c r="AEL4" s="1"/>
-      <c r="AEM4" s="1"/>
-      <c r="AEN4" s="1"/>
-      <c r="AEO4" s="1"/>
-      <c r="AEP4" s="1"/>
-      <c r="AEQ4" s="1"/>
-      <c r="AER4" s="1"/>
-      <c r="AES4" s="1"/>
-      <c r="AET4" s="1"/>
-      <c r="AEU4" s="1"/>
-      <c r="AEV4" s="1"/>
-      <c r="AEW4" s="1"/>
-      <c r="AEX4" s="1"/>
-      <c r="AEY4" s="1"/>
-      <c r="AEZ4" s="1"/>
-      <c r="AFA4" s="1"/>
-      <c r="AFB4" s="1"/>
-      <c r="AFC4" s="1"/>
-      <c r="AFD4" s="1"/>
-      <c r="AFE4" s="1"/>
-      <c r="AFF4" s="1"/>
-      <c r="AFG4" s="1"/>
-      <c r="AFH4" s="1"/>
-      <c r="AFI4" s="1"/>
-      <c r="AFJ4" s="1"/>
-      <c r="AFK4" s="1"/>
-      <c r="AFL4" s="1"/>
-      <c r="AFM4" s="1"/>
-      <c r="AFN4" s="1"/>
-      <c r="AFO4" s="1"/>
-      <c r="AFP4" s="1"/>
-      <c r="AFQ4" s="1"/>
-      <c r="AFR4" s="1"/>
-      <c r="AFS4" s="1"/>
-      <c r="AFT4" s="1"/>
-      <c r="AFU4" s="1"/>
-      <c r="AFV4" s="1"/>
-      <c r="AFW4" s="1"/>
-      <c r="AFX4" s="1"/>
-      <c r="AFY4" s="1"/>
-      <c r="AFZ4" s="1"/>
-      <c r="AGA4" s="1"/>
-      <c r="AGB4" s="1"/>
-      <c r="AGC4" s="1"/>
-      <c r="AGD4" s="1"/>
-      <c r="AGE4" s="1"/>
-      <c r="AGF4" s="1"/>
-      <c r="AGG4" s="1"/>
-      <c r="AGH4" s="1"/>
-      <c r="AGI4" s="1"/>
-      <c r="AGJ4" s="1"/>
-      <c r="AGK4" s="1"/>
-      <c r="AGL4" s="1"/>
-      <c r="AGM4" s="1"/>
-      <c r="AGN4" s="1"/>
-      <c r="AGO4" s="1"/>
-      <c r="AGP4" s="1"/>
-      <c r="AGQ4" s="1"/>
-      <c r="AGR4" s="1"/>
-      <c r="AGS4" s="1"/>
-      <c r="AGT4" s="1"/>
-      <c r="AGU4" s="1"/>
-      <c r="AGV4" s="1"/>
-      <c r="AGW4" s="1"/>
-      <c r="AGX4" s="1"/>
-      <c r="AGY4" s="1"/>
-      <c r="AGZ4" s="1"/>
-      <c r="AHA4" s="1"/>
-      <c r="AHB4" s="1"/>
-      <c r="AHC4" s="1"/>
-      <c r="AHD4" s="1"/>
-      <c r="AHE4" s="1"/>
-      <c r="AHF4" s="1"/>
-      <c r="AHG4" s="1"/>
-      <c r="AHH4" s="1"/>
-      <c r="AHI4" s="1"/>
-      <c r="AHJ4" s="1"/>
-      <c r="AHK4" s="1"/>
-      <c r="AHL4" s="1"/>
-      <c r="AHM4" s="1"/>
-      <c r="AHN4" s="1"/>
-      <c r="AHO4" s="1"/>
-      <c r="AHP4" s="1"/>
-      <c r="AHQ4" s="1"/>
-      <c r="AHR4" s="1"/>
-      <c r="AHS4" s="1"/>
-      <c r="AHT4" s="1"/>
-      <c r="AHU4" s="1"/>
-      <c r="AHV4" s="1"/>
-      <c r="AHW4" s="1"/>
-      <c r="AHX4" s="1"/>
-      <c r="AHY4" s="1"/>
-      <c r="AHZ4" s="1"/>
-      <c r="AIA4" s="1"/>
-      <c r="AIB4" s="1"/>
-      <c r="AIC4" s="1"/>
-      <c r="AID4" s="1"/>
-      <c r="AIE4" s="1"/>
-      <c r="AIF4" s="1"/>
-      <c r="AIG4" s="1"/>
-      <c r="AIH4" s="1"/>
-      <c r="AII4" s="1"/>
-      <c r="AIJ4" s="1"/>
-      <c r="AIK4" s="1"/>
-      <c r="AIL4" s="1"/>
-      <c r="AIM4" s="1"/>
-      <c r="AIN4" s="1"/>
-      <c r="AIO4" s="1"/>
-      <c r="AIP4" s="1"/>
-      <c r="AIQ4" s="1"/>
-      <c r="AIR4" s="1"/>
-      <c r="AIS4" s="1"/>
-      <c r="AIT4" s="1"/>
-      <c r="AIU4" s="1"/>
-      <c r="AIV4" s="1"/>
-      <c r="AIW4" s="1"/>
-      <c r="AIX4" s="1"/>
-      <c r="AIY4" s="1"/>
-      <c r="AIZ4" s="1"/>
-      <c r="AJA4" s="1"/>
-      <c r="AJB4" s="1"/>
-      <c r="AJC4" s="1"/>
-      <c r="AJD4" s="1"/>
-      <c r="AJE4" s="1"/>
-      <c r="AJF4" s="1"/>
-      <c r="AJG4" s="1"/>
-      <c r="AJH4" s="1"/>
-      <c r="AJI4" s="1"/>
-      <c r="AJJ4" s="1"/>
-      <c r="AJK4" s="1"/>
-      <c r="AJL4" s="1"/>
-      <c r="AJM4" s="1"/>
-      <c r="AJN4" s="1"/>
-      <c r="AJO4" s="1"/>
-      <c r="AJP4" s="1"/>
-      <c r="AJQ4" s="1"/>
-      <c r="AJR4" s="1"/>
-      <c r="AJS4" s="1"/>
-      <c r="AJT4" s="1"/>
-      <c r="AJU4" s="1"/>
-      <c r="AJV4" s="1"/>
-      <c r="AJW4" s="1"/>
-      <c r="AJX4" s="1"/>
-      <c r="AJY4" s="1"/>
-      <c r="AJZ4" s="1"/>
-      <c r="AKA4" s="1"/>
-      <c r="AKB4" s="1"/>
-      <c r="AKC4" s="1"/>
-      <c r="AKD4" s="1"/>
-      <c r="AKE4" s="1"/>
-      <c r="AKF4" s="1"/>
-      <c r="AKG4" s="1"/>
-      <c r="AKH4" s="1"/>
-      <c r="AKI4" s="1"/>
-      <c r="AKJ4" s="1"/>
-      <c r="AKK4" s="1"/>
-      <c r="AKL4" s="1"/>
-      <c r="AKM4" s="1"/>
-      <c r="AKN4" s="1"/>
-      <c r="AKO4" s="1"/>
-      <c r="AKP4" s="1"/>
-      <c r="AKQ4" s="1"/>
-      <c r="AKR4" s="1"/>
-      <c r="AKS4" s="1"/>
-      <c r="AKT4" s="1"/>
-      <c r="AKU4" s="1"/>
-      <c r="AKV4" s="1"/>
-      <c r="AKW4" s="1"/>
-      <c r="AKX4" s="1"/>
-      <c r="AKY4" s="1"/>
-      <c r="AKZ4" s="1"/>
-      <c r="ALA4" s="1"/>
-      <c r="ALB4" s="1"/>
-      <c r="ALC4" s="1"/>
-      <c r="ALD4" s="1"/>
-      <c r="ALE4" s="1"/>
-      <c r="ALF4" s="1"/>
-      <c r="ALG4" s="1"/>
-      <c r="ALH4" s="1"/>
-    </row>
-    <row r="5" spans="1:996" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:996" s="8" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
@@ -3976,7 +2076,7 @@
       <c r="ALG5" s="1"/>
       <c r="ALH5" s="1"/>
     </row>
-    <row r="6" spans="1:996" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:996" s="8" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
@@ -4974,7 +3074,7 @@
       <c r="ALG6" s="1"/>
       <c r="ALH6" s="1"/>
     </row>
-    <row r="7" spans="1:996" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:996" s="8" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -5972,7 +4072,7 @@
       <c r="ALG7" s="1"/>
       <c r="ALH7" s="1"/>
     </row>
-    <row r="8" spans="1:996" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:996" s="8" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
@@ -6970,132 +5070,129 @@
       <c r="ALG8" s="1"/>
       <c r="ALH8" s="1"/>
     </row>
-    <row r="9" spans="1:996" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:996" ht="15.6" x14ac:dyDescent="0.3">
       <c r="J9" s="3"/>
       <c r="K9" s="1"/>
     </row>
-    <row r="10" spans="1:996" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:996" ht="15.6" x14ac:dyDescent="0.3">
       <c r="J10" s="3"/>
       <c r="K10" s="1"/>
     </row>
-    <row r="11" spans="1:996" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:996" ht="15.6" x14ac:dyDescent="0.3">
       <c r="J11" s="3"/>
       <c r="K11" s="1"/>
     </row>
-    <row r="12" spans="1:996" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:996" ht="15.6" x14ac:dyDescent="0.3">
       <c r="J12" s="3"/>
       <c r="K12" s="1"/>
     </row>
-    <row r="13" spans="1:996" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:996" ht="15.6" x14ac:dyDescent="0.3">
       <c r="J13" s="3"/>
       <c r="K13" s="1"/>
     </row>
-    <row r="14" spans="1:996" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:996" ht="15.6" x14ac:dyDescent="0.3">
       <c r="J14" s="3"/>
       <c r="K14" s="1"/>
     </row>
-    <row r="15" spans="1:996" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:996" ht="15.6" x14ac:dyDescent="0.3">
       <c r="J15" s="3"/>
       <c r="K15" s="1"/>
     </row>
-    <row r="16" spans="1:996" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:996" ht="15.6" x14ac:dyDescent="0.3">
       <c r="J16" s="3"/>
       <c r="K16" s="1"/>
     </row>
-    <row r="17" spans="10:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="17" spans="10:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="J17" s="3"/>
       <c r="K17" s="1"/>
     </row>
-    <row r="18" spans="10:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="18" spans="10:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="J18" s="3"/>
       <c r="K18" s="1"/>
     </row>
-    <row r="19" spans="10:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="19" spans="10:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="J19" s="3"/>
       <c r="K19" s="1"/>
     </row>
-    <row r="20" spans="10:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="20" spans="10:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="J20" s="3"/>
       <c r="K20" s="1"/>
     </row>
-    <row r="21" spans="10:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="21" spans="10:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="J21" s="3"/>
       <c r="K21" s="1"/>
     </row>
-    <row r="22" spans="10:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="22" spans="10:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="J22" s="3"/>
       <c r="K22" s="1"/>
     </row>
-    <row r="23" spans="10:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="23" spans="10:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="J23" s="3"/>
       <c r="K23" s="1"/>
     </row>
-    <row r="24" spans="10:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="10:11" x14ac:dyDescent="0.3">
       <c r="K24" s="1"/>
     </row>
-    <row r="25" spans="10:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="10:11" x14ac:dyDescent="0.3">
       <c r="K25" s="1"/>
     </row>
-    <row r="26" spans="10:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="10:11" x14ac:dyDescent="0.3">
       <c r="K26" s="1"/>
     </row>
-    <row r="27" spans="10:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="10:11" x14ac:dyDescent="0.3">
       <c r="K27" s="1"/>
     </row>
-    <row r="28" spans="10:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="10:11" x14ac:dyDescent="0.3">
       <c r="K28" s="1"/>
     </row>
-    <row r="29" spans="10:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="10:11" x14ac:dyDescent="0.3">
       <c r="K29" s="1"/>
     </row>
-    <row r="30" spans="10:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="10:11" x14ac:dyDescent="0.3">
       <c r="K30" s="1"/>
     </row>
-    <row r="31" spans="10:11" x14ac:dyDescent="0.25">
+    <row r="31" spans="10:11" x14ac:dyDescent="0.3">
       <c r="K31" s="1"/>
     </row>
-    <row r="32" spans="10:11" x14ac:dyDescent="0.25">
+    <row r="32" spans="10:11" x14ac:dyDescent="0.3">
       <c r="K32" s="1"/>
     </row>
-    <row r="33" spans="11:11" x14ac:dyDescent="0.25">
+    <row r="33" spans="11:11" x14ac:dyDescent="0.3">
       <c r="K33" s="1"/>
     </row>
-    <row r="34" spans="11:11" x14ac:dyDescent="0.25">
+    <row r="34" spans="11:11" x14ac:dyDescent="0.3">
       <c r="K34" s="1"/>
     </row>
-    <row r="35" spans="11:11" x14ac:dyDescent="0.25">
+    <row r="35" spans="11:11" x14ac:dyDescent="0.3">
       <c r="K35" s="1"/>
     </row>
-    <row r="36" spans="11:11" x14ac:dyDescent="0.25">
+    <row r="36" spans="11:11" x14ac:dyDescent="0.3">
       <c r="K36" s="1"/>
     </row>
-    <row r="37" spans="11:11" x14ac:dyDescent="0.25">
+    <row r="37" spans="11:11" x14ac:dyDescent="0.3">
       <c r="K37" s="1"/>
     </row>
-    <row r="38" spans="11:11" x14ac:dyDescent="0.25">
+    <row r="38" spans="11:11" x14ac:dyDescent="0.3">
       <c r="K38" s="1"/>
     </row>
-    <row r="39" spans="11:11" x14ac:dyDescent="0.25">
+    <row r="39" spans="11:11" x14ac:dyDescent="0.3">
       <c r="K39" s="1"/>
     </row>
-    <row r="40" spans="11:11" x14ac:dyDescent="0.25">
+    <row r="40" spans="11:11" x14ac:dyDescent="0.3">
       <c r="K40" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="16" type="noConversion"/>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G28" xr:uid="{F5E067AE-9E98-48C4-8B1E-338F1C170DC3}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G5:G28 G2:G4" xr:uid="{F5E067AE-9E98-48C4-8B1E-338F1C170DC3}">
       <formula1>"IN1YR,IN3YRS,MORETHAN3YRS"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2:J23" xr:uid="{4FF073F2-2DA2-43FC-869C-552FD33A464D}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J5:J23 J2:J4" xr:uid="{4FF073F2-2DA2-43FC-869C-552FD33A464D}">
       <formula1>"LESSTHAN2.5LAKHS,UPTO5LAKHS,UPTO10LAKHS,MORETHAN10LAKHS"</formula1>
     </dataValidation>
   </dataValidations>
-  <hyperlinks>
-    <hyperlink ref="M2" r:id="rId1" xr:uid="{A111A7B2-D9C5-4F09-955C-F59643DB73F8}"/>
-  </hyperlinks>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0249999999999999" bottom="1.0249999999999999" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+  <pageSetup orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;"Arial,Regular"&amp;10&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Arial,Regular"&amp;10Page &amp;P</oddFooter>
@@ -7105,29 +5202,28 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82133CBD-184A-4904-91FF-20FD4A9F3DA6}">
-  <dimension ref="A1:P6"/>
+  <dimension ref="A1:O6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M2" sqref="M2"/>
+    <sheetView topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2:K2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.44140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="24" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="23.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="31.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="23.88671875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="31.44140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.88671875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="22" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="31.85546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="20.85546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="26.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="31.88671875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="26.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>1</v>
       </c>
@@ -7135,22 +5231,22 @@
         <v>12</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D1" s="6" t="s">
         <v>2</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="G1" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="H1" s="4" t="s">
         <v>33</v>
-      </c>
-      <c r="H1" s="4" t="s">
-        <v>36</v>
       </c>
       <c r="I1" s="4" t="s">
         <v>18</v>
@@ -7162,76 +5258,105 @@
         <v>10</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>47</v>
-      </c>
+        <v>42</v>
+      </c>
+      <c r="M1" s="2"/>
       <c r="N1" s="2"/>
       <c r="O1" s="2"/>
-      <c r="P1" s="2"/>
     </row>
-    <row r="2" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>7</v>
       </c>
       <c r="G2" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="I2" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="H2" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="J2" s="10" t="s">
-        <v>42</v>
+      <c r="J2" s="9" t="s">
+        <v>39</v>
       </c>
       <c r="K2" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="L2" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="L2" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="M2" s="3" t="s">
-        <v>48</v>
-      </c>
+      <c r="M2" s="3"/>
       <c r="N2" s="3"/>
       <c r="O2" s="3"/>
-      <c r="P2" s="3"/>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="G3" s="8"/>
+    <row r="3" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A3" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="J3" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="K3" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="L3" s="3" t="s">
+        <v>44</v>
+      </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="G4" s="8"/>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
       <c r="D6" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2" xr:uid="{5B2BC426-95CA-4978-8691-C5ED5BD2734C}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G3" xr:uid="{5B2BC426-95CA-4978-8691-C5ED5BD2734C}">
       <formula1>"Less than 3 Lac,3 Lac to 5 Lac,5 Lac to 7 Lac,7 Lac to 10 Lac,10 Lac to 15 Lac,15 Lac+"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M2" xr:uid="{A632C067-DF7C-428D-9CB8-89B17DD07518}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L2:L3" xr:uid="{A632C067-DF7C-428D-9CB8-89B17DD07518}">
       <formula1>"Critical Illness - 22 Illness,Waiver of Premium"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>